<commit_message>
modified:   Brighway/Libaries/LCA_plots.py 	modified:   Brighway/Libaries/__pycache__/LCA_plots.cpython-311.pyc 	modified:   Brighway/Results/Ananas - APOS_recipe.xlsx 	modified:   Brighway/Results/Ananas - CONSQ_recipe.xlsx 	modified:   Brighway/Results_Ofir/break_even_large_APOS.jpg 	modified:   Brighway/Results_Ofir/break_even_large_CONSQ.jpg 	modified:   Brighway/Results_Ofir/break_even_small_APOS.jpg 	modified:   Brighway/Results_Ofir/break_even_small_CONSQ.jpg 	modified:   Brighway/Results_Ofir/scaled_impact_score_multi_CONSQ_ReCiPe 2016 v1.03, endpoint (H).jpg 	modified:   Brighway/Results_Ofir/scaled_impact_score_multi_CONSQ_ReCiPe 2016 v1.03, midpoint (H).jpg
</commit_message>
<xml_diff>
--- a/Brighway/Results/Ananas - APOS_recipe.xlsx
+++ b/Brighway/Results/Ananas - APOS_recipe.xlsx
@@ -79,508 +79,508 @@
     <t>('ReCiPe 2016 v1.03, endpoint (H)', 'total: natural resources', 'natural resources')</t>
   </si>
   <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.00044776822019924786], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.00020169124361394091], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.0439435721381354e-05], ["'market for corrugated board box' (kilogram, RER, None)", 8.278808770870672e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.001699141242943235], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 1.1147787062239849e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.00024179483890759387], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -5.786314428266833e-06], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 5.376232279255772e-06], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 6.471508634910819e-07], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -2.326769117870964e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0001283726845058098], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 6.191064121177316e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.00044776822019924786], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.00020169124361394091], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.0439435721381354e-05], ["'market for corrugated board box' (kilogram, RER, None)", 8.278808770870672e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.001699141242943235], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 1.1147787062239849e-06], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.1687461476642983e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.4068497032414825e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -5.058193756681633e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.00027907105326378773], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 6.191064121177316e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0012739321194401136], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.000573825791690367], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00018227765959425067], ["'market for corrugated board box' (kilogram, RER, None)", 2.4967835971139877e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.0022655216572576467], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 3.362031019620352e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0006879233444976614], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -1.74507891920606e-05], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.5295759442389663e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.9517247868649822e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -6.619822038892923e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0003652293276891479], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.76140134166163e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0012739321194401136], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.000573825791690367], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00018227765959425067], ["'market for corrugated board box' (kilogram, RER, None)", 2.4967835971139877e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.0022655216572576467], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 3.362031019620352e-06], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 3.325165096171666e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 4.242879971445614e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.00014390917455258894], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0007939767993825057], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.76140134166163e-05]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.0004896365811427861], ["'alubox production - APOS' (kilogram, GLO, None)", 6.612054933148283e-05], ["'market for polysulfone' (kilogram, GLO, None)", 7.94001955732489e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.00339828248588647], ["'cabinet washer - APOS' (unit, GLO, None)", 0.0005723265694732038], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 2.682371061413364e-06], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -4.9136106031342715e-05], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0004651547520856468], ["'plastic incineration - APOS' (kilogram, CH, None)", 8.578567644751003e-08], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.3004463037451628e-06], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -1.4349664594095203e-06], ["'market for corrugated board box' (kilogram, RER, None)", 2.921828940576546e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.938806370883582e-06]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.0004896365811427861], ["'alubox production - APOS' (kilogram, GLO, None)", 6.612054933148283e-05], ["'market for polysulfone' (kilogram, GLO, None)", 7.94001955732489e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.00339828248588647], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 2.682371061413364e-06], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -4.9136106031342715e-05], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0004651547520856468], ["'plastic incineration - APOS' (kilogram, CH, None)", 8.578567644751003e-08], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -4.4485642147002576e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -4.9488364445030745e-05], ["'market for corrugated board box' (kilogram, RER, None)", 2.921828940576546e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.938806370883582e-06], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.00018338041914667665], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 9.025837036084666e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 2.100945517469414e-06], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 2.796795156198302e-06]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.00029257156857006184], ["'alubox production - APOS' (kilogram, GLO, None)", 3.950887980525451e-05], ["'market for polysulfone' (kilogram, GLO, None)", 3.970009778662445e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.0022655216572576467], ["'cabinet washer - APOS' (unit, GLO, None)", 0.0002861632847366019], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 1.6027918238727194e-06], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -2.936019931652653e-05], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0002779429901415588], ["'plastic incineration - APOS' (kilogram, CH, None)", 4.2892838223755016e-08], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -6.502231518725814e-07], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -7.174832297047602e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.1584911004046972e-06], ["'market for corrugated board box' (kilogram, RER, None)", 1.7458746140906223e-06]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.00029257156857006184], ["'alubox production - APOS' (kilogram, GLO, None)", 3.950887980525451e-05], ["'market for polysulfone' (kilogram, GLO, None)", 3.970009778662445e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.0022655216572576467], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 1.6027918238727194e-06], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -2.936019931652653e-05], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0002779429901415588], ["'plastic incineration - APOS' (kilogram, CH, None)", 4.2892838223755016e-08], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -4.4485642147002576e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -4.9488364445030745e-05], ["'market for corrugated board box' (kilogram, RER, None)", 1.7458746140906223e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.1584911004046972e-06], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.00018338041914667665], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 9.025837036084666e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 2.100945517469414e-06], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 2.796795156198302e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.17080706158518175], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.05584503651893412], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.022502500104376023], ["'market for corrugated board box' (kilogram, RER, None)", 0.004246803666530992], ["'autoclave - APOS' (unit, GLO, None)", 1.3239735387996632], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 0.00022704880868272586], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.09223581325599814], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0022685172575133443], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.08332804089748311], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.010108844417752633], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.014187000144314751], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.14768299577910418], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.003662370801342493]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.17080706158518175], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.05584503651893412], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.022502500104376023], ["'market for corrugated board box' (kilogram, RER, None)", 0.004246803666530992], ["'autoclave - APOS' (unit, GLO, None)", 1.3239735387996632], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 0.00022704880868272586], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.1811479149945285], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.021975748734244856], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.030841304796789013], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.3210499908129668], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.003662370801342493]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.48595811887615087], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.15888306164541818], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0678646814797115], ["'market for corrugated board box' (kilogram, RER, None)", 0.012807820579292088], ["'autoclave - APOS' (unit, GLO, None)", 1.7652980517328842], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 0.000684750375565388], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.26241738419312144], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.006841559844385156], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.23707414452523368], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.03048699048357433], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.04036301474855665], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.4201685231337544], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.010419702844105446]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.48595811887615087], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.15888306164541818], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0678646814797115], ["'market for corrugated board box' (kilogram, RER, None)", 0.012807820579292088], ["'autoclave - APOS' (unit, GLO, None)", 1.7652980517328842], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 0.000684750375565388], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.5153785750548557], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.06627606626863984], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.08774568411041717], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.9134098329665025], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.010419702844105446]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.10942935516731966], ["'alubox production - APOS' (kilogram, GLO, None)", 0.022058003180153652], ["'market for polysulfone' (kilogram, GLO, None)", 0.0026526193575519097], ["'autoclave - APOS' (unit, GLO, None)", 2.6479470775993263], ["'cabinet washer - APOS' (unit, GLO, None)", 0.47885036908640016], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 0.0016686511101938139], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.0042922430874401405], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.10395788740895366], ["'plastic incineration - APOS' (kilogram, CH, None)", 0.000749633601018745], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0007929206106959067], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0016508196146551829], ["'market for corrugated board box' (kilogram, RER, None)", 0.0014988187553596386], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.0011469155710877297]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.10942935516731966], ["'alubox production - APOS' (kilogram, GLO, None)", 0.022058003180153652], ["'market for polysulfone' (kilogram, GLO, None)", 0.0026526193575519097], ["'autoclave - APOS' (unit, GLO, None)", 2.6479470775993263], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 0.0016686511101938139], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.0042922430874401405], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.10395788740895366], ["'plastic incineration - APOS' (kilogram, CH, None)", 0.000749633601018745], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.02712421300042628], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.05693259392047285], ["'market for corrugated board box' (kilogram, RER, None)", 0.0014988187553596386], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.0011469155710877297], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.0222116532216841], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.033604532607296525], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.032817898521688024], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 0.00332891369539865]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.06538710407255446], ["'alubox production - APOS' (kilogram, GLO, None)", 0.013180274592389995], ["'market for polysulfone' (kilogram, GLO, None)", 0.0013263096787759548], ["'autoclave - APOS' (unit, GLO, None)", 1.7652980517328842], ["'cabinet washer - APOS' (unit, GLO, None)", 0.23942518454320008], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 0.0009970657657280139], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.002564735440814947], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.06211774886892675], ["'plastic incineration - APOS' (kilogram, CH, None)", 0.0003748168005093725], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.00039646030534795337], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0008254098073275914], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.0006853141716339495], ["'market for corrugated board box' (kilogram, RER, None)", 0.0008955861788366533]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.06538710407255446], ["'alubox production - APOS' (kilogram, GLO, None)", 0.013180274592389995], ["'market for polysulfone' (kilogram, GLO, None)", 0.0013263096787759548], ["'autoclave - APOS' (unit, GLO, None)", 1.7652980517328842], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 0.0009970657657280139], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.002564735440814947], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.06211774886892675], ["'plastic incineration - APOS' (kilogram, CH, None)", 0.0003748168005093725], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.02712421300042628], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.05693259392047285], ["'market for corrugated board box' (kilogram, RER, None)", 0.0008955861788366533], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.0006853141716339495], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.0222116532216841], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.033604532607296525], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.032817898521688024], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 0.00332891369539865]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0038893164281314303], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.003196864257907693], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0005916230734843358], ["'market for corrugated board box' (kilogram, RER, None)", 0.00014086296987526385], ["'autoclave - APOS' (unit, GLO, None)", 0.18289560255800133], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 4.499571160094361e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0021002308711909725], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0002418228629488159], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.004374392906285103], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.00053069646304317], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0005936267349580011], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.00211037963182978], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.00014328905202340439]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0038893164281314303], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.003196864257907693], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0005916230734843358], ["'market for corrugated board box' (kilogram, RER, None)", 0.00014086296987526385], ["'autoclave - APOS' (unit, GLO, None)", 0.18289560255800133], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 4.499571160094361e-06], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.009509549796271964], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.001153687963137326], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0012904929077412585], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.004587781808165952], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.00014328905202340439]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.011065379133557027], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.009095303945033153], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0017842600267449584], ["'market for corrugated board box' (kilogram, RER, None)", 0.0004248248297059437], ["'autoclave - APOS' (unit, GLO, None)", 0.24386080341066843], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 1.3570135248158271e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.005975304732120794], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0007293070322146941], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.01244545587421959], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.001600513110089058], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0016889098762608527], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.006004178669856974], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.0004076674438181271]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.011065379133557027], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.009095303945033153], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0017842600267449584], ["'market for corrugated board box' (kilogram, RER, None)", 0.0004248248297059437], ["'autoclave - APOS' (unit, GLO, None)", 0.24386080341066843], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 1.3570135248158271e-05], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.027055338856999105], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.0034793763262805605], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.003671543204008265], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.013052562326733977], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.0004076674438181271]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.004540664081734213], ["'alubox production - APOS' (kilogram, GLO, None)", 0.001776359395416686], ["'market for polysulfone' (kilogram, GLO, None)", 9.050919199766397e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.36579120511600266], ["'cabinet washer - APOS' (unit, GLO, None)", 0.07507997292982625], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 4.096812045140882e-05], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.003880676105075475], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.004313630877647501], ["'plastic incineration - APOS' (kilogram, CH, None)", 3.793261229936504e-05], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -3.3178182027223115e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -2.3590096288433488e-05], ["'market for corrugated board box' (kilogram, RER, None)", 4.971458013201856e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 4.4872694177170966e-05]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.004540664081734213], ["'alubox production - APOS' (kilogram, GLO, None)", 0.001776359395416686], ["'market for polysulfone' (kilogram, GLO, None)", 9.050919199766397e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.36579120511600266], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 4.096812045140882e-05], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.003880676105075475], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.004313630877647501], ["'plastic incineration - APOS' (kilogram, CH, None)", 3.793261229936504e-05], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0011349586126705542], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0008135627664048369], ["'market for corrugated board box' (kilogram, RER, None)", 4.971458013201856e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 4.4872694177170966e-05], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.0010501800425814362], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0008835114663666673], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.0017228816618627373], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 3.667831067943272e-05]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.0027131739414611154], ["'alubox production - APOS' (kilogram, GLO, None)", 0.0010614244823134854], ["'market for polysulfone' (kilogram, GLO, None)", 4.525459599883198e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.24386080341066843], ["'cabinet washer - APOS' (unit, GLO, None)", 0.037539986464913126], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 2.4479599203680723e-05], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.0023188126437048125], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0025775152443880595], ["'plastic incineration - APOS' (kilogram, CH, None)", 1.896630614968252e-05], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.6589091013611557e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -1.1795048144216744e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.6812691373477915e-05], ["'market for corrugated board box' (kilogram, RER, None)", 2.970585382234541e-05]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.0027131739414611154], ["'alubox production - APOS' (kilogram, GLO, None)", 0.0010614244823134854], ["'market for polysulfone' (kilogram, GLO, None)", 4.525459599883198e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.24386080341066843], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 2.4479599203680723e-05], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.0023188126437048125], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0025775152443880595], ["'plastic incineration - APOS' (kilogram, CH, None)", 1.896630614968252e-05], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0011349586126705542], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0008135627664048369], ["'market for corrugated board box' (kilogram, RER, None)", 2.970585382234541e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.6812691373477915e-05], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.0010501800425814362], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0008835114663666673], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.0017228816618627373], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 3.667831067943272e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.005187092290987113], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.004161632668358269], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0007865998650084757], ["'market for corrugated board box' (kilogram, RER, None)", 0.00018484304338308005], ["'autoclave - APOS' (unit, GLO, None)", 0.2395255102724744], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 6.396241821226289e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0028010298371330413], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0003170268513029706], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.006334064001046305], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.000768449143903179], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0007611001365818738], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0027596641809934453], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.00018998561109331909]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.005187092290987113], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.004161632668358269], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0007865998650084757], ["'market for corrugated board box' (kilogram, RER, None)", 0.00018484304338308005], ["'autoclave - APOS' (unit, GLO, None)", 0.2395255102724744], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 6.396241821226289e-06], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.013769704350100663], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.0016705416171808238], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.001654565521563481], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.005999269958472625], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.00018998561109331909]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.014757642856047842], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.011840138014202398], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0023722852591123015], ["'market for corrugated board box' (kilogram, RER, None)", 0.0005574631466103629], ["'autoclave - APOS' (unit, GLO, None)", 0.3193673470299659], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 1.929025311650959e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.007969127142265834], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.000956112706783545], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.018020858143821882], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.002317544990221091], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0021653835007743615], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.007851438936189293], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.0005405224428729392]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.014757642856047842], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.011840138014202398], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0023722852591123015], ["'market for corrugated board box' (kilogram, RER, None)", 0.0005574631466103629], ["'autoclave - APOS' (unit, GLO, None)", 0.3193673470299659], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 1.929025311650959e-05], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.039175778573525825], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.0050381412830893275], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.004707355429729163], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.017068345514707657], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.0005405224428729392]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.005985809390783058], ["'alubox production - APOS' (kilogram, GLO, None)", 0.0022976263247923697], ["'market for polysulfone' (kilogram, GLO, None)", 0.0001175989876189449], ["'autoclave - APOS' (unit, GLO, None)", 0.4790510205449488], ["'cabinet washer - APOS' (unit, GLO, None)", 0.098414938582881], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 7.273796492625837e-05], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.004962173841942533], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.005686518921243904], ["'plastic incineration - APOS' (kilogram, CH, None)", 5.051402403444565e-05], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -4.25383787242068e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -3.084788289817386e-05], ["'market for corrugated board box' (kilogram, RER, None)", 6.523640883229748e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 5.949628463771938e-05]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.005985809390783058], ["'alubox production - APOS' (kilogram, GLO, None)", 0.0022976263247923697], ["'market for polysulfone' (kilogram, GLO, None)", 0.0001175989876189449], ["'autoclave - APOS' (unit, GLO, None)", 0.4790510205449488], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 7.273796492625837e-05], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.004962173841942533], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.005686518921243904], ["'plastic incineration - APOS' (kilogram, CH, None)", 5.051402403444565e-05], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.001455152041256106], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.001063865473100082], ["'market for corrugated board box' (kilogram, RER, None)", 6.523640883229748e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 5.949628463771938e-05], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.0009072609867581994], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0011746837324725496], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.002494734806621858], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 4.8690173987212356e-05]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.003576688732151947], ["'alubox production - APOS' (kilogram, GLO, None)", 0.0013728960697001918], ["'market for polysulfone' (kilogram, GLO, None)", 5.879949380947245e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.3193673470299659], ["'cabinet washer - APOS' (unit, GLO, None)", 0.0492074692914405], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 4.34629709312173e-05], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.0029650378267613363], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0033978542955443495], ["'plastic incineration - APOS' (kilogram, CH, None)", 2.5257012017222824e-05], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -2.12691893621034e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -1.542394144908693e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 3.5550696188671304e-05], ["'market for corrugated board box' (kilogram, RER, None)", 3.8980581139795035e-05]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.003576688732151947], ["'alubox production - APOS' (kilogram, GLO, None)", 0.0013728960697001918], ["'market for polysulfone' (kilogram, GLO, None)", 5.879949380947245e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.3193673470299659], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 4.34629709312173e-05], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.0029650378267613363], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0033978542955443495], ["'plastic incineration - APOS' (kilogram, CH, None)", 2.5257012017222824e-05], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.001455152041256106], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.001063865473100082], ["'market for corrugated board box' (kilogram, RER, None)", 3.8980581139795035e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 3.5550696188671304e-05], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.0009072609867581994], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0011746837324725496], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.002494734806621858], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 4.8690173987212356e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.3578401328221148], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.2611178645187945], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.04456693785426435], ["'market for corrugated board box' (kilogram, RER, None)", 0.011345660278595016], ["'autoclave - APOS' (unit, GLO, None)", 1.8184930985238714], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 0.0008182394338512325], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.19323367172394199], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.016232216181721347], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.24367517358232688], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.02955992029081428], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.019325612922416628], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.20297142052789444], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.004775465332273835]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.3578401328221148], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.2611178645187945], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.04456693785426435], ["'market for corrugated board box' (kilogram, RER, None)", 0.011345660278595016], ["'autoclave - APOS' (unit, GLO, None)", 1.8184930985238714], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 0.0008182394338512325], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.5297286382224498], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.06426069628437886], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.042012202189471715], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.44124221852354545], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.004775465332273835]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.01808037788827], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.7428987131379786], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.1344082225520165], ["'market for corrugated board box' (kilogram, RER, None)", 0.034217070675307514], ["'autoclave - APOS' (unit, GLO, None)", 2.424657464698495], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 0.0024677062296987484], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.549763404059666], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.048954301778588276], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.6932730290652117], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.08914896415050584], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.054982730068201896], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.5774679850693567], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.013586535171802049]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.01808037788827], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.7428987131379786], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.1344082225520165], ["'market for corrugated board box' (kilogram, RER, None)", 0.034217070675307514], ["'autoclave - APOS' (unit, GLO, None)", 2.424657464698495], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 0.0024677062296987484], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.507115280576547], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.19380209597936052], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.11952767389024874], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -1.255365185025517], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.013586535171802049]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.12275723913911238], ["'alubox production - APOS' (kilogram, GLO, None)", 0.07271287674687871], ["'market for polysulfone' (kilogram, GLO, None)", 0.008110339097513275], ["'autoclave - APOS' (unit, GLO, None)", 3.636986197047743], ["'cabinet washer - APOS' (unit, GLO, None)", 0.6430113020583837], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 0.031538618830432755], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.34033910168240944], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.11661937718215674], ["'plastic incineration - APOS' (kilogram, CH, None)", 0.0003997203771060025], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0010801210012432443], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0022688407724546105], ["'market for corrugated board box' (kilogram, RER, None)", 0.004004208753871521], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.001495494543252368]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.12275723913911238], ["'alubox production - APOS' (kilogram, GLO, None)", 0.07271287674687871], ["'market for polysulfone' (kilogram, GLO, None)", 0.008110339097513275], ["'autoclave - APOS' (unit, GLO, None)", 3.636986197047743], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 0.031538618830432755], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.34033910168240944], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.11661937718215674], ["'plastic incineration - APOS' (kilogram, CH, None)", 0.0003997203771060025], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.03694875843653827], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.07824658080244039], ["'market for corrugated board box' (kilogram, RER, None)", 0.004004208753871521], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.001495494543252368], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.04622897145967616], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.06655487654190648], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.09596492183710925], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 0.0002950255884151562]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.07335088796763493], ["'alubox production - APOS' (kilogram, GLO, None)", 0.04344798004149145], ["'market for polysulfone' (kilogram, GLO, None)", 0.004055169548756637], ["'autoclave - APOS' (unit, GLO, None)", 2.424657464698495], ["'cabinet washer - APOS' (unit, GLO, None)", 0.3215056510291919], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 0.018845207929965017], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.20336214380173326], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0696833435692532], ["'plastic incineration - APOS' (kilogram, CH, None)", 0.00019986018855300126], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0005400605006216221], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0011344203862273053], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.0008935998690122351], ["'market for corrugated board box' (kilogram, RER, None)", 0.0023926268632017433]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.07335088796763493], ["'alubox production - APOS' (kilogram, GLO, None)", 0.04344798004149145], ["'market for polysulfone' (kilogram, GLO, None)", 0.004055169548756637], ["'autoclave - APOS' (unit, GLO, None)", 2.424657464698495], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 0.018845207929965017], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.20336214380173326], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0696833435692532], ["'plastic incineration - APOS' (kilogram, CH, None)", 0.00019986018855300126], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.03694875843653827], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.07824658080244039], ["'market for corrugated board box' (kilogram, RER, None)", 0.0023926268632017433], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.0008935998690122351], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.04622897145967616], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.06655487654190648], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.09596492183710925], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 0.0002950255884151562]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.12160802955097787], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.01398801497552866], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.01341615937285153], ["'market for corrugated board box' (kilogram, RER, None)", 0.0007403664796185518], ["'autoclave - APOS' (unit, GLO, None)", 0.1777594167481993], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 6.275383538786159e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.06566833595752805], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0004943311668072049], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.00014232807687588331], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.6743018471277034e-05], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0034997922719116298], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.01148925222700415], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.0003492632851573382]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.12160802955097787], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.01398801497552866], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.01341615937285153], ["'market for corrugated board box' (kilogram, RER, None)", 0.0007403664796185518], ["'autoclave - APOS' (unit, GLO, None)", 0.1777594167481993], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 6.275383538786159e-05], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.00030940886277365943], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 3.63978662419066e-05], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.007608244102734292], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.02497663527522678], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.0003492632851573382]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.34598340801827504], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.039796887676856185], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.04046143220959501], ["'market for corrugated board box' (kilogram, RER, None)", 0.0022328512873358948], ["'autoclave - APOS' (unit, GLO, None)", 0.23701255566426574], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 0.00018925759883661535], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.18683104032986853], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0014908399966784642], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.00040493340181589345], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 5.049481658889875e-05], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.009957155540360136], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.03268773168274644], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.0009936786423596217]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.34598340801827504], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.039796887676856185], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.04046143220959501], ["'market for corrugated board box' (kilogram, RER, None)", 0.0022328512873358948], ["'autoclave - APOS' (unit, GLO, None)", 0.23701255566426574], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 0.00018925759883661535], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.0008802900039475944], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.00010977134041064945], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.02164599027415249], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0710602862720553], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.0009936786423596217]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.022981548034039796], ["'alubox production - APOS' (kilogram, GLO, None)", 0.005016176585510375], ["'market for polysulfone' (kilogram, GLO, None)", 0.0012730290747981396], ["'autoclave - APOS' (unit, GLO, None)", 0.3555188334963986], ["'cabinet washer - APOS' (unit, GLO, None)", 0.05477341734897272], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 0.0005208426789368262], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.0010836719002031965], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.021832470632337807], ["'plastic incineration - APOS' (kilogram, CH, None)", 2.495830869459455e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.00019560565287405393], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.00012842834636445536], ["'market for corrugated board box' (kilogram, RER, None)", 0.0002612965544504003], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.00010937600857055998]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.022981548034039796], ["'alubox production - APOS' (kilogram, GLO, None)", 0.005016176585510375], ["'market for polysulfone' (kilogram, GLO, None)", 0.0012730290747981396], ["'autoclave - APOS' (unit, GLO, None)", 0.3555188334963986], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 0.0005208426789368262], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.0010836719002031965], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.021832470632337807], ["'plastic incineration - APOS' (kilogram, CH, None)", 2.495830869459455e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.006691274411427875], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.004429168896792291], ["'market for corrugated board box' (kilogram, RER, None)", 0.0002612965544504003], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.00010937600857055998], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.002855191486274772], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.020035274436994724], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 5.43554394973342e-05], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 5.383455906749426e-05]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.013732118504696628], ["'alubox production - APOS' (kilogram, GLO, None)", 0.00299730597828681], ["'market for polysulfone' (kilogram, GLO, None)", 0.0006365145373990698], ["'autoclave - APOS' (unit, GLO, None)", 0.23701255566426574], ["'cabinet washer - APOS' (unit, GLO, None)", 0.02738670867448636], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 0.00031121808586916555], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.0006475243065331577], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.013045512579461797], ["'plastic incineration - APOS' (kilogram, CH, None)", 1.2479154347297276e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -9.780282643702696e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -6.421417318222768e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 6.535522805664957e-05], ["'market for corrugated board box' (kilogram, RER, None)", 0.00015613200856114617]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.013732118504696628], ["'alubox production - APOS' (kilogram, GLO, None)", 0.00299730597828681], ["'market for polysulfone' (kilogram, GLO, None)", 0.0006365145373990698], ["'autoclave - APOS' (unit, GLO, None)", 0.23701255566426574], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 0.00031121808586916555], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.0006475243065331577], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.013045512579461797], ["'plastic incineration - APOS' (kilogram, CH, None)", 1.2479154347297276e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.006691274411427875], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.004429168896792291], ["'market for corrugated board box' (kilogram, RER, None)", 0.00015613200856114617], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 6.535522805664957e-05], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.002855191486274772], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.020035274436994724], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 5.43554394973342e-05], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 5.383455906749426e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 2.7820788855704762e-05], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 2.03085312752671e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 5.771668255169241e-06], ["'market for corrugated board box' (kilogram, RER, None)", 1.516700055431044e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.00036381489119654544], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 2.5474719020016852e-08], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -1.5023225982080572e-05], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -3.840660149966872e-06], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 7.884780135491285e-08], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 8.886831188436638e-09], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -5.777294415194854e-06], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -1.242822888776668e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.1357420168807041e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 2.7820788855704762e-05], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 2.03085312752671e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 5.771668255169241e-06], ["'market for corrugated board box' (kilogram, RER, None)", 1.516700055431044e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.00036381489119654544], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 2.5474719020016852e-08], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.7140826381502794e-07], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.9319198235731823e-08], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.2559335740277296e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -2.7017888885509065e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.1357420168807041e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 7.915210350496285e-05], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 5.7779201656393715e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.740661819472455e-05], ["'market for corrugated board box' (kilogram, RER, None)", 4.574174769522845e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.0004850865215953939], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 7.682851769883089e-08], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -4.274213589267994e-05], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -1.1582943074784635e-05], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 2.2432754751679433e-07], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 2.6801553834897404e-08], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.6436809566165485e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -3.535918640729556e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 3.2312660201211675e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 7.915210350496285e-05], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 5.7779201656393715e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.740661819472455e-05], ["'market for corrugated board box' (kilogram, RER, None)", 4.574174769522845e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.0004850865215953939], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 7.682851769883089e-08], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 4.876685815582485e-07], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 5.826424746716827e-08], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -3.573219465791796e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -7.686779654324047e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 3.2312660201211675e-06]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 3.401088911889249e-05], ["'alubox production - APOS' (kilogram, GLO, None)", 1.2873970175015666e-05], ["'market for polysulfone' (kilogram, GLO, None)", 7.228334426162012e-07], ["'autoclave - APOS' (unit, GLO, None)", 0.0007276297823930909], ["'cabinet washer - APOS' (unit, GLO, None)", 0.00011033674379167988], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 1.1736799591732176e-07], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -5.467509718432362e-06], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 3.231034466294787e-05], ["'plastic incineration - APOS' (kilogram, CH, None)", 1.6535761758289208e-09], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -3.2289672018521146e-07], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -1.3892434883997888e-07], ["'market for corrugated board box' (kilogram, RER, None)", 5.352869282021617e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 3.5567130543460443e-07]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 3.401088911889249e-05], ["'alubox production - APOS' (kilogram, GLO, None)", 1.2873970175015666e-05], ["'market for polysulfone' (kilogram, GLO, None)", 7.228334426162012e-07], ["'autoclave - APOS' (unit, GLO, None)", 0.0007276297823930909], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 1.1736799591732176e-07], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -5.467509718432362e-06], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 3.231034466294787e-05], ["'plastic incineration - APOS' (kilogram, CH, None)", 1.6535761758289208e-09], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.1045644793816095e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -4.79114947990529e-06], ["'market for corrugated board box' (kilogram, RER, None)", 5.352869282021617e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 3.5567130543460443e-07], ["'production of wet wipe - APOS' (unit, GLO, None)", 9.71701290873255e-06], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 8.619229560257396e-06], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 2.885068877005467e-08], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 1.952361360397637e-08]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 2.0322458658527112e-05], ["'alubox production - APOS' (kilogram, GLO, None)", 7.692557690517278e-06], ["'market for polysulfone' (kilogram, GLO, None)", 3.614167213081006e-07], ["'autoclave - APOS' (unit, GLO, None)", 0.0004850865215953939], ["'cabinet washer - APOS' (unit, GLO, None)", 5.516837189583994e-05], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 7.013066422715202e-08], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -3.266990163930036e-06], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 1.9306335725600756e-05], ["'plastic incineration - APOS' (kilogram, CH, None)", 8.267880879144604e-10], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.6144836009260573e-07], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -6.946217441998944e-08], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.125235651188458e-07], ["'market for corrugated board box' (kilogram, RER, None)", 3.198489296290891e-07]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 2.0322458658527112e-05], ["'alubox production - APOS' (kilogram, GLO, None)", 7.692557690517278e-06], ["'market for polysulfone' (kilogram, GLO, None)", 3.614167213081006e-07], ["'autoclave - APOS' (unit, GLO, None)", 0.0004850865215953939], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 7.013066422715202e-08], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -3.266990163930036e-06], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 1.9306335725600756e-05], ["'plastic incineration - APOS' (kilogram, CH, None)", 8.267880879144604e-10], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.1045644793816095e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -4.79114947990529e-06], ["'market for corrugated board box' (kilogram, RER, None)", 3.198489296290891e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.125235651188458e-07], ["'production of wet wipe - APOS' (unit, GLO, None)", 9.71701290873255e-06], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 8.619229560257396e-06], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 2.885068877005467e-08], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 1.952361360397637e-08]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 2.8165094887766917e-06], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 2.712469693085515e-06], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 7.868421577361211e-07], ["'market for corrugated board box' (kilogram, RER, None)", 1.6026019729633196e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.0005291744184886976], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 5.416698624596908e-09], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -1.5209151239394136e-06], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -3.5050431936777156e-07], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.311470835321409e-07], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.5835262187088882e-08], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -4.870860264611179e-07], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -1.3482722082220904e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 9.019456703665286e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 2.8165094887766917e-06], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 2.712469693085515e-06], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 7.868421577361211e-07], ["'market for corrugated board box' (kilogram, RER, None)", 1.6026019729633196e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.0005291744184886976], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 5.416698624596908e-09], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 2.8510235550465413e-07], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 3.442448301541061e-08], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.0588826708628879e-06], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -2.931026539511239e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 9.019456703665286e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 8.013167841308334e-06], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 7.71716729582076e-06], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 2.373015983196747e-06], ["'market for corrugated board box' (kilogram, RER, None)", 4.833244044573473e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.0007055658913182633], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 1.633607522116651e-08], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -4.3271106343065004e-06], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -1.057076497314674e-06], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 3.731226883590488e-07], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 4.775713896188452e-08], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.3857940558169756e-06], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -3.835929380511093e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.5660989497026737e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 8.013167841308334e-06], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 7.71716729582076e-06], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 2.373015983196747e-06], ["'market for corrugated board box' (kilogram, RER, None)", 4.833244044573473e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.0007055658913182633], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 1.633607522116651e-08], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 8.111362790414103e-07], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.038198673084446e-07], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -3.012595769203746e-06], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -8.338976914766559e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.5660989497026737e-05]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 2.746686004102047e-06], ["'alubox production - APOS' (kilogram, GLO, None)", 2.7296373689588363e-06], ["'market for polysulfone' (kilogram, GLO, None)", 1.200900986770645e-07], ["'autoclave - APOS' (unit, GLO, None)", 0.0010583488369773951], ["'cabinet washer - APOS' (unit, GLO, None)", 0.000188952437183112], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 4.640461358369972e-08], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -1.6860703098206212e-07], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 2.6093517038969446e-06], ["'plastic incineration - APOS' (kilogram, CH, None)", 6.775843940454812e-09], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -2.7223552945247902e-08], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -1.507116100594709e-08], ["'market for corrugated board box' (kilogram, RER, None)", 5.656041774155925e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.8245516080439977e-06]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 2.746686004102047e-06], ["'alubox production - APOS' (kilogram, GLO, None)", 2.7296373689588363e-06], ["'market for polysulfone' (kilogram, GLO, None)", 1.200900986770645e-07], ["'autoclave - APOS' (unit, GLO, None)", 0.0010583488369773951], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 4.640461358369972e-08], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -1.6860703098206212e-07], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 2.6093517038969446e-06], ["'plastic incineration - APOS' (kilogram, CH, None)", 6.775843940454812e-09], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -9.312627755598563e-07], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -5.197662311765511e-07], ["'market for corrugated board box' (kilogram, RER, None)", 5.656041774155925e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.8245516080439977e-06], ["'production of wet wipe - APOS' (unit, GLO, None)", 9.480215969870325e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.1750455648835664e-06], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 5.1408450466165156e-08], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 4.6660602946941943e-07]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 1.6412218031463373e-06], ["'alubox production - APOS' (kilogram, GLO, None)", 1.6310347662338046e-06], ["'market for polysulfone' (kilogram, GLO, None)", 6.004504933853225e-08], ["'autoclave - APOS' (unit, GLO, None)", 0.0007055658913182633], ["'cabinet washer - APOS' (unit, GLO, None)", 9.4476218591556e-05], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 2.772805608883098e-08], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -1.0074742252964469e-07], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 1.5591607129890205e-06], ["'plastic incineration - APOS' (kilogram, CH, None)", 3.387921970227406e-09], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.3611776472623951e-08], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -7.535580502973545e-09], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.6877486837746894e-06], ["'market for corrugated board box' (kilogram, RER, None)", 3.3796433503004436e-07]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 1.6412218031463373e-06], ["'alubox production - APOS' (kilogram, GLO, None)", 1.6310347662338046e-06], ["'market for polysulfone' (kilogram, GLO, None)", 6.004504933853225e-08], ["'autoclave - APOS' (unit, GLO, None)", 0.0007055658913182633], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 2.772805608883098e-08], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -1.0074742252964469e-07], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 1.5591607129890205e-06], ["'plastic incineration - APOS' (kilogram, CH, None)", 3.387921970227406e-09], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -9.312627755598563e-07], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -5.197662311765511e-07], ["'market for corrugated board box' (kilogram, RER, None)", 3.3796433503004436e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.6877486837746894e-06], ["'production of wet wipe - APOS' (unit, GLO, None)", 9.480215969870325e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.1750455648835664e-06], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 5.1408450466165156e-08], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 4.6660602946941943e-07]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.006163217792741251], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.0027284119152065477], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.000905708533043928], ["'market for corrugated board box' (kilogram, RER, None)", 0.00015781328132461432], ["'autoclave - APOS' (unit, GLO, None)", 0.07359486666609583], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 2.6041536632474646e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0033281376080802755], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0003082963444235658], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.0002809081465027925], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 3.2899921324107254e-05], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0009226184376774954], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0018295054352353481], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 8.096556878010072e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.006163217792741251], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.0027284119152065477], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.000905708533043928], ["'market for corrugated board box' (kilogram, RER, None)", 0.00015781328132461432], ["'autoclave - APOS' (unit, GLO, None)", 0.07359486666609583], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 2.6041536632474646e-05], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.0006106698837017229], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 7.152156809588534e-05], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.002005692264615348], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.003977185728634087], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 8.096556878010072e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.017534788649770882], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.007762524040446798], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0027315018697202367], ["'market for corrugated board box' (kilogram, RER, None)", 0.00047594481660746596], ["'autoclave - APOS' (unit, GLO, None)", 0.09812648888812778], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 7.85379676415959e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.009468785870876276], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0009297826072044314], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.000799203459064283], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 9.922198293574986e-05], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.002624914444805326], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0052050718008036035], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.00023035274499878157]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.017534788649770882], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.007762524040446798], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0027315018697202367], ["'market for corrugated board box' (kilogram, RER, None)", 0.00047594481660746596], ["'autoclave - APOS' (unit, GLO, None)", 0.09812648888812778], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 7.85379676415959e-05], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.001737398824052789], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.00021569996290380402], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.005706335741410284], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.011315373480838284], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.00023035274499878157]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.021747164400469948], ["'alubox production - APOS' (kilogram, GLO, None)", 0.0015690717936241686], ["'market for polysulfone' (kilogram, GLO, None)", 0.00011911039136193448], ["'autoclave - APOS' (unit, GLO, None)", 0.14718973333219165], ["'cabinet washer - APOS' (unit, GLO, None)", 0.025571879387756444], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 8.548884920569733e-05], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.0005548138502198018], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.02065980618044645], ["'plastic incineration - APOS' (kilogram, CH, None)", 7.576165333493608e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -5.1565741002385704e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -2.0450448216273988e-05], ["'market for corrugated board box' (kilogram, RER, None)", 5.569683095036782e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.535534400881328e-05]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.021747164400469948], ["'alubox production - APOS' (kilogram, GLO, None)", 0.0015690717936241686], ["'market for polysulfone' (kilogram, GLO, None)", 0.00011911039136193448], ["'autoclave - APOS' (unit, GLO, None)", 0.14718973333219165], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 8.548884920569733e-05], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.0005548138502198018], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.02065980618044645], ["'plastic incineration - APOS' (kilogram, CH, None)", 7.576165333493608e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0017639598764445956], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0007052842439311452], ["'market for corrugated board box' (kilogram, RER, None)", 5.569683095036782e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.535534400881328e-05], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.000654604724331231], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00135255690657513], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.00010680808159337649], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 1.2977040930919572e-05]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.012994539717082662], ["'alubox production - APOS' (kilogram, GLO, None)", 0.000937564335549088], ["'market for polysulfone' (kilogram, GLO, None)", 5.955519568096724e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.09812648888812778], ["'cabinet washer - APOS' (unit, GLO, None)", 0.012785939693878222], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 5.108198135234208e-05], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.0003315168120085104], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.012344812731228528], ["'plastic incineration - APOS' (kilogram, CH, None)", 3.788082666746804e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -2.5782870501192852e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -1.0225224108136994e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.5150528089364082e-05], ["'market for corrugated board box' (kilogram, RER, None)", 3.328041621161996e-05]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.012994539717082662], ["'alubox production - APOS' (kilogram, GLO, None)", 0.000937564335549088], ["'market for polysulfone' (kilogram, GLO, None)", 5.955519568096724e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.09812648888812778], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 5.108198135234208e-05], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.0003315168120085104], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.012344812731228528], ["'plastic incineration - APOS' (kilogram, CH, None)", 3.788082666746804e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0017639598764445956], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0007052842439311452], ["'market for corrugated board box' (kilogram, RER, None)", 3.328041621161996e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.5150528089364082e-05], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.000654604724331231], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00135255690657513], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.00010680808159337649], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 1.2977040930919572e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.08227176533761078], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.05617292099088791], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.013688097170889708], ["'market for corrugated board box' (kilogram, RER, None)", 0.0032036538358738618], ["'autoclave - APOS' (unit, GLO, None)", 3.8280017765525995], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 8.820584758614293e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.04442675328230982], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.004557659174500415], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.0528962044425517], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.006417240333406325], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.011865380993004838], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.05072810362977204], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.00370090052776332]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.08227176533761078], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.05617292099088791], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.013688097170889708], ["'market for corrugated board box' (kilogram, RER, None)", 0.0032036538358738618], ["'autoclave - APOS' (unit, GLO, None)", 3.8280017765525995], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 8.820584758614293e-05], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.11499174878815586], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.013950522463926793], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.025794306619637015], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.1102784861478406], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.00370090052776332]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.23406896617179404], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.15981591605858247], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.04128156206008065], ["'market for corrugated board box' (kilogram, RER, None)", 0.009661813154067984], ["'autoclave - APOS' (unit, GLO, None)", 5.1040023687368], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 0.00026601763564448053], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.12639724173276878], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.013745321041478662], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.1504934267238795], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.019353581565840595], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.03375784472729563], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.14432502720474438], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.01052932262914265]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.23406896617179404], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.15981591605858247], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.04128156206008065], ["'market for corrugated board box' (kilogram, RER, None)", 0.009661813154067984], ["'autoclave - APOS' (unit, GLO, None)", 5.1040023687368], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 0.00026601763564448053], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.3271596233127815], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.04207300340400129], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.07338661886735595], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.3137500591637752], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.01052932262914265]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.09654217417855032], ["'alubox production - APOS' (kilogram, GLO, None)", 0.033842449781809336], ["'market for polysulfone' (kilogram, GLO, None)", 0.002310598647783998], ["'autoclave - APOS' (unit, GLO, None)", 7.656003553105199], ["'cabinet washer - APOS' (unit, GLO, None)", 1.5584801389813074], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 0.0012879710296650718], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.056716450046849505], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0917150654696228], ["'plastic incineration - APOS' (kilogram, CH, None)", 0.000742088521516806], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0006631638152822077], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0005670452989154309], ["'market for corrugated board box' (kilogram, RER, None)", 0.001130661276557168], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.0011589816194424178]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.09654217417855032], ["'alubox production - APOS' (kilogram, GLO, None)", 0.033842449781809336], ["'market for polysulfone' (kilogram, GLO, None)", 0.002310598647783998], ["'autoclave - APOS' (unit, GLO, None)", 7.656003553105199], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 0.0012879710296650718], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.056716450046849505], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0917150654696228], ["'plastic incineration - APOS' (kilogram, CH, None)", 0.000742088521516806], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.022685495038529725], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.019555958416697515], ["'market for corrugated board box' (kilogram, RER, None)", 0.001130661276557168], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.0011589816194424178], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.018810053238438915], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.020441377872566013], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.020833275629523654], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 0.000869493903790299]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.05768665255087576], ["'alubox production - APOS' (kilogram, GLO, None)", 0.02022181143779801], ["'market for polysulfone' (kilogram, GLO, None)", 0.001155299323891999], ["'autoclave - APOS' (unit, GLO, None)", 5.1040023687368], ["'cabinet washer - APOS' (unit, GLO, None)", 0.7792400694906537], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 0.0007695987573935358], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.03388966713884751], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.054802319923331975], ["'plastic incineration - APOS' (kilogram, CH, None)", 0.000371044260758403], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.00033158190764110383], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.00028352264945771544], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.0006925239734201838], ["'market for corrugated board box' (kilogram, RER, None)", 0.0006756017754711337]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.05768665255087576], ["'alubox production - APOS' (kilogram, GLO, None)", 0.02022181143779801], ["'market for polysulfone' (kilogram, GLO, None)", 0.001155299323891999], ["'autoclave - APOS' (unit, GLO, None)", 5.1040023687368], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 0.0007695987573935358], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.03388966713884751], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.054802319923331975], ["'plastic incineration - APOS' (kilogram, CH, None)", 0.000371044260758403], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.022685495038529725], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.019555958416697515], ["'market for corrugated board box' (kilogram, RER, None)", 0.0006756017754711337], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.0006925239734201838], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.018810053238438915], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.020441377872566013], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.020833275629523654], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 0.000869493903790299]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0033518088012856615], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.005699222367795836], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0017894591454651648], ["'market for corrugated board box' (kilogram, RER, None)", 0.0002570042584643343], ["'autoclave - APOS' (unit, GLO, None)", 0.09516491017293233], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 3.5998554509729677e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0018099767526942572], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0004546499972774677], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.2324953663342778e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.433427559309469e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0032068496033723346], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0033719954330666004], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.00013698684289934363]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0033518088012856615], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.005699222367795836], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0017894591454651648], ["'market for corrugated board box' (kilogram, RER, None)", 0.0002570042584643343], ["'autoclave - APOS' (unit, GLO, None)", 0.09516491017293233], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 3.5998554509729677e-06], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 2.679337752900604e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 3.116146868064063e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.006971412211812963], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0073304248542375074], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.00013698684289934363]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.009536132082531037], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.016214688990067026], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.005396781440491304], ["'market for corrugated board box' (kilogram, RER, None)", 0.0007750922079272868], ["'autoclave - APOS' (unit, GLO, None)", 0.1268865468972431], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 1.0856706918376308e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.00514951132456676], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.001371166630679708], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 3.506536112669354e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 4.323035408757078e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.009123713013366758], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.009593564469971453], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.00038973721504116876]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.009536132082531037], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.016214688990067026], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.005396781440491304], ["'market for corrugated board box' (kilogram, RER, None)", 0.0007750922079272868], ["'autoclave - APOS' (unit, GLO, None)", 0.1268865468972431], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 1.0856706918376308e-05], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 7.622904592759465e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 9.397903062515385e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.019834158696325068], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.020855574936251172], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.00038973721504116876]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.001713507960233992], ["'alubox production - APOS' (kilogram, GLO, None)", 0.006760525475713876], ["'market for polysulfone' (kilogram, GLO, None)", 0.0001246382208782475], ["'autoclave - APOS' (unit, GLO, None)", 0.19032982034586465], ["'cabinet washer - APOS' (unit, GLO, None)", 0.020920322230852356], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 2.6629610273703898e-05], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.0003865100370934076], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0016278325622222922], ["'plastic incineration - APOS' (kilogram, CH, None)", 3.29904104740962e-07], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0001792328977267898], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -3.769260077687061e-05], ["'market for corrugated board box' (kilogram, RER, None)", 9.07041702514809e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 4.2899081408636746e-05]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.001713507960233992], ["'alubox production - APOS' (kilogram, GLO, None)", 0.006760525475713876], ["'market for polysulfone' (kilogram, GLO, None)", 0.0001246382208782475], ["'autoclave - APOS' (unit, GLO, None)", 0.19032982034586465], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 2.6629610273703898e-05], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.0003865100370934076], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0016278325622222922], ["'plastic incineration - APOS' (kilogram, CH, None)", 3.29904104740962e-07], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.006131195518247818], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0012999224838289249], ["'market for corrugated board box' (kilogram, RER, None)", 9.07041702514809e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 4.2899081408636746e-05], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.0006033510993987782], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.002672322538574945], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 4.65355665153934e-06], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 3.654304976335396e-06]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.0010238689897574297], ["'alubox production - APOS' (kilogram, GLO, None)", 0.004039603287342358], ["'market for polysulfone' (kilogram, GLO, None)", 6.231911043912375e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.1268865468972431], ["'cabinet washer - APOS' (unit, GLO, None)", 0.010460161115426178], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 1.591193784991112e-05], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.0002309505706386642], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0009726755402695583], ["'plastic incineration - APOS' (kilogram, CH, None)", 1.64952052370481e-07], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -8.96164488633949e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -1.8846300388435306e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.563340247576815e-05], ["'market for corrugated board box' (kilogram, RER, None)", 5.41982817799616e-05]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.0010238689897574297], ["'alubox production - APOS' (kilogram, GLO, None)", 0.004039603287342358], ["'market for polysulfone' (kilogram, GLO, None)", 6.231911043912375e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.1268865468972431], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 1.591193784991112e-05], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.0002309505706386642], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0009726755402695583], ["'plastic incineration - APOS' (kilogram, CH, None)", 1.64952052370481e-07], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.006131195518247818], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0012999224838289249], ["'market for corrugated board box' (kilogram, RER, None)", 5.41982817799616e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.563340247576815e-05], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.0006033510993987782], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.002672322538574945], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 4.65355665153934e-06], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 3.654304976335396e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0013207950818693518], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.0011482939111115064], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0005957474106542295], ["'market for corrugated board box' (kilogram, RER, None)", 0.0011380431270982202], ["'autoclave - APOS' (unit, GLO, None)", 0.02865927517048255], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 7.892479440964108e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.00071322934420945], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.00012281030538521104], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 9.0551581947656e-06], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.0459819392531231e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.00026614484518127247], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.026135974489495777], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 5.478383471812598e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0013207950818693518], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.0011482939111115064], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0005957474106542295], ["'market for corrugated board box' (kilogram, RER, None)", 0.0011380431270982202], ["'autoclave - APOS' (unit, GLO, None)", 0.02865927517048255], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 7.892479440964108e-06], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.9685126510360004e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 2.27387378098505e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0005785757529310518], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.056817335844752674], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 5.478383471812598e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.003757755021656466], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.003266977042880624], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0017966985036720331], ["'market for corrugated board box' (kilogram, RER, None)", 0.003432193557296425], ["'autoclave - APOS' (unit, GLO, None)", 0.03821236689397673], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 2.3802715780351274e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0020291877116944915], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0003703802785794745], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 2.5762562751304952e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 3.154548641781353e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0007572008318903769], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.07435868797202924], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.00015586386780230274]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.003757755021656466], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.003266977042880624], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0017966985036720331], ["'market for corrugated board box' (kilogram, RER, None)", 0.003432193557296425], ["'autoclave - APOS' (unit, GLO, None)", 0.03821236689397673], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 2.3802715780351274e-05], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 5.600557119848902e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 6.857714438655115e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.001646088762623312], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.1616493216901881], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.00015586386780230274]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.001252317123516156], ["'alubox production - APOS' (kilogram, GLO, None)", 0.0011490147079334023], ["'market for polysulfone' (kilogram, GLO, None)", 3.353268334471497e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.0573185503409651], ["'cabinet washer - APOS' (unit, GLO, None)", 0.010656897505563319], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 6.230212309070663e-05], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.0002647636366250949], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0011897012673403482], ["'plastic incineration - APOS' (kilogram, CH, None)", 1.757865092673772e-07], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.4875007473603942e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.00029215130088451147], ["'market for corrugated board box' (kilogram, RER, None)", 0.0004016480433851245], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.715621833242094e-05]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.001252317123516156], ["'alubox production - APOS' (kilogram, GLO, None)", 0.0011490147079334023], ["'market for polysulfone' (kilogram, GLO, None)", 3.353268334471497e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.0573185503409651], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 6.230212309070663e-05], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.0002647636366250949], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0011897012673403482], ["'plastic incineration - APOS' (kilogram, CH, None)", 1.757865092673772e-07], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0005088439695657025], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.010075559575944339], ["'market for corrugated board box' (kilogram, RER, None)", 0.0004016480433851245], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.715621833242094e-05], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.019660182631987582], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0008896706230055435], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 3.395732263684289e-06], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 1.59683313047684e-06]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.0007482945500500169], ["'alubox production - APOS' (kilogram, GLO, None)", 0.0006865684639524811], ["'market for polysulfone' (kilogram, GLO, None)", 1.6766341672357485e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.03821236689397673], ["'cabinet washer - APOS' (unit, GLO, None)", 0.0053284487527816594], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 3.7227263198657037e-05], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.00015820368708343834], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.000710879822547516], ["'plastic incineration - APOS' (kilogram, CH, None)", 8.78932546336886e-08], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -7.437503736801971e-06], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.00014607565044225573], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.02513208916534e-05], ["'market for corrugated board box' (kilogram, RER, None)", 0.00023999595356423876]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.0007482945500500169], ["'alubox production - APOS' (kilogram, GLO, None)", 0.0006865684639524811], ["'market for polysulfone' (kilogram, GLO, None)", 1.6766341672357485e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.03821236689397673], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 3.7227263198657037e-05], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.00015820368708343834], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.000710879822547516], ["'plastic incineration - APOS' (kilogram, CH, None)", 8.78932546336886e-08], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0005088439695657025], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.010075559575944339], ["'market for corrugated board box' (kilogram, RER, None)", 0.00023999595356423876], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.02513208916534e-05], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.019660182631987582], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0008896706230055435], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 3.395732263684289e-06], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 1.59683313047684e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0012989509221187153], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.0005892081487004746], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00014519187021813312], ["'market for corrugated board box' (kilogram, RER, None)", 3.0438550705806856e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.009751364919147791], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 3.864587460542977e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0007014334979441063], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -6.005277350824894e-05], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.905648197566849e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 2.09196053591378e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -7.917330401631962e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.00023595892111971968], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.3580584486039177e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0012989509221187153], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.0005892081487004746], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00014519187021813312], ["'market for corrugated board box' (kilogram, RER, None)", 3.0438550705806856e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.009751364919147791], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 3.864587460542977e-06], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 4.1427134729714115e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 4.54774029546474e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.00017211587905105325], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0005129541763293656], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.3580584486039177e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0036956068488447954], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.001676338676584449], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0004378802346447291], ["'market for corrugated board box' (kilogram, RER, None)", 9.179880369937363e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.013001819892197055], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 1.1655105042678095e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0019956276983761896], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.00018111153548302944], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 5.42170332265498e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 6.309087202728489e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.000225253626925724], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.000671319747301161], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 3.863771924512008e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0036956068488447954], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.001676338676584449], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0004378802346447291], ["'market for corrugated board box' (kilogram, RER, None)", 9.179880369937363e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.013001819892197055], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 1.1655105042678095e-05], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.00011786311570989085], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.3715406962453237e-05], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0004896817969638187], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0014593907551096307], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 3.863771924512008e-05]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.0016993364308568917], ["'alubox production - APOS' (kilogram, GLO, None)", 0.00020228344345516995], ["'market for polysulfone' (kilogram, GLO, None)", 6.169988243712124e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.019502729838295582], ["'cabinet washer - APOS' (unit, GLO, None)", 0.0034651248250365157], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 1.8556450010247273e-05], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.00019946384308320068], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.001614369609314047], ["'plastic incineration - APOS' (kilogram, CH, None)", 3.9970205978131766e-07], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -4.425047151112515e-06], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -2.6375793176618552e-06], ["'market for corrugated board box' (kilogram, RER, None)", 1.0742637113972112e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 4.25292376342703e-06]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.0016993364308568917], ["'alubox production - APOS' (kilogram, GLO, None)", 0.00020228344345516995], ["'market for polysulfone' (kilogram, GLO, None)", 6.169988243712124e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.019502729838295582], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 1.8556450010247273e-05], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.00019946384308320068], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.001614369609314047], ["'plastic incineration - APOS' (kilogram, CH, None)", 3.9970205978131766e-07], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.00015137192783822912], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -9.096344076142203e-05], ["'market for corrugated board box' (kilogram, RER, None)", 1.0742637113972112e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 4.25292376342703e-06], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.00011335676606923576], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00021682501563951944], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 6.791453675795855e-06], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 4.196312874609168e-06]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.0010154011041079998], ["'alubox production - APOS' (kilogram, GLO, None)", 0.00012087002202593586], ["'market for polysulfone' (kilogram, GLO, None)", 3.084994121856062e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.013001819892197055], ["'cabinet washer - APOS' (unit, GLO, None)", 0.0017325624125182578], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 1.1087998519062382e-05], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.00011918523184616125], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0009646310489025998], ["'plastic incineration - APOS' (kilogram, CH, None)", 1.9985102989065883e-07], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -2.2125235755562576e-06], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -1.3187896588309276e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.54124104635806e-06], ["'market for corrugated board box' (kilogram, RER, None)", 6.419026509461157e-06]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.0010154011041079998], ["'alubox production - APOS' (kilogram, GLO, None)", 0.00012087002202593586], ["'market for polysulfone' (kilogram, GLO, None)", 3.084994121856062e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.013001819892197055], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 1.1087998519062382e-05], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.00011918523184616125], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0009646310489025998], ["'plastic incineration - APOS' (kilogram, CH, None)", 1.9985102989065883e-07], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.00015137192783822912], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -9.096344076142203e-05], ["'market for corrugated board box' (kilogram, RER, None)", 6.419026509461157e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.54124104635806e-06], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.00011335676606923576], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00021682501563951944], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 6.791453675795855e-06], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 4.196312874609168e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.942586541245365e-08], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 2.1365172293593314e-08], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 4.025177202411406e-09], ["'market for corrugated board box' (kilogram, RER, None)", 2.5011791136710915e-09], ["'autoclave - APOS' (unit, GLO, None)", 4.6873260419332326e-07], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 6.943037542027535e-11], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -1.048996732272497e-08], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -9.599595730614724e-10], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 6.08381577473906e-09], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 7.378602237886549e-10], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -6.348190414613136e-09], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -3.856382607831381e-08], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.6158711102267305e-09]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.942586541245365e-08], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 2.1365172293593314e-08], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 4.025177202411406e-09], ["'market for corrugated board box' (kilogram, RER, None)", 2.5011791136710915e-09], ["'autoclave - APOS' (unit, GLO, None)", 4.6873260419332326e-07], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 6.943037542027535e-11], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.3225686466824044e-08], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.6040439647579454e-09], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.3800414005324228e-08], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -8.383440451515602e-08], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.6158711102267305e-09]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 5.5267955117121646e-08], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 6.078541976487112e-08], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.2139423062947743e-08], ["'market for corrugated board box' (kilogram, RER, None)", 7.543238595425746e-09], ["'autoclave - APOS' (unit, GLO, None)", 6.249768055910977e-07], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 2.0939319576485633e-10], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -2.984469576324569e-08], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -2.8951161140778123e-09], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.7308884316863242e-08], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 2.225292693331786e-09], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.806104889865371e-08], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -1.0971680093724575e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 4.597267102709941e-09]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 5.5267955117121646e-08], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 6.078541976487112e-08], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.2139423062947743e-08], ["'market for corrugated board box' (kilogram, RER, None)", 7.543238595425746e-09], ["'autoclave - APOS' (unit, GLO, None)", 6.249768055910977e-07], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 2.0939319576485633e-10], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 3.7628009384485305e-08], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 4.837592811590839e-09], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -3.9263149723491276e-08], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -2.385147846636913e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 4.597267102709941e-09]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 2.2538925097084422e-08], ["'alubox production - APOS' (kilogram, GLO, None)", 9.066373066979957e-09], ["'market for polysulfone' (kilogram, GLO, None)", 7.169071248888733e-10], ["'autoclave - APOS' (unit, GLO, None)", 9.374652083866465e-07], ["'cabinet washer - APOS' (unit, GLO, None)", 1.517304219876885e-07], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 7.563958925857879e-10], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -1.881641801436443e-09], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 2.1411978842230197e-08], ["'plastic incineration - APOS' (kilogram, CH, None)", 3.2123499214498354e-10], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -3.5480446670652224e-10], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -4.3107143222807705e-10], ["'market for corrugated board box' (kilogram, RER, None)", 8.827378095268184e-10], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 5.060295195971182e-10]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 2.2538925097084422e-08], ["'alubox production - APOS' (kilogram, GLO, None)", 9.066373066979957e-09], ["'market for polysulfone' (kilogram, GLO, None)", 7.169071248888733e-10], ["'autoclave - APOS' (unit, GLO, None)", 9.374652083866465e-07], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 7.563958925857879e-10], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -1.881641801436443e-09], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 2.1411978842230197e-08], ["'plastic incineration - APOS' (kilogram, CH, None)", 3.2123499214498354e-10], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.2137144373134713e-08], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -1.486656360506353e-08], ["'market for corrugated board box' (kilogram, RER, None)", 8.827378095268184e-10], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 5.060295195971182e-10], ["'production of wet wipe - APOS' (unit, GLO, None)", 1.3763590934157995e-07], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.011074232692752e-09], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 2.3954292841782104e-09], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 2.334751771912932e-08]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 1.3467638905055853e-08], ["'alubox production - APOS' (kilogram, GLO, None)", 5.417411793981457e-09], ["'market for polysulfone' (kilogram, GLO, None)", 3.5845356244443666e-10], ["'autoclave - APOS' (unit, GLO, None)", 6.249768055910977e-07], ["'cabinet washer - APOS' (unit, GLO, None)", 7.586521099384425e-08], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 4.519677272422607e-10], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -1.1243336681429808e-09], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 1.279425695980306e-08], ["'plastic incineration - APOS' (kilogram, CH, None)", 1.6061749607249177e-10], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.7740223335326112e-10], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -2.1553571611403853e-10], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 3.023668086711309e-10], ["'market for corrugated board box' (kilogram, RER, None)", 5.274605611397395e-10]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 1.3467638905055853e-08], ["'alubox production - APOS' (kilogram, GLO, None)", 5.417411793981457e-09], ["'market for polysulfone' (kilogram, GLO, None)", 3.5845356244443666e-10], ["'autoclave - APOS' (unit, GLO, None)", 6.249768055910977e-07], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 4.519677272422607e-10], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -1.1243336681429808e-09], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 1.279425695980306e-08], ["'plastic incineration - APOS' (kilogram, CH, None)", 1.6061749607249177e-10], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.2137144373134713e-08], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -1.486656360506353e-08], ["'market for corrugated board box' (kilogram, RER, None)", 5.274605611397395e-10], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 3.023668086711309e-10], ["'production of wet wipe - APOS' (unit, GLO, None)", 1.3763590934157995e-07], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.011074232692752e-09], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 2.3954292841782104e-09], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 2.334751771912932e-08]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.00016998806206562595], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.000110838933467122], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 2.563845938850817e-05], ["'market for corrugated board box' (kilogram, RER, None)", 3.2210710524177033e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.0006560896967725333], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 4.449414831409708e-07], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -9.179355351543801e-05], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -2.7731595025459803e-06], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.8140406646135314e-06], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 2.132991509327611e-07], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -8.612086268481757e-06], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -5.5954923554735624e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 3.187934530495913e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.00016998806206562595], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.000110838933467122], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 2.563845938850817e-05], ["'market for corrugated board box' (kilogram, RER, None)", 3.2210710524177033e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.0006560896967725333], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 4.449414831409708e-07], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 3.94356666220333e-06], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 4.6369380637556756e-07], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.872192675270579e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.00012164113815823557], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 3.187934530495913e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0004836280075669921], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.0003153445712726569], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 7.732233627201546e-05], ["'market for corrugated board box' (kilogram, RER, None)", 9.714341267444702e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.0008747862623633778], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 1.3418870129864744e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.00026115912408617575], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -8.363496743018314e-06], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 5.161073440168076e-06], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 6.43283140575554e-07], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -2.450199207264203e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.00015919569797474215], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 9.06989824243191e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0004836280075669921], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.0003153445712726569], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 7.732233627201546e-05], ["'market for corrugated board box' (kilogram, RER, None)", 9.714341267444702e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.0008747862623633778], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 1.3418870129864744e-06], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.1219724869930598e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.3984416099468563e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -5.3265200081687986e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0003460776043183169], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 9.06989824243191e-06]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.00021599600147081347], ["'alubox production - APOS' (kilogram, GLO, None)", 2.597174833237654e-05], ["'market for polysulfone' (kilogram, GLO, None)", 3.868790417823136e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.0013121793935450667], ["'cabinet washer - APOS' (unit, GLO, None)", 0.00022338461312882037], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 1.3138137780382486e-06], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -1.7084091274759938e-05], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0002051962013972728], ["'plastic incineration - APOS' (kilogram, CH, None)", 2.8984146201064396e-08], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -4.81335069705127e-07], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -6.254713675963946e-07], ["'market for corrugated board box' (kilogram, RER, None)", 1.1368083115679469e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 9.983401329253032e-07]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.00021599600147081347], ["'alubox production - APOS' (kilogram, GLO, None)", 2.597174833237654e-05], ["'market for polysulfone' (kilogram, GLO, None)", 3.868790417823136e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.0013121793935450667], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 1.3138137780382486e-06], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -1.7084091274759938e-05], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0002051962013972728], ["'plastic incineration - APOS' (kilogram, CH, None)", 2.8984146201064396e-08], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.6465500806945155e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -2.1570925777790906e-05], ["'market for corrugated board box' (kilogram, RER, None)", 1.1368083115679469e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 9.983401329253032e-07], ["'production of wet wipe - APOS' (unit, GLO, None)", 3.66743140902013e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 3.8287676503750914e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 6.924658844071709e-07], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 8.776607994799e-07]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.00012906365943427905], ["'alubox production - APOS' (kilogram, GLO, None)", 1.551884691780089e-05], ["'market for polysulfone' (kilogram, GLO, None)", 1.934395208911568e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.0008747862623633778], ["'cabinet washer - APOS' (unit, GLO, None)", 0.00011169230656441018], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 7.850405232233174e-07], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -1.0208222944014532e-05], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0001226104764625651], ["'plastic incineration - APOS' (kilogram, CH, None)", 1.4492073100532198e-08], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -2.406675348525635e-07], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -3.127356837981973e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 5.965361866660864e-07], ["'market for corrugated board box' (kilogram, RER, None)", 6.792748010299562e-07]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.00012906365943427905], ["'alubox production - APOS' (kilogram, GLO, None)", 1.551884691780089e-05], ["'market for polysulfone' (kilogram, GLO, None)", 1.934395208911568e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.0008747862623633778], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 7.850405232233174e-07], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -1.0208222944014532e-05], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0001226104764625651], ["'plastic incineration - APOS' (kilogram, CH, None)", 1.4492073100532198e-08], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.6465500806945155e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -2.1570925777790906e-05], ["'market for corrugated board box' (kilogram, RER, None)", 6.792748010299562e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 5.965361866660864e-07], ["'production of wet wipe - APOS' (unit, GLO, None)", 3.66743140902013e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 3.8287676503750914e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 6.924658844071709e-07], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 8.776607994799e-07]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0003504637141768082], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.00017202377786909893], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 5.042776174752089e-05], ["'market for corrugated board box' (kilogram, RER, None)", 8.205839676126542e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.001173434895622745], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 2.3446821182988132e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.00018925040565547643], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -4.6240275497054505e-06], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.286386276443755e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.5549615719126231e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.9310921884561185e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.00014686255948619177], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 3.6356299116105775e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0003504637141768082], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.00017202377786909893], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 5.042776174752089e-05], ["'market for corrugated board box' (kilogram, RER, None)", 8.205839676126542e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.001173434895622745], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 2.3446821182988132e-06], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 2.796491905312511e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 3.380351243288311e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -4.198026515051549e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0003192664336545236], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 3.6356299116105775e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.000997093947376271], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.0004894197623881406], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00015208372282441468], ["'market for corrugated board box' (kilogram, RER, None)", 2.4747770447348056e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.0015645798608303267], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 7.07126353316432e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0005384307315831864], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -1.394547962931219e-05], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 3.6598595470653314e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 4.689566550452766e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -5.494093303066056e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.00041783432410359684], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.0343623129650697e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.000997093947376271], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.0004894197623881406], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00015208372282441468], ["'market for corrugated board box' (kilogram, RER, None)", 2.4747770447348056e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.0015645798608303267], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 7.07126353316432e-06], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 7.956216406663763e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.0194709892288622e-05], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.00011943681076528892], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0009083354872483962], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.0343623129650697e-05]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.00028581829031370945], ["'alubox production - APOS' (kilogram, GLO, None)", 3.66508666591304e-05], ["'market for polysulfone' (kilogram, GLO, None)", 5.830554314203478e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.00234686979124549], ["'cabinet washer - APOS' (unit, GLO, None)", 0.00037993232930458136], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 3.0530269051826787e-06], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -1.2499992244360293e-05], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.00027152737579802397], ["'plastic incineration - APOS' (kilogram, CH, None)", 1.9033009747171134e-07], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.079299909638987e-06], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -1.641648671732677e-06], ["'market for corrugated board box' (kilogram, RER, None)", 2.8960760552651672e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.138541339071946e-06]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.00028581829031370945], ["'alubox production - APOS' (kilogram, GLO, None)", 3.66508666591304e-05], ["'market for polysulfone' (kilogram, GLO, None)", 5.830554314203478e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.00234686979124549], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 3.0530269051826787e-06], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -1.2499992244360293e-05], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.00027152737579802397], ["'plastic incineration - APOS' (kilogram, CH, None)", 1.9033009747171134e-07], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -3.69206705507319e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -5.661631129053577e-05], ["'market for corrugated board box' (kilogram, RER, None)", 2.8960760552651672e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.138541339071946e-06], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.0007658611910073358], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 7.530724835450617e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 5.048111234409315e-06], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 6.316669418757423e-06]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.0001707844322577476], ["'alubox production - APOS' (kilogram, GLO, None)", 2.1899919166347908e-05], ["'market for polysulfone' (kilogram, GLO, None)", 2.915277157101739e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.0015645798608303267], ["'cabinet washer - APOS' (unit, GLO, None)", 0.00018996616465229068], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 1.8242690700338352e-06], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -7.4690954044130455e-06], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0001622452106448602], ["'plastic incineration - APOS' (kilogram, CH, None)", 9.516504873585567e-08], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -5.396499548194935e-07], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -8.208243358663385e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 6.803103334948225e-07], ["'market for corrugated board box' (kilogram, RER, None)", 1.7304865439403376e-06]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.0001707844322577476], ["'alubox production - APOS' (kilogram, GLO, None)", 2.1899919166347908e-05], ["'market for polysulfone' (kilogram, GLO, None)", 2.915277157101739e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.0015645798608303267], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 1.8242690700338352e-06], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -7.4690954044130455e-06], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0001622452106448602], ["'plastic incineration - APOS' (kilogram, CH, None)", 9.516504873585567e-08], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -3.69206705507319e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -5.661631129053577e-05], ["'market for corrugated board box' (kilogram, RER, None)", 1.7304865439403376e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 6.803103334948225e-07], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.0007658611910073358], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 7.530724835450617e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 5.048111234409315e-06], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 6.316669418757423e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0003752848134254249], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.00017648306688504862], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 5.542429940590573e-05], ["'market for corrugated board box' (kilogram, RER, None)", 8.53350850804001e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.0012279241797793225], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 2.395849469652867e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.00020265379924972948], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -4.820451221870887e-06], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.2937392412833076e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.5632753833092448e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.985032419720325e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.00015214914656646293], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 3.7489374398610376e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0003752848134254249], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.00017648306688504862], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 5.542429940590573e-05], ["'market for corrugated board box' (kilogram, RER, None)", 8.53350850804001e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.0012279241797793225], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 2.395849469652867e-06], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 2.8124766114854516e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 3.3984247463244455e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -4.315287887879218e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.00033075901426340884], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 3.7489374398610376e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0010677117227033215], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.0005021067536729552], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.000167152645615875], ["'market for corrugated board box' (kilogram, RER, None)", 2.5735978035480335e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.0016372322397057632], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 7.2255777674457005e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0005765643302597937], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -1.4537868469874413e-05], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 3.680779249848284e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 4.714639949394975e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -5.647557060584252e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0004328750366393715], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.066599102695293e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0010677117227033215], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.0005021067536729552], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.000167152645615875], ["'market for corrugated board box' (kilogram, RER, None)", 2.5735978035480335e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.0016372322397057632], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 7.2255777674457005e-06], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 8.001694021409312e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.0249217281293424e-05], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.00012277297940221433], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0009410326884155234], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.066599102695293e-05]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.0002902557988383286], ["'alubox production - APOS' (kilogram, GLO, None)", 3.860467294312466e-05], ["'market for polysulfone' (kilogram, GLO, None)", 6.29803767904099e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.002455848359558645], ["'cabinet washer - APOS' (unit, GLO, None)", 0.0003999088094947557], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 3.3998082355773054e-06], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -1.3025156638695387e-05], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.00027574300889641215], ["'plastic incineration - APOS' (kilogram, CH, None)", 1.91629166926558e-07], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.1094474536440758e-06], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -1.7007428254004966e-06], ["'market for corrugated board box' (kilogram, RER, None)", 3.0117197792002222e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.1740249576133233e-06]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.0002902557988383286], ["'alubox production - APOS' (kilogram, GLO, None)", 3.860467294312466e-05], ["'market for polysulfone' (kilogram, GLO, None)", 6.29803767904099e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.002455848359558645], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 3.3998082355773054e-06], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -1.3025156638695387e-05], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.00027574300889641215], ["'plastic incineration - APOS' (kilogram, CH, None)", 1.91629166926558e-07], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -3.795195715622962e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -5.8654319213373987e-05], ["'market for corrugated board box' (kilogram, RER, None)", 3.0117197792002222e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.1740249576133233e-06], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.0012091062151199882], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 8.276892203014035e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 5.075101640776993e-06], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 6.338024624840571e-06]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.00017343596786515813], ["'alubox production - APOS' (kilogram, GLO, None)", 2.3067373133647682e-05], ["'market for polysulfone' (kilogram, GLO, None)", 3.149018839520495e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.0016372322397057632], ["'cabinet washer - APOS' (unit, GLO, None)", 0.00019995440474737786], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 2.0314806258934286e-06], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -7.782895836254061e-06], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.00016476416947190021], ["'plastic incineration - APOS' (kilogram, CH, None)", 9.5814583463279e-08], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -5.547237268220379e-07], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -8.503714127002483e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 7.015127892468152e-07], ["'market for corrugated board box' (kilogram, RER, None)", 1.7995869074466548e-06]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.00017343596786515813], ["'alubox production - APOS' (kilogram, GLO, None)", 2.3067373133647682e-05], ["'market for polysulfone' (kilogram, GLO, None)", 3.149018839520495e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.0016372322397057632], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 2.0314806258934286e-06], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -7.782895836254061e-06], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.00016476416947190021], ["'plastic incineration - APOS' (kilogram, CH, None)", 9.5814583463279e-08], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -3.795195715622962e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -5.8654319213373987e-05], ["'market for corrugated board box' (kilogram, RER, None)", 1.7995869074466548e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 7.015127892468152e-07], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.0012091062151199882], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 8.276892203014035e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 5.075101640776993e-06], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 6.338024624840571e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0012426762753245935], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.00036398055433329543], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0003511865862773925], ["'market for corrugated board box' (kilogram, RER, None)", 4.2225104178167744e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.010704359580710858], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 4.711286406182188e-07], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0006710451886752805], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -1.9004050940381406e-05], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 4.73351468627404e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 5.111994846159728e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -7.640119589227457e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.00027095474400126615], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.183085572672973e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0012426762753245935], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.00036398055433329543], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0003511865862773925], ["'market for corrugated board box' (kilogram, RER, None)", 4.2225104178167744e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.010704359580710858], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 4.711286406182188e-07], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.00010290249317987043], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.1113032274260279e-05], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.00016608955701583503], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0005890320521561669], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.183085572672973e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0035355015157122237], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.0010355503095116293], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0010591341276353407], ["'market for corrugated board box' (kilogram, RER, None)", 0.00012734555226040197], ["'autoclave - APOS' (unit, GLO, None)", 0.01427247944094781], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 1.420864154604482e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0019091708184846008], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -5.731380326234904e-05], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.00013467182628554313], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.5417127001505536e-05], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.00021736678404440758], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0007708853278774344], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 3.3659617704143766e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0035355015157122237], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.0010355503095116293], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0010591341276353407], ["'market for corrugated board box' (kilogram, RER, None)", 0.00012734555226040197], ["'autoclave - APOS' (unit, GLO, None)", 0.01427247944094781], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 1.420864154604482e-06], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.0002927648397511807], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 3.3515493481533774e-05], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0004725364863767985], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0016758376694217625], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 3.3659617704143766e-05]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.0006367618977553125], ["'alubox production - APOS' (kilogram, GLO, None)", 0.0006762028182161041], ["'market for polysulfone' (kilogram, GLO, None)", 4.240918684364896e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.021408719161421716], ["'cabinet washer - APOS' (unit, GLO, None)", 0.004039357611284405], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 2.6740040886812073e-06], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -3.511925773874729e-05], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0006049238028675468], ["'plastic incineration - APOS' (kilogram, CH, None)", 1.175813793438848e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -4.270112235748204e-06], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -3.028767148996665e-06], ["'market for corrugated board box' (kilogram, RER, None)", 1.4902449714834396e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 3.704975107191457e-06]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.0006367618977553125], ["'alubox production - APOS' (kilogram, GLO, None)", 0.0006762028182161041], ["'market for polysulfone' (kilogram, GLO, None)", 4.240918684364896e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.021408719161421716], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 2.6740040886812073e-06], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -3.511925773874729e-05], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0006049238028675468], ["'plastic incineration - APOS' (kilogram, CH, None)", 1.175813793438848e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.00014607191723331337], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.00010445451982923834], ["'market for corrugated board box' (kilogram, RER, None)", 1.4902449714834396e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 3.704975107191457e-06], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.009010382556659601], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0005244511069909417], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.659585618016259e-05], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 4.24396011408411e-06]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.0003804830652095282], ["'alubox production - APOS' (kilogram, GLO, None)", 0.0004040501196524964], ["'market for polysulfone' (kilogram, GLO, None)", 2.120459342182448e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.01427247944094781], ["'cabinet washer - APOS' (unit, GLO, None)", 0.0020196788056422027], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 1.5977923233641655e-06], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -2.098473994663656e-05], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.00036145891194905175], ["'plastic incineration - APOS' (kilogram, CH, None)", 5.87906896719424e-07], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -2.135056117874102e-06], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -1.5143835744983325e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.213826379653449e-06], ["'market for corrugated board box' (kilogram, RER, None)", 8.904631028727327e-06]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.0003804830652095282], ["'alubox production - APOS' (kilogram, GLO, None)", 0.0004040501196524964], ["'market for polysulfone' (kilogram, GLO, None)", 2.120459342182448e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.01427247944094781], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 1.5977923233641655e-06], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -2.098473994663656e-05], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.00036145891194905175], ["'plastic incineration - APOS' (kilogram, CH, None)", 5.87906896719424e-07], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.00014607191723331337], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.00010445451982923834], ["'market for corrugated board box' (kilogram, RER, None)", 8.904631028727327e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.213826379653449e-06], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.009010382556659601], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0005244511069909417], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.659585618016259e-05], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 4.24396011408411e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 6.594758818767752e-10], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 2.513503048988018e-10], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 9.314310917586194e-11], ["'market for corrugated board box' (kilogram, RER, None)", 2.6107095004555252e-11], ["'autoclave - APOS' (unit, GLO, None)", 4.897503985765704e-09], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 1.2814611037247904e-12], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -3.561169762134587e-10], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -1.2252929497775287e-11], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 2.4275037332741033e-10], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 2.944618815966076e-11], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -5.4167145333541937e-11], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -7.045313455879403e-10], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.348792747494446e-11]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 6.594758818767752e-10], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 2.513503048988018e-10], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 9.314310917586194e-11], ["'market for corrugated board box' (kilogram, RER, None)", 2.6107095004555252e-11], ["'autoclave - APOS' (unit, GLO, None)", 4.897503985765704e-09], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 1.2814611037247904e-12], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 5.277182028856747e-10], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 6.401345252100166e-11], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.1775466428490867e-10], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -1.5315898816596134e-09], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.348792747494446e-11]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.876255325902938e-09], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 7.151093181627883e-10], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 2.8090778388756033e-10], ["'market for corrugated board box' (kilogram, RER, None)", 7.873568333287495e-11], ["'autoclave - APOS' (unit, GLO, None)", 6.530005314354272e-09], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 3.864723964591084e-12], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -1.0131778759875866e-09], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -3.695327868916099e-11], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 6.906419072131957e-10], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 8.880596249207051e-11], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.5410934402937285e-10], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -2.004441292753123e-09], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 3.83741035233925e-11]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.876255325902938e-09], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 7.151093181627883e-10], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 2.8090778388756033e-10], ["'market for corrugated board box' (kilogram, RER, None)", 7.873568333287495e-11], ["'autoclave - APOS' (unit, GLO, None)", 6.530005314354272e-09], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 3.864723964591084e-12], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.5013954504634687e-09], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.9305644020015327e-10], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -3.350203126278744e-10], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -4.357481071522242e-09], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 3.83741035233925e-11]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 4.868087151423871e-10], ["'alubox production - APOS' (kilogram, GLO, None)", 1.018901480440111e-10], ["'market for polysulfone' (kilogram, GLO, None)", 1.0875171631154611e-11], ["'autoclave - APOS' (unit, GLO, None)", 9.795007971531408e-09], ["'cabinet washer - APOS' (unit, GLO, None)", 1.75224406374857e-09], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 6.707778065272973e-12], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -3.7222590595168694e-11], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 4.624682793852677e-10], ["'plastic incineration - APOS' (kilogram, CH, None)", 2.1807394992709287e-12], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -3.0274367745557354e-12], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -7.87534244074796e-12], ["'market for corrugated board box' (kilogram, RER, None)", 9.213942228873176e-12], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 4.223907103301839e-12]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 4.868087151423871e-10], ["'alubox production - APOS' (kilogram, GLO, None)", 1.018901480440111e-10], ["'market for polysulfone' (kilogram, GLO, None)", 1.0875171631154611e-11], ["'autoclave - APOS' (unit, GLO, None)", 9.795007971531408e-09], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 6.707778065272973e-12], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -3.7222590595168694e-11], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 4.624682793852677e-10], ["'plastic incineration - APOS' (kilogram, CH, None)", 2.1807394992709287e-12], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.0356249895724549e-10], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -2.716006456328795e-10], ["'market for corrugated board box' (kilogram, RER, None)", 9.213942228873176e-12], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 4.223907103301839e-12], ["'production of wet wipe - APOS' (unit, GLO, None)", 4.392788796950162e-10], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.3909701743925513e-10], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 9.559569570357645e-11], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 1.0792811361554383e-11]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 2.9088183944583734e-10], ["'alubox production - APOS' (kilogram, GLO, None)", 6.088221669528204e-11], ["'market for polysulfone' (kilogram, GLO, None)", 5.4375858155773054e-12], ["'autoclave - APOS' (unit, GLO, None)", 6.530005314354272e-09], ["'cabinet washer - APOS' (unit, GLO, None)", 8.76122031874285e-10], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 4.008085232513434e-12], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -2.224154022816762e-11], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 2.7633774747354547e-10], ["'plastic incineration - APOS' (kilogram, CH, None)", 1.0903697496354644e-12], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.5137183872778677e-12], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -3.93767122037398e-12], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.5239027793586677e-12], ["'market for corrugated board box' (kilogram, RER, None)", 5.505588506462332e-12]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 2.9088183944583734e-10], ["'alubox production - APOS' (kilogram, GLO, None)", 6.088221669528204e-11], ["'market for polysulfone' (kilogram, GLO, None)", 5.4375858155773054e-12], ["'autoclave - APOS' (unit, GLO, None)", 6.530005314354272e-09], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 4.008085232513434e-12], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -2.224154022816762e-11], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 2.7633774747354547e-10], ["'plastic incineration - APOS' (kilogram, CH, None)", 1.0903697496354644e-12], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.0356249895724549e-10], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -2.716006456328795e-10], ["'market for corrugated board box' (kilogram, RER, None)", 5.505588506462332e-12], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.5239027793586677e-12], ["'production of wet wipe - APOS' (unit, GLO, None)", 4.392788796950162e-10], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.3909701743925513e-10], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 9.559569570357645e-11], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 1.0792811361554383e-11]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 3.076268826759314e-07], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 1.4437574095097888e-07], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 4.3960972279403205e-08], ["'market for corrugated board box' (kilogram, RER, None)", 7.325167901430008e-09], ["'autoclave - APOS' (unit, GLO, None)", 2.7845578783600164e-06], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 6.002837272676786e-10], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -1.66118516645003e-07], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -5.961856734412428e-09], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 9.15874890852756e-08], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.1101302285616891e-08], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -2.4561663639056362e-08], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -1.9064393577245598e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 6.54901193661524e-09]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 3.076268826759314e-07], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 1.4437574095097888e-07], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 4.3960972279403205e-08], ["'market for corrugated board box' (kilogram, RER, None)", 7.325167901430008e-09], ["'autoclave - APOS' (unit, GLO, None)", 2.7845578783600164e-06], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 6.002837272676786e-10], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.9910323714190347e-07], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 2.413326583829759e-08], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -5.3394921188600304e-08], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -4.14443338621351e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 6.54901193661524e-09]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 8.75220145078002e-07], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 4.107591503112357e-07], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.3258070736326534e-07], ["'market for corrugated board box' (kilogram, RER, None)", 2.2091776206678668e-08], ["'autoclave - APOS' (unit, GLO, None)", 3.712743837813355e-06], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 1.8103794953917617e-09], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -4.726188783421211e-07], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -1.798020248558473e-08], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 2.605728562707841e-07], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 3.348011732602431e-08], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -6.987966318655482e-08], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -5.423954228131452e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.8632400159212842e-08]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 8.75220145078002e-07], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 4.107591503112357e-07], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.3258070736326534e-07], ["'market for corrugated board box' (kilogram, RER, None)", 2.2091776206678668e-08], ["'autoclave - APOS' (unit, GLO, None)", 3.712743837813355e-06], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 1.8103794953917617e-09], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 5.664627310234437e-07], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 7.278286375222676e-08], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.519123110577128e-07], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -1.1791204844629398e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.8632400159212842e-08]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 3.331508929349619e-07], ["'alubox production - APOS' (kilogram, GLO, None)", 5.130891409080537e-08], ["'market for polysulfone' (kilogram, GLO, None)", 5.915531344963806e-09], ["'autoclave - APOS' (unit, GLO, None)", 5.569115756720033e-06], ["'cabinet washer - APOS' (unit, GLO, None)", 1.0348270460808225e-06], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 2.9610874763512365e-09], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -2.9578093637089378e-08], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 3.164933482882138e-07], ["'plastic incineration - APOS' (kilogram, CH, None)", 9.112894422399398e-10], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.372767261174135e-09], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -2.1310425545468453e-09], ["'market for corrugated board box' (kilogram, RER, None)", 2.585261740105352e-09], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.050902044814825e-09]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 3.331508929349619e-07], ["'alubox production - APOS' (kilogram, GLO, None)", 5.130891409080537e-08], ["'market for polysulfone' (kilogram, GLO, None)", 5.915531344963806e-09], ["'autoclave - APOS' (unit, GLO, None)", 5.569115756720033e-06], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 2.9610874763512365e-09], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -2.9578093637089378e-08], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 3.164933482882138e-07], ["'plastic incineration - APOS' (kilogram, CH, None)", 9.112894422399398e-10], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -4.695959606778231e-08], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -7.349426873062975e-08], ["'market for corrugated board box' (kilogram, RER, None)", 2.585261740105352e-09], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.050902044814825e-09], ["'production of wet wipe - APOS' (unit, GLO, None)", 7.092161060082882e-08], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.564994643081361e-08], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 3.603986734904693e-08], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 3.911140445855908e-09]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 1.9906698778307688e-07], ["'alubox production - APOS' (kilogram, GLO, None)", 3.06585129773951e-08], ["'market for polysulfone' (kilogram, GLO, None)", 2.957765672481903e-09], ["'autoclave - APOS' (unit, GLO, None)", 3.712743837813355e-06], ["'cabinet washer - APOS' (unit, GLO, None)", 5.174135230404112e-07], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 1.7693326867189491e-09], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -1.767373922617894e-08], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 1.8911363839392304e-07], ["'plastic incineration - APOS' (kilogram, CH, None)", 4.556447211199699e-10], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -6.863836305870675e-10], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -1.0655212772734226e-09], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.2254714046751174e-09], ["'market for corrugated board box' (kilogram, RER, None)", 1.5447662866735288e-09]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 1.9906698778307688e-07], ["'alubox production - APOS' (kilogram, GLO, None)", 3.06585129773951e-08], ["'market for polysulfone' (kilogram, GLO, None)", 2.957765672481903e-09], ["'autoclave - APOS' (unit, GLO, None)", 3.712743837813355e-06], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 1.7693326867189491e-09], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -1.767373922617894e-08], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 1.8911363839392304e-07], ["'plastic incineration - APOS' (kilogram, CH, None)", 4.556447211199699e-10], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -4.695959606778231e-08], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -7.349426873062975e-08], ["'market for corrugated board box' (kilogram, RER, None)", 1.5447662866735288e-09], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.2254714046751174e-09], ["'production of wet wipe - APOS' (unit, GLO, None)", 7.092161060082882e-08], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.564994643081361e-08], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 3.603986734904693e-08], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 3.911140445855908e-09]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.04813660124284061], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.003585106468493621], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.005074179597921867], ["'market for corrugated board box' (kilogram, RER, None)", 0.00024889132757794676], ["'autoclave - APOS' (unit, GLO, None)", 0.05087673060843365], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 2.5740261101999055e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.02599376467113393], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.00015679095243401186], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 5.226880221697493e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 6.146015557016038e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0006061891267982785], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.003509209681066763], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 7.894024659335565e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.04813660124284061], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.003585106468493621], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.005074179597921867], ["'market for corrugated board box' (kilogram, RER, None)", 0.00024889132757794676], ["'autoclave - APOS' (unit, GLO, None)", 0.05087673060843365], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 2.5740261101999055e-05], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.00011362783090646725], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.3360903384817474e-05], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0013178024553398714], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.00762871669770574], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 7.894024659335565e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.1369520204373775], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.010199880375150865], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.015303081017066697], ["'market for corrugated board box' (kilogram, RER, None)", 0.0007506246385917995], ["'autoclave - APOS' (unit, GLO, None)", 0.06783564081124487], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 7.762935889866213e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.07395409103618385], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.00047286159299986225], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.00014870842320885828], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.8535602098059e-05], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0017246507659463624], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.009983948668443234], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.00022459056074869915]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.1369520204373775], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.010199880375150865], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.015303081017066697], ["'market for corrugated board box' (kilogram, RER, None)", 0.0007506246385917995], ["'autoclave - APOS' (unit, GLO, None)", 0.06783564081124487], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 7.762935889866213e-05], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.0003232791808888223], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 4.029478716969348e-05], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0037492407901699165], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.021704236237339063], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.00022459056074869915]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.0045326307586048215], ["'alubox production - APOS' (kilogram, GLO, None)", 0.0012805993133763874], ["'market for polysulfone' (kilogram, GLO, None)", 0.0004548315760085618], ["'autoclave - APOS' (unit, GLO, None)", 0.1017534612168673], ["'cabinet washer - APOS' (unit, GLO, None)", 0.018091794245463536], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 0.00022504716122111656], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.00035513013294828546], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.004305999220674581], ["'plastic incineration - APOS' (kilogram, CH, None)", 9.422288368560032e-07], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -3.3880302229412986e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -3.9226399375780656e-05], ["'market for corrugated board box' (kilogram, RER, None)", 8.784088437149415e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.4721089948138736e-05]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.0045326307586048215], ["'alubox production - APOS' (kilogram, GLO, None)", 0.0012805993133763874], ["'market for polysulfone' (kilogram, GLO, None)", 0.0004548315760085618], ["'autoclave - APOS' (unit, GLO, None)", 0.1017534612168673], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 0.00022504716122111656], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.00035513013294828546], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.004305999220674581], ["'plastic incineration - APOS' (kilogram, CH, None)", 9.422288368560032e-07], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0011589767270431721], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0013528193188388333], ["'market for corrugated board box' (kilogram, RER, None)", 8.784088437149415e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.4721089948138736e-05], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.0009750444546189048], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.007577621729262176], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.995275686592369e-05], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 1.93932876931901e-05]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.0027083738059334337], ["'alubox production - APOS' (kilogram, GLO, None)", 0.0007651939504802129], ["'market for polysulfone' (kilogram, GLO, None)", 0.0002274157880042809], ["'autoclave - APOS' (unit, GLO, None)", 0.06783564081124487], ["'cabinet washer - APOS' (unit, GLO, None)", 0.009045897122731768], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 0.00013447198084552608], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.00021220019917767387], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.002572955115636762], ["'plastic incineration - APOS' (kilogram, CH, None)", 4.711144184280016e-07], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.6940151114706493e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -1.9613199687890328e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.4771543526634314e-05], ["'market for corrugated board box' (kilogram, RER, None)", 5.2487388283997186e-05]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.0027083738059334337], ["'alubox production - APOS' (kilogram, GLO, None)", 0.0007651939504802129], ["'market for polysulfone' (kilogram, GLO, None)", 0.0002274157880042809], ["'autoclave - APOS' (unit, GLO, None)", 0.06783564081124487], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 0.00013447198084552608], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.00021220019917767387], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.002572955115636762], ["'plastic incineration - APOS' (kilogram, CH, None)", 4.711144184280016e-07], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0011589767270431721], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0013528193188388333], ["'market for corrugated board box' (kilogram, RER, None)", 5.2487388283997186e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.4771543526634314e-05], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.0009750444546189048], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.007577621729262176], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.995275686592369e-05], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 1.93932876931901e-05]]</t>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.00032945166331691244], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00015801064853070173], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 4.6389205711862454e-05], ["'market for corrugated board box' (kilogram, RER, None)", 2.013778491028875e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0004622626384260705], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.1147787062239849e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.00017790389819113272], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -1.8781572123565963e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.66507922162909e-06], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.2504469565799618e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.3860842943139076e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -8.303594843869356e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.0142047379371389e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.00032945166331691244], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00015801064853070173], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 4.6389205711862454e-05], ["'market for corrugated board box' (kilogram, RER, None)", 2.013778491028875e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0004622626384260705], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.1147787062239849e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.2315389612237151e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -2.7183629490868737e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.1871397929925744e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0001805129313821823], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.0142047379371389e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0009373131829579762], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.0004495514225803063], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0001399039509001107], ["'market for corrugated board box' (kilogram, RER, None)", 6.073300209944417e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000616350184568094], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 3.362031019620352e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0005061491187973072], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -5.664283541570399e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.6117549334775722e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -4.427048141689966e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.78857789405792e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00023624312087142089], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.8854839025352327e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0009373131829579762], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.0004495514225803063], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0001399039509001107], ["'market for corrugated board box' (kilogram, RER, None)", 6.073300209944417e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000616350184568094], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.5809710865610812e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.5038150727773306e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -8.198237299425862e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.00014757778009440384], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.000513572001932085], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.8854839025352327e-05]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0006799317205210687], ["'alubox production - CONSQ' (kilogram, GLO, None)", 5.9310919264254154e-05], ["'market for polysulfone' (kilogram, GLO, None)", 4.019118309206293e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000924525276852141], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.00016623361404338074], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.495551281007104e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 5.907099145686869e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0006459351344950152], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 9.505013037587547e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.3335979393624514e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -9.281865639367464e-07], ["'market for corrugated board box' (kilogram, RER, None)", 7.107201576755263e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.176104412433239e-06]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0006799317205210687], ["'alubox production - CONSQ' (kilogram, GLO, None)", 5.9310919264254154e-05], ["'market for polysulfone' (kilogram, GLO, None)", 4.019118309206293e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000924525276852141], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.495551281007104e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 5.907099145686869e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0006459351344950152], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 9.505013037587547e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -4.561969266059266e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -3.201080739405175e-05], ["'market for corrugated board box' (kilogram, RER, None)", 7.107201576755263e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.176104412433239e-06], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.000406571962381337], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.927619458904985e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -4.059518539599607e-06], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 1.6280211335475744e-06]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.00040627824320049955], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.543993514940177e-05], ["'market for polysulfone' (kilogram, GLO, None)", 2.0095591546031464e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000616350184568094], ["'cabinet washer - CONSQ' (unit, GLO, None)", 8.311680702169037e-05], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.4911617735488555e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 3.529657156576897e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0003859643310404746], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 4.752506518793773e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.667989696812257e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -4.640932819683732e-07], ["'market for corrugated board box' (kilogram, RER, None)", 4.246751970234578e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.8978113291855574e-06]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.00040627824320049955], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.543993514940177e-05], ["'market for polysulfone' (kilogram, GLO, None)", 2.0095591546031464e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000616350184568094], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.4911617735488555e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 3.529657156576897e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0003859643310404746], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 4.752506518793773e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -4.561969266059266e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -3.201080739405175e-05], ["'market for corrugated board box' (kilogram, RER, None)", 4.246751970234578e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.8978113291855574e-06], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.000406571962381337], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.927619458904985e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -4.059518539599607e-06], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 1.6280211335475744e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.1542416527930872], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.04709841261544819], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.02063117391319887], ["'market for corrugated board box' (kilogram, RER, None)", 0.009064392528043634], ["'autoclave - CONSQ' (unit, GLO, None)", 0.3136194154086757], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.00022704880868272586], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.08329049250826709], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.008701529761054663], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.08382272141506765], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.00012275371607556898], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0023423681624823384], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.10075442332658927], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.006893154355111719]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.1542416527930872], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.04709841261544819], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.02063117391319887], ["'market for corrugated board box' (kilogram, RER, None)", 0.009064392528043634], ["'autoclave - CONSQ' (unit, GLO, None)", 0.3136194154086757], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.00022704880868272586], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.18222330742406012], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.00026685590451210647], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.005092104723376794], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.21903135505018034], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.006893154355111719]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.4388283642845579], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.1339983006805709], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.06222099943016971], ["'market for corrugated board box' (kilogram, RER, None)", 0.02733705682567877], ["'autoclave - CONSQ' (unit, GLO, None)", 0.41815922054490096], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.000684750375565388], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.23696731671366128], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.026242708271574065], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.23848154543441785], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.0004345938928302989], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.006664202419615243], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.28665342969915536], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.01961150957529672]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.4388283642845579], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.1339983006805709], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.06222099943016971], ["'market for corrugated board box' (kilogram, RER, None)", 0.02733705682567877], ["'autoclave - CONSQ' (unit, GLO, None)", 0.41815922054490096], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.003219989759056317], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.5184381422487344], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.0008048035052412941], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.014487396543647602], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.6231596298265071], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.01961150957529672]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.15652274511716874], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.02506742788826223], ["'market for polysulfone' (kilogram, GLO, None)", 0.0021337009725469172], ["'autoclave - CONSQ' (unit, GLO, None)", 0.6272388308173514], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.16276703443760637], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.0017058255370440256], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0050526572112086264], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.14869660786131028], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 0.000757439926670406], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.00013091647106343603], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0011262459663236265], ["'market for corrugated board box' (kilogram, RER, None)", 0.0031990839685017074], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0021586743922518232]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.15652274511716874], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.02506742788826223], ["'market for polysulfone' (kilogram, GLO, None)", 0.0021337009725469172], ["'autoclave - CONSQ' (unit, GLO, None)", 0.6272388308173514], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.0017058255370440256], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0050526572112086264], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.14869660786131028], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 0.000757439926670406], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.004478388124218693], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.038841375330197256], ["'market for corrugated board box' (kilogram, RER, None)", 0.0031990839685017074], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0021586743922518232], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.010868049153376982], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.030809952373161937], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.0003985142941020487], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 0.0018118957594268734]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.09352672332802628], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.01497849012867581], ["'market for polysulfone' (kilogram, GLO, None)", 0.0010668504862734586], ["'autoclave - CONSQ' (unit, GLO, None)", 0.41815922054490096], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.08138351721880319], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.0010192785267698358], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0030191041737117597], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.08885038716162497], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 0.000378719963335203], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.545823553171801e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0005631229831618132], ["'market for corrugated board box' (kilogram, RER, None)", 0.0019115422574496515], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0012898684002959776]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.09352672332802628], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.01497849012867581], ["'market for polysulfone' (kilogram, GLO, None)", 0.0010668504862734586], ["'autoclave - CONSQ' (unit, GLO, None)", 0.41815922054490096], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.0010192785267698358], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0030191041737117597], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.08885038716162497], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 0.000378719963335203], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.004478388124218693], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.038841375330197256], ["'market for corrugated board box' (kilogram, RER, None)", 0.0019115422574496515], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0012898684002959776], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.010868049153376982], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.030809952373161937], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.0003985142941020487], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 0.0018118957594268734]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.002575880061279917], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.002681386540153435], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0004757341683104748], ["'market for corrugated board box' (kilogram, RER, None)", 0.0001428264265713875], ["'autoclave - CONSQ' (unit, GLO, None)", 0.008117449325061815], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 4.499571160094361e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0013909752330911553], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.00014971537875144706], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.004375708434223258], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -5.808364895075279e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.001108343554986862], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.002244252344669314], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.00012908718849570378]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.002575880061279917], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.002681386540153435], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0004757341683104748], ["'market for corrugated board box' (kilogram, RER, None)", 0.0001428264265713875], ["'autoclave - CONSQ' (unit, GLO, None)", 0.008117449325061815], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 4.499571160094361e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.009512409639615778], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.00012626880206685387], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0024094425214061035], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.004878809444763506], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.00012908718849570378]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.007328560174345679], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.007628733536774561], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0014347538118721001], ["'market for corrugated board box' (kilogram, RER, None)", 0.00043074636577255046], ["'autoclave - CONSQ' (unit, GLO, None)", 0.010823265766749086], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.3570135248158271e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.003957422494146667], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0004515225616910651], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.012449198643846453], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.0002056377592003514], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0031533154861022395], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.006385055965478946], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.000367262141947291]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.007328560174345679], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.007628733536774561], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0014347538118721001], ["'market for corrugated board box' (kilogram, RER, None)", 0.00043074636577255046], ["'autoclave - CONSQ' (unit, GLO, None)", 0.010823265766749086], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 6.381259227787924e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.02706347531270968], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.0003808106651858359], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.006855033655629201], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.013880556447712073], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.000367262141947291]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0037239953774620004], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0014142961560177963], ["'market for polysulfone' (kilogram, GLO, None)", 5.2525211287247595e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.01623489865012363], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.006926399749254169], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.632351514481635e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.001537849262441289], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0035377956085889], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 3.7775049817998695e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.194603788971084e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.508654277542893e-05], ["'market for corrugated board box' (kilogram, RER, None)", 5.0407540285717045e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.0425209391520094e-05]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0037239953774620004], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0014142961560177963], ["'market for polysulfone' (kilogram, GLO, None)", 5.2525211287247595e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.01623489865012363], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.632351514481635e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.001537849262441289], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0035377956085889], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 3.7775049817998695e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.002119048872721739], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0008651714215307485], ["'market for corrugated board box' (kilogram, RER, None)", 5.0407540285717045e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.0425209391520094e-05], ["'production of wet wipe - CONSQ' (unit, GLO, None)", -0.00301221424263572], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.000710446585812281], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.0001885658951964494], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 2.354023179482034e-05]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0022251915214112454], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0008450815578831715], ["'market for polysulfone' (kilogram, GLO, None)", 2.6262605643623798e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.010823265766749086], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.0034631998746270844], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.767959750059128e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0009189079988399667], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0021139319453406832], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.8887524908999347e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -3.097301894485542e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.2543271387714466e-05], ["'market for corrugated board box' (kilogram, RER, None)", 3.0119916919646303e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.4155194667907616e-05]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0022251915214112454], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0008450815578831715], ["'market for polysulfone' (kilogram, GLO, None)", 2.6262605643623798e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.010823265766749086], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.767959750059128e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0009189079988399667], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0021139319453406832], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.8887524908999347e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.002119048872721739], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0008651714215307485], ["'market for corrugated board box' (kilogram, RER, None)", 3.0119916919646303e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.4155194667907616e-05], ["'production of wet wipe - CONSQ' (unit, GLO, None)", -0.00301221424263572], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.000710446585812281], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.0001885658951964494], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 2.354023179482034e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0034951468413655707], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.003493197791441804], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0006326924433916711], ["'market for corrugated board box' (kilogram, RER, None)", 0.00020000116535978177], ["'autoclave - CONSQ' (unit, GLO, None)", 0.009204020002652483], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 6.396241821226289e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0018873792943374082], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.00020290888734322889], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.006334986637136535], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -7.171006407607947e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0013683607828049085], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0028768610170369943], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.00016294154332445007]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0034951468413655707], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.003493197791441804], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0006326924433916711], ["'market for corrugated board box' (kilogram, RER, None)", 0.00020000116535978177], ["'autoclave - CONSQ' (unit, GLO, None)", 0.009204020002652483], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 6.396241821226289e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.013771710080731598], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.00015589144364365102], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.002974697366967384], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.006254045688993213], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.00016294154332445007]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.009943938900786552], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.0099383937164964], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0019081200287183278], ["'market for corrugated board box' (kilogram, RER, None)", 0.0006031781176429667], ["'autoclave - CONSQ' (unit, GLO, None)", 0.012272026670203311], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.929025311650959e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.005369727006424739], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0006119474256228533], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.01802348310847296], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.0002538803459338703], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.003893082814962413], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.008184872187976932], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0004635801655524203]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.009943938900786552], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.0099383937164964], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0019081200287183278], ["'market for corrugated board box' (kilogram, RER, None)", 0.0006031781176429667], ["'autoclave - CONSQ' (unit, GLO, None)", 0.012272026670203311], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 9.071103821371131e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.039181485018419476], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.00047014878876642645], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.008463223498675876], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.01779320040995137], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0004635801655524203]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.005214791760272705], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0018439750484988964], ["'market for polysulfone' (kilogram, GLO, None)", 6.729644141243289e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.018408040005304965], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.008443231015985712], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 7.828661645115836e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0021159771037727914], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.004954052172259069], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 5.029642135612412e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -7.647856886706219e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -3.215792427900825e-05], ["'market for corrugated board box' (kilogram, RER, None)", 7.058614460976231e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -5.102710876445776e-05]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.005214791760272705], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0018439750484988964], ["'market for polysulfone' (kilogram, GLO, None)", 6.729644141243289e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.018408040005304965], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 7.828661645115836e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0021159771037727914], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.004954052172259069], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 5.029642135612412e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0026161774128904904], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0011090454874953188], ["'market for corrugated board box' (kilogram, RER, None)", 7.058614460976231e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -5.102710876445776e-05], ["'production of wet wipe - CONSQ' (unit, GLO, None)", -0.000575151872486603], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0009448431839007462], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.00023280342525597167], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 3.126067645767488e-05]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.003115984107045915], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0011018267284773244], ["'market for polysulfone' (kilogram, GLO, None)", 3.3648220706216446e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.012272026670203311], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.004221615507992856], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.6778445596733054e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0012643555734015094], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0029601849016936193], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 2.514821067806206e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -3.8239284433531094e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.6078962139504127e-05], ["'market for corrugated board box' (kilogram, RER, None)", 4.2177198079363444e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.0490126435919597e-05]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.003115984107045915], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0011018267284773244], ["'market for polysulfone' (kilogram, GLO, None)", 3.3648220706216446e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.012272026670203311], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.6778445596733054e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0012643555734015094], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0029601849016936193], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 2.514821067806206e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0026161774128904904], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0011090454874953188], ["'market for corrugated board box' (kilogram, RER, None)", 4.2177198079363444e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.0490126435919597e-05], ["'production of wet wipe - CONSQ' (unit, GLO, None)", -0.000575151872486603], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0009448431839007462], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.00023280342525597167], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 3.126067645767488e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.4246843526982598], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.26410464946150747], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.05097297854386099], ["'market for corrugated board box' (kilogram, RER, None)", 0.014805773880272764], ["'autoclave - CONSQ' (unit, GLO, None)", 1.1292716339098199], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.0008182394338512325], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.22932955045706033], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.024969496910015338], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.24355136923318338], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.003639984059497851], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.06945763472986953], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.22575725177525385], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.023218345690887605]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.4246843526982598], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.26410464946150747], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.05097297854386099], ["'market for corrugated board box' (kilogram, RER, None)", 0.014805773880272764], ["'autoclave - CONSQ' (unit, GLO, None)", 1.1292716339098199], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.0008182394338512325], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.5294594983330074], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.007913008824995328], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.1509948587705053], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.49077663427695084], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.023218345690887605]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.2082568907753308], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.7513963266369649], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.1537280274149883], ["'market for corrugated board box' (kilogram, RER, None)", 0.0446523339165811], ["'autoclave - CONSQ' (unit, GLO, None)", 1.50569551187976], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.0024677062296987484], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.6524587210186786], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.07530483042536665], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.6929207969732823], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.012886899825367042], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.19761186343013165], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.6422952795934875], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.06605782859072676]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.2082568907753308], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.7513963266369649], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.1537280274149883], ["'market for corrugated board box' (kilogram, RER, None)", 0.0446523339165811], ["'autoclave - CONSQ' (unit, GLO, None)", 1.50569551187976], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.011604212383861145], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.5063495586375701], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.02386462930623526], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.429591006842007], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.3962940861752748], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.06605782859072676]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.13224599475672763], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.06762232827194302], ["'market for polysulfone' (kilogram, GLO, None)", 0.008388737139565776], ["'autoclave - CONSQ' (unit, GLO, None)", 2.2585432678196398], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.4854281992055989], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.032035708103587614], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.47366216002384215], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.12563369501889124], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 0.0003957376479410388], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0038820321130095775], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0025235437391768374], ["'market for corrugated board box' (kilogram, RER, None)", 0.005225382033611543], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.007271104880482139]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.13224599475672763], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.06762232827194302], ["'market for polysulfone' (kilogram, GLO, None)", 0.008388737139565776], ["'autoclave - CONSQ' (unit, GLO, None)", 2.2585432678196398], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.032035708103587614], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.47366216002384215], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.12563369501889124], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 0.0003957376479410388], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.13279647985862383], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.087030642032392], ["'market for corrugated board box' (kilogram, RER, None)", 0.005225382033611543], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.007271104880482139], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.02761327726609024], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.07612145813233852], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.011817040855370064], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", -0.0014486263719564294]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.07902068516363756], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0404062347766303], ["'market for polysulfone' (kilogram, GLO, None)", 0.004194368569782888], ["'autoclave - CONSQ' (unit, GLO, None)", 1.50569551187976], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.24271409960279944], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.019142232690710696], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.2830264046183406], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.07506965090545568], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 0.0001978688239705194], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0019410160565047887], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0012617718695884187], ["'market for corrugated board box' (kilogram, RER, None)", 0.0031223120952479397], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.004344688784114543]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.07902068516363756], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0404062347766303], ["'market for polysulfone' (kilogram, GLO, None)", 0.004194368569782888], ["'autoclave - CONSQ' (unit, GLO, None)", 1.50569551187976], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.019142232690710696], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.2830264046183406], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.07506965090545568], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 0.0001978688239705194], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.13279647985862383], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.087030642032392], ["'market for corrugated board box' (kilogram, RER, None)", 0.0031223120952479397], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.004344688784114543], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.02761327726609024], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.07612145813233852], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.011817040855370064], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", -0.0014486263719564294]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.11757236403331361], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.011546059896976347], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.013085324881130274], ["'market for corrugated board box' (kilogram, RER, None)", 0.0010078044055488917], ["'autoclave - CONSQ' (unit, GLO, None)", 0.011794864263106601], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 6.275383538786159e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.06348907657798936], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.006385849014992495], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0003101352144363789], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -2.9267281593496865e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0005584739167065958], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.015215451300440504], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0008178808066219231]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.11757236403331361], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.011546059896976347], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.013085324881130274], ["'market for corrugated board box' (kilogram, RER, None)", 0.0010078044055488917], ["'autoclave - CONSQ' (unit, GLO, None)", 0.011794864263106601], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 6.275383538786159e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0006742069879051715], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -6.362452520325406e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0012140737372944197], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.03307706804328478], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0008178808066219231]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.33450165541872323], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.03284935350970735], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.03946367741350463], ["'market for corrugated board box' (kilogram, RER, None)", 0.0030394101114248266], ["'autoclave - CONSQ' (unit, GLO, None)", 0.015726485684142134], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.00018925759883661535], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.18063089392611056], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.019258909337621453], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0008823565255795569], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.000103617081803439], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0015888976321569858], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.04328903045332324], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0023269284922689485]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.33450165541872323], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.03284935350970735], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.03946367741350463], ["'market for corrugated board box' (kilogram, RER, None)", 0.0030394101114248266], ["'autoclave - CONSQ' (unit, GLO, None)", 0.015726485684142134], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.0008899703480619658], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0019181663599555584], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.00019188348482118331], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.00345412528235449], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.09410658794891366], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0023269284922689485]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.033832419440732626], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.006149296159342674], ["'market for polysulfone' (kilogram, GLO, None)", 0.0011275973997964702], ["'autoclave - CONSQ' (unit, GLO, None)", 0.023589728526213202], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.004343848313710668], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.000535042693546586], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.000971249625905885], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.032140798468696], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 4.876235116799861e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -3.1213468287034964e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00017008028121374185], ["'market for corrugated board box' (kilogram, RER, None)", 0.0003556830650484527], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.00025612923521141666]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.033832419440732626], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.006149296159342674], ["'market for polysulfone' (kilogram, GLO, None)", 0.0011275973997964702], ["'autoclave - CONSQ' (unit, GLO, None)", 0.023589728526213202], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.000535042693546586], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.000971249625905885], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.032140798468696], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 4.876235116799861e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0010677497228335797], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00586563880042361], ["'market for corrugated board box' (kilogram, RER, None)", 0.0003556830650484527], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.00025612923521141666], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.002322671898890378], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.019541216513959615], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -9.50148837639922e-05], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", -3.41135056606014e-05]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.02021581802812413], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0036743766545010107], ["'market for polysulfone' (kilogram, GLO, None)", 0.0005637986998982351], ["'autoclave - CONSQ' (unit, GLO, None)", 0.015726485684142134], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.002171924156855334], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.000319702992242784], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0005803488494694493], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.019205027126717927], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 2.4381175583999304e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.5606734143517482e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -8.504014060687093e-05], ["'market for corrugated board box' (kilogram, RER, None)", 0.00021253059181743317], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.00015304439061166296]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.02021581802812413], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0036743766545010107], ["'market for polysulfone' (kilogram, GLO, None)", 0.0005637986998982351], ["'autoclave - CONSQ' (unit, GLO, None)", 0.015726485684142134], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.000319702992242784], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0005803488494694493], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.019205027126717927], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 2.4381175583999304e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0010677497228335797], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00586563880042361], ["'market for corrugated board box' (kilogram, RER, None)", 0.00021253059181743317], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.00015304439061166296], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.002322671898890378], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.019541216513959615], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -9.50148837639922e-05], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", -3.41135056606014e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.6107683632415326e-05], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 2.1979795666106068e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 4.66479725541961e-06], ["'market for corrugated board box' (kilogram, RER, None)", 6.970377403646815e-06], ["'autoclave - CONSQ' (unit, GLO, None)", -2.297772908378533e-05], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.5474719020016852e-08], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -8.698149161504277e-06], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -1.0066393616264027e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.40526299876735e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -4.784905353066169e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -9.130485265809544e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -8.73795938304418e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.590766710592349e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.6107683632415326e-05], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 2.1979795666106068e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 4.66479725541961e-06], ["'market for corrugated board box' (kilogram, RER, None)", 6.970377403646815e-06], ["'autoclave - CONSQ' (unit, GLO, None)", -2.297772908378533e-05], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.5474719020016852e-08], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.054919562537718e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.0401968158839498e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.9848881099664267e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.8995563875521945e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.590766710592349e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 4.5827494278139374e-05], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 6.253406654300599e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.4068435882149842e-05], ["'market for corrugated board box' (kilogram, RER, None)", 2.1021773118319107e-05], ["'autoclave - CONSQ' (unit, GLO, None)", -3.0636972111713774e-05], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 7.682851769883089e-08], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -2.4746846910195263e-05], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -3.035896425945613e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.998072193676123e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.6940347801229882e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.5976873736272905e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.486010978994426e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.525843317828836e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 4.5827494278139374e-05], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 6.253406654300599e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.4068435882149842e-05], ["'market for corrugated board box' (kilogram, RER, None)", 2.1021773118319107e-05], ["'autoclave - CONSQ' (unit, GLO, None)", -3.0636972111713774e-05], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 3.6128061994774187e-07], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 8.691461290600267e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -3.1371014446722e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.647146456325348e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -5.404371693862777e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.525843317828836e-06]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 5.11835150644143e-05], ["'alubox production - CONSQ' (kilogram, GLO, None)", 1.2403929145125681e-05], ["'market for polysulfone' (kilogram, GLO, None)", 1.9126691235872395e-07], ["'autoclave - CONSQ' (unit, GLO, None)", -4.595545816757066e-05], ["'cabinet washer - CONSQ' (unit, GLO, None)", 3.457256187858905e-06], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.673248658294235e-07], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 2.9829706100578206e-06], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -4.862433931119358e-05], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 3.6405520745686866e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.1030872483757e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -9.767403935362618e-08], ["'market for corrugated board box' (kilogram, RER, None)", 2.4600460027988033e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.981677741853955e-07]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 5.11835150644143e-05], ["'alubox production - CONSQ' (kilogram, GLO, None)", 1.2403929145125681e-05], ["'market for polysulfone' (kilogram, GLO, None)", 1.9126691235872395e-07], ["'autoclave - CONSQ' (unit, GLO, None)", -4.595545816757066e-05], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.673248658294235e-07], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 2.9829706100578206e-06], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -4.862433931119358e-05], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 3.6405520745686866e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.7456631044464828e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -3.3685306194122313e-06], ["'market for corrugated board box' (kilogram, RER, None)", 2.4600460027988033e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.981677741853955e-07], ["'production of wet wipe - CONSQ' (unit, GLO, None)", -5.585643992490576e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.9662628929703256e-06], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.5533975182864459e-07], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 4.105538325255076e-08]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 3.0583583547566214e-05], ["'alubox production - CONSQ' (kilogram, GLO, None)", 7.411695012556751e-06], ["'market for polysulfone' (kilogram, GLO, None)", 9.563345617936197e-08], ["'autoclave - CONSQ' (unit, GLO, None)", -3.0636972111713774e-05], ["'cabinet washer - CONSQ' (unit, GLO, None)", 1.7286280939294524e-06], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 9.998129294635685e-08], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.7824084719039972e-06], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -2.90544043701879e-05], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.8202760372843433e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.55154362418785e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -4.883701967681309e-08], ["'market for corrugated board box' (kilogram, RER, None)", 1.4699463771257078e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.976691956294648e-07]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 3.0583583547566214e-05], ["'alubox production - CONSQ' (kilogram, GLO, None)", 7.411695012556751e-06], ["'market for polysulfone' (kilogram, GLO, None)", 9.563345617936197e-08], ["'autoclave - CONSQ' (unit, GLO, None)", -3.0636972111713774e-05], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 9.998129294635685e-08], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.7824084719039972e-06], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -2.90544043701879e-05], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.8202760372843433e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.7456631044464828e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -3.3685306194122313e-06], ["'market for corrugated board box' (kilogram, RER, None)", 1.4699463771257078e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.976691956294648e-07], ["'production of wet wipe - CONSQ' (unit, GLO, None)", -5.585643992490576e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.9662628929703256e-06], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.5533975182864459e-07], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 4.105538325255076e-08]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.889600857085989e-06], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 2.610063690232733e-06], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.497219433011155e-07], ["'market for corrugated board box' (kilogram, RER, None)", 4.0183387331173233e-07], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00013286553723601384], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 5.416698624596908e-09], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -1.0203844628264341e-06], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -1.1181151213323185e-07], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.3082978885587858e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -5.1120125029280634e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -9.75466626663982e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -7.69691715696436e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 7.777152232684407e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.889600857085989e-06], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 2.610063690232733e-06], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.497219433011155e-07], ["'market for corrugated board box' (kilogram, RER, None)", 4.0183387331173233e-07], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00013286553723601384], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 5.416698624596908e-09], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.8441258446930124e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.1113070658539269e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.1205796324810419e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.6732428601514137e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 7.777152232684407e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 5.376047508892532e-06], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 7.425815006014254e-06], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.9594788369286424e-06], ["'market for corrugated board box' (kilogram, RER, None)", 1.2118799351660813e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00017715404964801845], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.633607522116651e-08], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -2.9030656548019673e-06], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -3.3720931547561873e-07], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.7221996266038696e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.8098428991567045e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.7752712651195124e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.18982713443991e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.2126545790567683e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 5.376047508892532e-06], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 7.425815006014254e-06], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.9594788369286424e-06], ["'market for corrugated board box' (kilogram, RER, None)", 1.2118799351660813e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00017715404964801845], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 7.681922754974344e-08], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 8.091738318704064e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -3.3515609243642666e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.033198393799426e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -4.760493770870923e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.2126545790567683e-05]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 3.692348298539384e-06], ["'alubox production - CONSQ' (kilogram, GLO, None)", 2.0619203610568115e-06], ["'market for polysulfone' (kilogram, GLO, None)", 8.462756924699476e-08], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0002657310744720277], ["'cabinet washer - CONSQ' (unit, GLO, None)", 1.1320412288153831e-05], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.5525177438659536e-08], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 6.292610430619047e-08], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -3.5077308836124148e-06], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 6.849922026495211e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.4519460453930945e-09], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -8.603713479714355e-09], ["'market for corrugated board box' (kilogram, RER, None)", 1.4181869310440799e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.435508985358827e-06]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 3.692348298539384e-06], ["'alubox production - CONSQ' (kilogram, GLO, None)", 2.0619203610568115e-06], ["'market for polysulfone' (kilogram, GLO, None)", 8.462756924699476e-08], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0002657310744720277], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.5525177438659536e-08], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 6.292610430619047e-08], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -3.5077308836124148e-06], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 6.849922026495211e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.865000654634105e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.967203208637608e-07], ["'market for corrugated board box' (kilogram, RER, None)", 1.4181869310440799e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.435508985358827e-06], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.00012707952535413478], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 9.70274508524164e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.6595913502048998e-08], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 4.5676381986026424e-07]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 2.2062815055389833e-06], ["'alubox production - CONSQ' (kilogram, GLO, None)", 1.2320551558728802e-06], ["'market for polysulfone' (kilogram, GLO, None)", 4.231378462349738e-08], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00017715404964801845], ["'cabinet washer - CONSQ' (unit, GLO, None)", 5.6602061440769155e-06], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.7202568365239955e-08], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 3.76001094483108e-08], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -2.095967430262034e-06], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 3.4249610132476057e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.7259730226965472e-09], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -4.3018567398571776e-09], ["'market for corrugated board box' (kilogram, RER, None)", 8.474064058166177e-08], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.4552848220774163e-06]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 2.2062815055389833e-06], ["'alubox production - CONSQ' (kilogram, GLO, None)", 1.2320551558728802e-06], ["'market for polysulfone' (kilogram, GLO, None)", 4.231378462349738e-08], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00017715404964801845], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.7202568365239955e-08], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 3.76001094483108e-08], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -2.095967430262034e-06], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 3.4249610132476057e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.865000654634105e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.967203208637608e-07], ["'market for corrugated board box' (kilogram, RER, None)", 8.474064058166177e-08], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.4552848220774163e-06], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.00012707952535413478], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 9.70274508524164e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.6595913502048998e-08], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 4.5676381986026424e-07]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.003517252466384169], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.0017785803198210638], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0005449558282524257], ["'market for corrugated board box' (kilogram, RER, None)", 0.00027532070921551684], ["'autoclave - CONSQ' (unit, GLO, None)", 0.001364620512139065], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.6041536632474646e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0018993163318474513], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0002603292224294203], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.00019388848660040697], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.783486055448272e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0003403221579004145], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.000851953695479976], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -7.659206092784872e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.003517252466384169], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.0017785803198210638], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0005449558282524257], ["'market for corrugated board box' (kilogram, RER, None)", 0.00027532070921551684], ["'autoclave - CONSQ' (unit, GLO, None)", 0.001364620512139065], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.6041536632474646e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.00042149671000088474], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -3.877143598800591e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0007398307812884433], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0018520732509789732], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -7.659206092784872e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.010006830960698621], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.005060186262026125], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0016435175439759764], ["'market for corrugated board box' (kilogram, RER, None)", 0.0008303322974843852], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00181949401618542], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 7.85379676415959e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.005403688718777256], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0007851198612636768], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0005516263984969325], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -6.314205161566439e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0009682405116559995], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.002423868259982945], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.00021790980716459963]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.010006830960698621], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.005060186262026125], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0016435175439759764], ["'market for corrugated board box' (kilogram, RER, None)", 0.0008303322974843852], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00181949401618542], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.0003693191862716783], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0011991878228194185], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.00011692972521419331], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.002104870674500697], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.005269278826436599], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.00021790980716459963]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.03049272720877801], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.001165474968186897], ["'market for polysulfone' (kilogram, GLO, None)", 4.904841909964629e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00272924102427813], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.002007297634397571], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.2365670834025218e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.00047576668126590743], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.028968090848339106], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 6.736656759332428e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.9020825440950147e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -9.523248521989348e-06], ["'market for corrugated board box' (kilogram, RER, None)", 9.716857079202168e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.3985727296550403e-05]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.03049272720877801], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.001165474968186897], ["'market for polysulfone' (kilogram, GLO, None)", 4.904841909964629e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00272924102427813], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.2365670834025218e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.00047576668126590743], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.028968090848339106], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 6.736656759332428e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0006506640308560747], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00032843275915364747], ["'market for corrugated board box' (kilogram, RER, None)", 9.716857079202168e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.3985727296550403e-05], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.0003744621018078424], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.000813820056220492], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -5.7900054609366824e-05], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 2.640739817933754e-06]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.018220258397829116], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0006964039303920935], ["'market for polysulfone' (kilogram, GLO, None)", 2.4524209549823146e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00181949401618542], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.0010036488171987854], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.3364114631223246e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0002842839149935723], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.017309245477937663], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 3.368328379666214e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -9.510412720475074e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -4.761624260994674e-06], ["'market for corrugated board box' (kilogram, RER, None)", 5.806094213023414e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.4332143749416316e-05]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.018220258397829116], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0006964039303920935], ["'market for polysulfone' (kilogram, GLO, None)", 2.4524209549823146e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00181949401618542], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.3364114631223246e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0002842839149935723], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.017309245477937663], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 3.368328379666214e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0006506640308560747], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00032843275915364747], ["'market for corrugated board box' (kilogram, RER, None)", 5.806094213023414e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.4332143749416316e-05], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.0003744621018078424], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.000813820056220492], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -5.7900054609366824e-05], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 2.640739817933754e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.05867514610319985], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.04857522255953673], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.010937123796594487], ["'market for corrugated board box' (kilogram, RER, None)", 0.005092068621364678], ["'autoclave - CONSQ' (unit, GLO, None)", 0.030221729446096055], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 8.820584758614293e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.03168457889572792], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.003461367295099731], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.05279006118834249], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.000578297916757895], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.011034994882025827], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.033846953585926466], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.007571224971604384]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.05867514610319985], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.04857522255953673], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.010937123796594487], ["'market for corrugated board box' (kilogram, RER, None)", 0.005092068621364678], ["'autoclave - CONSQ' (unit, GLO, None)", 0.030221729446096055], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 8.820584758614293e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.11476100258335324], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.0012571693842562935], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.023989119413941037], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0735803338798882], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.007571224971604384]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.16693492271614604], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.13819992897220307], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.03298497586122507], ["'market for corrugated board box' (kilogram, RER, None)", 0.01535703234737849], ["'autoclave - CONSQ' (unit, GLO, None)", 0.04029563926146141], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.00026601763564448053], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.09014485826671886], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.010439044011849703], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.15019144169077725], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.00204739009859992], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.03139533774882958], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.09629696652448094], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.021540668230827467]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.16693492271614604], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.13819992897220307], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.03298497586122507], ["'market for corrugated board box' (kilogram, RER, None)", 0.01535703234737849], ["'autoclave - CONSQ' (unit, GLO, None)", 0.04029563926146141], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.0012509289415085633], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.3265031341103853], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.003791463145555407], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.06825073413891031], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.20934123159032242], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.021540668230827467]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.13032565584744885], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.02856025811114962], ["'market for polysulfone' (kilogram, GLO, None)", 0.0014311051476188273], ["'autoclave - CONSQ' (unit, GLO, None)", 0.06044345889219211], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.062405983766129255], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.00140736120379972], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.043111645823239425], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.1238093730550764], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 0.0007369206162690872], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0006167529986519748], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0003783456218584972], ["'market for corrugated board box' (kilogram, RER, None)", 0.0017971369887965557], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0023710203808304294]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.13032565584744885], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.02856025811114962], ["'market for polysulfone' (kilogram, GLO, None)", 0.0014311051476188273], ["'autoclave - CONSQ' (unit, GLO, None)", 0.06044345889219211], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.00140736120379972], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.043111645823239425], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.1238093730550764], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 0.0007369206162690872], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.021097874715862962], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.013048183738329177], ["'market for corrugated board box' (kilogram, RER, None)", 0.0017971369887965557], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0023710203808304294], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.03006852054364752], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.016333159939913692], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.0018774175922754415], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 0.00045464490567682323]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0778732288899202], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.017065553996890095], ["'market for polysulfone' (kilogram, GLO, None)", 0.0007155525738094137], ["'autoclave - CONSQ' (unit, GLO, None)", 0.04029563926146141], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.031202991883064628], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.000840937729732779], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.025760415638683427], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.07397956744542418], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 0.0003684603081345436], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0003083764993259874], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0001891728109292486], ["'market for corrugated board box' (kilogram, RER, None)", 0.0010738396773371857], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0014167510749505082]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0778732288899202], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.017065553996890095], ["'market for polysulfone' (kilogram, GLO, None)", 0.0007155525738094137], ["'autoclave - CONSQ' (unit, GLO, None)", 0.04029563926146141], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.000840937729732779], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.025760415638683427], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.07397956744542418], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 0.0003684603081345436], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.021097874715862962], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.013048183738329177], ["'market for corrugated board box' (kilogram, RER, None)", 0.0010738396773371857], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0014167510749505082], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.03006852054364752], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.016333159939913692], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.0018774175922754415], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 0.00045464490567682323]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.002255350308311721], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.004441772806237658], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0009261542488092973], ["'market for corrugated board box' (kilogram, RER, None)", -9.542395253881106e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.001106686692725594], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 3.5998554509729677e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0012178891664883292], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0001548050699876318], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.921512688146157e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -2.9712864071981104e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.669764553239924e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0034524003173216104], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0001837103101131711]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.002255350308311721], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.004441772806237658], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0009261542488092973], ["'market for corrugated board box' (kilogram, RER, None)", -9.542395253881106e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.001106686692725594], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 3.5998554509729677e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.2872853669882952e-06], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -6.459318276517631e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.2325575169785046e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0075052180808727505], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0001837103101131711]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.006416630454633346], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.012637156434647984], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0027931635509381237], ["'market for corrugated board box' (kilogram, RER, None)", -0.00028778652347785823], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0014755822569674588], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.0856706918376308e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.003464980445502007], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0004668724238384532], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.6847120605711605e-06], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.0519460980089878e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.61308795344571e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00982232202795531], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0005226687696603586]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.006416630454633346], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.012637156434647984], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0027931635509381237], ["'market for corrugated board box' (kilogram, RER, None)", -0.00028778652347785823], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0014755822569674588], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 5.1052889259655955e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.662417522980783e-06], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.9480483296462735e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -3.5067129372547175e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.02135287397538301], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0005226687696603586]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0008274258581216459], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0018752795072104864], ["'market for polysulfone' (kilogram, GLO, None)", 0.00011308662079259678], ["'autoclave - CONSQ' (unit, GLO, None)", 0.002213373385451188], ["'cabinet washer - CONSQ' (unit, GLO, None)", 8.559651273248125e-05], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 7.260377921681201e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.00018725643970961882], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0007860545652155636], ["'plastic incineration - CONSQ' (kilogram, CH, None)", -7.254875744731232e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -3.1688680667692706e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -3.85913769653005e-05], ["'market for corrugated board box' (kilogram, RER, None)", -3.367784833164815e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -5.7531098478864144e-05]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0008274258581216459], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0018752795072104864], ["'market for polysulfone' (kilogram, GLO, None)", 0.00011308662079259678], ["'autoclave - CONSQ' (unit, GLO, None)", 0.002213373385451188], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 7.260377921681201e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.00018725643970961882], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0007860545652155636], ["'plastic incineration - CONSQ' (kilogram, CH, None)", -7.254875744731232e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.0840057788113499e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0013309190017446375], ["'market for corrugated board box' (kilogram, RER, None)", -3.367784833164815e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -5.7531098478864144e-05], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.0003322238773375482], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0013830899015281333], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -9.646144678916427e-07], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", -2.364164646650264e-06]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0004944101207084536], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.001120532019179074], ["'market for polysulfone' (kilogram, GLO, None)", 5.654331039629839e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0014755822569674588], ["'cabinet washer - CONSQ' (unit, GLO, None)", 4.279825636624063e-05], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.33827912122086e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.00011189096648543079], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0004696896146730309], ["'plastic incineration - CONSQ' (kilogram, CH, None)", -3.627437872365616e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.5844340333846353e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.929568848265025e-05], ["'market for corrugated board box' (kilogram, RER, None)", -2.0123457483385945e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.4376442426221206e-05]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0004944101207084536], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.001120532019179074], ["'market for polysulfone' (kilogram, GLO, None)", 5.654331039629839e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0014755822569674588], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.33827912122086e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.00011189096648543079], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0004696896146730309], ["'plastic incineration - CONSQ' (kilogram, CH, None)", -3.627437872365616e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.0840057788113499e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0013309190017446375], ["'market for corrugated board box' (kilogram, RER, None)", -2.0123457483385945e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.4376442426221206e-05], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.0003322238773375482], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0013830899015281333], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -9.646144678916427e-07], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", -2.364164646650264e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0017000890525980025], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.002503989405533837], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0008158651922520887], ["'market for corrugated board box' (kilogram, RER, None)", 0.005106828816268815], ["'autoclave - CONSQ' (unit, GLO, None)", 0.16825543378483399], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 7.892479440964108e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0009180480884029214], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -9.774151212120025e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.890777616975627e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.0005851693666298558], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.011166114867022986], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.016528115476612544], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.006324265221133046]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0017000890525980025], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.002503989405533837], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0008158651922520887], ["'market for corrugated board box' (kilogram, RER, None)", 0.005106828816268815], ["'autoclave - CONSQ' (unit, GLO, None)", 0.16825543378483399], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 7.892479440964108e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -4.110386123860059e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.0012721073187605561], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.024274162860836918], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.03593068581747251], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.006324265221133046]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0048368730792224856], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.007124026196025846], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.002460545768059087], ["'market for corrugated board box' (kilogram, RER, None)", 0.015401547220890875], ["'autoclave - CONSQ' (unit, GLO, None)", 0.22434057837977864], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.3802715780351274e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0026119114627801425], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0002947759829655848], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -5.3793954736489674e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.002071717591442624], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.03176838334229084], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.04702365247506063], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.017992979926380392]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0048368730792224856], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.007124026196025846], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.002460545768059087], ["'market for corrugated board box' (kilogram, RER, None)", 0.015401547220890875], ["'autoclave - CONSQ' (unit, GLO, None)", 0.22434057837977864], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.0001119305717608042], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.00011694337986193407], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.0038365140582270808], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.06906170281918723], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.10222533147502556], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.017992979926380392]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0015002092875017413], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0029475230312975362], ["'market for polysulfone' (kilogram, GLO, None)", -2.4624839406446756e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.33651086756966797], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.069985841831298], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 6.877537770762638e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0010375830249309001], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0014251988231266542], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.1170202915333108e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0006240813793893255], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00018475341103514135], ["'market for corrugated board box' (kilogram, RER, None)", 0.001802346284702894], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0019805199012473667]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0015002092875017413], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0029475230312975362], ["'market for polysulfone' (kilogram, GLO, None)", -2.4624839406446756e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.33651086756966797], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 6.877537770762638e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0010375830249309001], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0014251988231266542], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.1170202915333108e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.02134856382317935], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0063716779425854915], ["'market for corrugated board box' (kilogram, RER, None)", 0.001802346284702894], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0019805199012473667], ["'production of wet wipe - CONSQ' (unit, GLO, None)", -0.010429304020692188], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0012183876604387558], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.0018997254382839182], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", -0.0004015194186031602]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0008964170597779814], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0017612275509529892], ["'market for polysulfone' (kilogram, GLO, None)", -1.2312419703223378e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.22434057837977864], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.034992920915649], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.109521410339819e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0006199849129270385], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0008515962067890824], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 5.585101457666554e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.00031204068969466274], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -9.237670551757067e-05], ["'market for corrugated board box' (kilogram, RER, None)", 0.0010769523775209166], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0011834161029313202]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0008964170597779814], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0017612275509529892], ["'market for polysulfone' (kilogram, GLO, None)", -1.2312419703223378e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.22434057837977864], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.109521410339819e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0006199849129270385], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0008515962067890824], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 5.585101457666554e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.02134856382317935], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0063716779425854915], ["'market for corrugated board box' (kilogram, RER, None)", 0.0010769523775209166], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0011834161029313202], ["'production of wet wipe - CONSQ' (unit, GLO, None)", -0.010429304020692188], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0012183876604387558], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.0018997254382839182], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", -0.0004015194186031602]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.00015443045132739234], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 7.391801978784976e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 2.2017600119227295e-05], ["'market for corrugated board box' (kilogram, RER, None)", 1.064265430836516e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0006835164091632984], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 3.864587460542977e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -8.339244371679187e-05], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -6.646838932200662e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 8.698552676877363e-06], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.542409954457635e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.9432037467552094e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -5.371829091195071e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.238972508580597e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.00015443045132739234], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 7.391801978784976e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 2.2017600119227295e-05], ["'market for corrugated board box' (kilogram, RER, None)", 1.064265430836516e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0006835164091632984], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 3.864587460542977e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.8909897123646443e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -3.3530651183861628e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.398269042740835e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0001167788932827854], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.238972508580597e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0004393655094103275], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00021030197179078383], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.640228472872845e-05], ["'market for corrugated board box' (kilogram, RER, None)", 3.209689394007594e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0009113552122177312], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.1655105042678095e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.00023725737508157685], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -2.0046021770399717e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.4747994939848278e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -5.460705939323969e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -8.373621979971138e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0001528323205977195], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.2060175307085602e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0004393655094103275], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00021030197179078383], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.640228472872845e-05], ["'market for corrugated board box' (kilogram, RER, None)", 3.209689394007594e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0009113552122177312], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 5.480729944421238e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.379998899967016e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.0112418406155496e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0001820352601736389], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0003322441752368176], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.2060175307085602e-05]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.001909903381614274], ["'alubox production - CONSQ' (kilogram, GLO, None)", 5.383540016672161e-05], ["'market for polysulfone' (kilogram, GLO, None)", 2.2951165960977628e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0013670328183265968], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.0001925900372458725], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 7.255637685124479e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", -0.00018516774676524117], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.00181440821253356], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 8.908884162993076e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.6449756033976153e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -6.004699988334661e-07], ["'market for corrugated board box' (kilogram, RER, None)", 3.7560977941833362e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.3274853473934867e-06]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.001909903381614274], ["'alubox production - CONSQ' (kilogram, GLO, None)", 5.383540016672161e-05], ["'market for polysulfone' (kilogram, GLO, None)", 2.2951165960977628e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0013670328183265968], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 7.255637685124479e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", -0.00018516774676524117], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.00181440821253356], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 8.908884162993076e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.627129380317419e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.0708691792563442e-05], ["'market for corrugated board box' (kilogram, RER, None)", 3.7560977941833362e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.3274853473934867e-06], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 2.90697019629001e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 3.288039807617217e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -5.007362985559282e-06], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 8.483230911981653e-07]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.001141220753710808], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.216815915717201e-05], ["'market for polysulfone' (kilogram, GLO, None)", 1.1475582980488814e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0009113552122177312], ["'cabinet washer - CONSQ' (unit, GLO, None)", 9.629501862293625e-05], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.335446697136949e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", -0.00011064291396130866], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0010841597160252676], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 4.454442081496538e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -8.224878016988077e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -3.002349994167331e-07], ["'market for corrugated board box' (kilogram, RER, None)", 2.2443736167567994e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -7.93209669603121e-07]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.001141220753710808], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.216815915717201e-05], ["'market for polysulfone' (kilogram, GLO, None)", 1.1475582980488814e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0009113552122177312], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.335446697136949e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", -0.00011064291396130866], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0010841597160252676], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 4.454442081496538e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.627129380317419e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.0708691792563442e-05], ["'market for corrugated board box' (kilogram, RER, None)", 2.2443736167567994e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -7.93209669603121e-07], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 2.90697019629001e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 3.288039807617217e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -5.007362985559282e-06], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 8.483230911981653e-07]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.1390439608595256e-08], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 1.5366018306686846e-08], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 3.0761387717593778e-09], ["'market for corrugated board box' (kilogram, RER, None)", 1.2242259622376303e-09], ["'autoclave - CONSQ' (unit, GLO, None)", -1.944112734983769e-07], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 6.943037542027535e-11], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -6.150837388641439e-09], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -1.2857762786126436e-09], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 6.5080690789901095e-09], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -5.618410544827927e-10], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.0720967482449381e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.6761919027072856e-08], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -9.475535564947016e-10]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.1390439608595256e-08], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 1.5366018306686846e-08], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 3.0761387717593778e-09], ["'market for corrugated board box' (kilogram, RER, None)", 1.2242259622376303e-09], ["'autoclave - CONSQ' (unit, GLO, None)", -1.944112734983769e-07], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 6.943037542027535e-11], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.4147976258674152e-08], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.2213935967017234e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.330645115099883e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -5.81780848394381e-08], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -9.475535564947016e-10]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 3.2406602830087913e-08], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 4.371740419648934e-08], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 9.27724372689787e-09], ["'market for corrugated board box' (kilogram, RER, None)", 3.6921100441779405e-09], ["'autoclave - CONSQ' (unit, GLO, None)", -2.592150313311692e-07], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.0939319576485633e-10], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -1.7499565528247473e-08], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -3.877737904564959e-09], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.8515914844450735e-08], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.9891266743341663e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -3.050190767681859e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -7.613954426174581e-08], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.6958565975708696e-09]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 3.2406602830087913e-08], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 4.371740419648934e-08], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 9.27724372689787e-09], ["'market for corrugated board box' (kilogram, RER, None)", 3.6921100441779405e-09], ["'autoclave - CONSQ' (unit, GLO, None)", -2.592150313311692e-07], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 9.846565552040756e-10], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 4.02519887922842e-08], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -3.6835679154336406e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.630849485470951e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.6552074840724738e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.6958565975708696e-09]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 2.9426490598608053e-08], ["'alubox production - CONSQ' (kilogram, GLO, None)", 6.159776879286204e-09], ["'market for polysulfone' (kilogram, GLO, None)", 8.608425911461889e-10], ["'autoclave - CONSQ' (unit, GLO, None)", -3.888225469967538e-07], ["'cabinet washer - CONSQ' (unit, GLO, None)", 3.865988162882121e-08], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 7.510652856842942e-10], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 2.8252359290012935e-09], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -2.7955166068677648e-08], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 3.2674656970296917e-10], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.992018042546741e-10], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.9914818982807066e-10], ["'market for corrugated board box' (kilogram, RER, None)", 4.320644364750669e-10], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.967378202078723e-10]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 2.9426490598608053e-08], ["'alubox production - CONSQ' (kilogram, GLO, None)", 6.159776879286204e-09], ["'market for polysulfone' (kilogram, GLO, None)", 8.608425911461889e-10], ["'autoclave - CONSQ' (unit, GLO, None)", -3.888225469967538e-07], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 7.510652856842942e-10], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 2.8252359290012935e-09], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -2.7955166068677648e-08], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 3.2674656970296917e-10], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.04974837954826e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.0316864581890436e-08], ["'market for corrugated board box' (kilogram, RER, None)", 4.320644364750669e-10], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.967378202078723e-10], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 1.7828518486191989e-07], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 4.593809806940272e-09], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.8239911457093788e-09], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 2.304408595474606e-08]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 1.7583152165332816e-08], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.6806391781598138e-09], ["'market for polysulfone' (kilogram, GLO, None)", 4.3042129557309444e-10], ["'autoclave - CONSQ' (unit, GLO, None)", -2.592150313311692e-07], ["'cabinet washer - CONSQ' (unit, GLO, None)", 1.9329940814410604e-08], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.487825403451534e-10], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.6881575829142531e-09], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -1.6703994557066173e-08], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.6337328485148458e-10], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.9960090212733706e-10], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.4957409491403533e-10], ["'market for corrugated board box' (kilogram, RER, None)", 2.5817060020780766e-10], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.773091573387197e-10]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 1.7583152165332816e-08], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.6806391781598138e-09], ["'market for polysulfone' (kilogram, GLO, None)", 4.3042129557309444e-10], ["'autoclave - CONSQ' (unit, GLO, None)", -2.592150313311692e-07], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.487825403451534e-10], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.6881575829142531e-09], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -1.6703994557066173e-08], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.6337328485148458e-10], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.04974837954826e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.0316864581890436e-08], ["'market for corrugated board box' (kilogram, RER, None)", 2.5817060020780766e-10], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.773091573387197e-10], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 1.7828518486191989e-07], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 4.593809806940272e-09], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.8239911457093788e-09], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 2.304408595474606e-08]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.00014168997134467824], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00011137929805245783], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 2.4109122727607444e-05], ["'market for corrugated board box' (kilogram, RER, None)", 1.6328052074237104e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0002012539542205681], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 4.449414831409708e-07], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -7.651258452612626e-05], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -8.30383797456183e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.996131450780361e-06], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -4.4095347002889386e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -8.414208566166241e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -5.0787150428346334e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -8.888003634907142e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.00014168997134467824], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00011137929805245783], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 2.4109122727607444e-05], ["'market for corrugated board box' (kilogram, RER, None)", 1.6328052074237104e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0002012539542205681], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 4.449414831409708e-07], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 4.339416197348611e-06], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -9.585945000628128e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.829175783274234e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00011040684875343242], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -8.888003634907142e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0004031179466426057], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00031688194657178144], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 7.27100511976521e-05], ["'market for corrugated board box' (kilogram, RER, None)", 4.9243331643582276e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0002683386056274241], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.3418870129864744e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.00021768369118700708], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -2.5043320368352365e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.679134550107507e-06], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.5611395827635214e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.3939016070969654e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.000144493019504886], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.5286996259120968e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0004031179466426057], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00031688194657178144], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 7.27100511976521e-05], ["'market for corrugated board box' (kilogram, RER, None)", 4.9243331643582276e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0002683386056274241], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 6.310127885741498e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.2345944674146753e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -2.890999227339854e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.204133921023868e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0003141152598162838], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.5286996259120968e-05]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0003070959975220654], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.269211273872963e-05], ["'market for polysulfone' (kilogram, GLO, None)", 1.8956198489533308e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0004025079084411362], ["'cabinet washer - CONSQ' (unit, GLO, None)", 6.212970614681401e-05], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.411296257488632e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.9268351301255548e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0002917411976459621], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 3.50440480181107e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -4.702755569845327e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -5.677053316616167e-07], ["'market for corrugated board box' (kilogram, RER, None)", 5.762637646808395e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.7833854947245283e-06]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0003070959975220654], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.269211273872963e-05], ["'market for polysulfone' (kilogram, GLO, None)", 1.8956198489533308e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0004025079084411362], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.411296257488632e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.9268351301255548e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0002917411976459621], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 3.50440480181107e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.6087177208506912e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.9578721277024118e-05], ["'market for corrugated board box' (kilogram, RER, None)", 5.762637646808395e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.7833854947245283e-06], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 4.867140766356924e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 3.600381277970284e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.4315351620983423e-06], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 5.476801820179796e-07]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.00018349845815629013], ["'alubox production - CONSQ' (kilogram, GLO, None)", 1.9534452841566142e-05], ["'market for polysulfone' (kilogram, GLO, None)", 9.478099244766654e-07], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0002683386056274241], ["'cabinet washer - CONSQ' (unit, GLO, None)", 3.1064853073407005e-05], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 8.432890345055666e-07], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.1513379475875757e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.00017432353524847563], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.752202400905535e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.3513777849226634e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.8385266583080837e-07], ["'market for corrugated board box' (kilogram, RER, None)", 3.443337369291871e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.6631507782617617e-06]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.00018349845815629013], ["'alubox production - CONSQ' (kilogram, GLO, None)", 1.9534452841566142e-05], ["'market for polysulfone' (kilogram, GLO, None)", 9.478099244766654e-07], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0002683386056274241], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 8.432890345055666e-07], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.1513379475875757e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.00017432353524847563], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.752202400905535e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.6087177208506912e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.9578721277024118e-05], ["'market for corrugated board box' (kilogram, RER, None)", 3.443337369291871e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.6631507782617617e-06], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 4.867140766356924e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 3.600381277970284e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.4315351620983423e-06], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 5.476801820179796e-07]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0002935749893174448], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.0001387753076477897], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 4.3243948373555644e-05], ["'market for corrugated board box' (kilogram, RER, None)", 1.1226053340561828e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00037007040312632286], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.3446821182988132e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0001585304942314202], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -1.7558362767586567e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.3645575151839235e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.4600373811464844e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.7860216268534373e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00011080807991803284], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.326310774277151e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0002935749893174448], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.0001387753076477897], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 4.3243948373555644e-05], ["'market for corrugated board box' (kilogram, RER, None)", 1.1226053340561828e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00037007040312632286], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.3446821182988132e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.966429380834616e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -3.1739943068401833e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.0565687805864964e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00024088713024821013], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.326310774277151e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0008352415189031528], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.000394825523166951], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00013041825435768927], ["'market for corrugated board box' (kilogram, RER, None)", 3.385635133844707e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0004934272041684305], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 7.07126353316432e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0004510304202077025], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -5.2953791400972424e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.882262226297923e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -5.169076337856718e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -7.926427776879018e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00031525679070111627], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.7734475552932816e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0008352415189031528], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.000394825523166951], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00013041825435768927], ["'market for corrugated board box' (kilogram, RER, None)", 3.385635133844707e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0004934272041684305], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 3.3252111970843614e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 8.439700491952006e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -9.572363588623551e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.00017231364707685353], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0006853408494005509], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.7734475552932816e-05]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.00040270113347142325], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.55134149702434e-05], ["'market for polysulfone' (kilogram, GLO, None)", 3.841999494362337e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0007401408062526457], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.00017398150328724294], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 3.092243820393865e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.7908722229360266e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0003825660767978521], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 2.012315978333832e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.5571255003207255e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.238627039124905e-06], ["'market for corrugated board box' (kilogram, RER, None)", 3.961996036714828e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.15350209367736e-06]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.00040270113347142325], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.55134149702434e-05], ["'market for polysulfone' (kilogram, GLO, None)", 3.841999494362337e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0007401408062526457], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 3.092243820393865e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.7908722229360266e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0003825660767978521], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 2.012315978333832e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.3266119166742874e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -4.2717114342105416e-05], ["'market for corrugated board box' (kilogram, RER, None)", 3.961996036714828e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.15350209367736e-06], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.0007846475745748834], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.457916526816494e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -4.739944214413862e-06], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 4.816899922592571e-06]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.00024062520412525756], ["'alubox production - CONSQ' (kilogram, GLO, None)", 2.1220259930075914e-05], ["'market for polysulfone' (kilogram, GLO, None)", 1.9209997471811684e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0004934272041684305], ["'cabinet washer - CONSQ' (unit, GLO, None)", 8.699075164362147e-05], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.8477022750673254e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.0700963031603065e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0002285939439189947], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.006157989166916e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -7.785627501603627e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -6.193135195624525e-07], ["'market for corrugated board box' (kilogram, RER, None)", 2.3674035825872675e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.481833814505466e-06]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.00024062520412525756], ["'alubox production - CONSQ' (kilogram, GLO, None)", 2.1220259930075914e-05], ["'market for polysulfone' (kilogram, GLO, None)", 1.9209997471811684e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0004934272041684305], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.8477022750673254e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.0700963031603065e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0002285939439189947], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.006157989166916e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.3266119166742874e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -4.2717114342105416e-05], ["'market for corrugated board box' (kilogram, RER, None)", 2.3674035825872675e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.481833814505466e-06], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.0007846475745748834], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.457916526816494e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -4.739944214413862e-06], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 4.816899922592571e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.000317642348754344], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00014298353781804255], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 4.8239456800970866e-05], ["'market for corrugated board box' (kilogram, RER, None)", 1.1597092085675906e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0003776406112181805], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.395849469652867e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0001715268683273458], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -1.910963649336365e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.379367762451718e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.4920981622522928e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.8471995327673646e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0001171029226109728], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.3605872382790101e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.000317642348754344], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00014298353781804255], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 4.8239456800970866e-05], ["'market for corrugated board box' (kilogram, RER, None)", 1.1597092085675906e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0003776406112181805], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.395849469652867e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.998625570547213e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -3.2436916570702013e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.189564228808637e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0002545715708845599], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.3605872382790101e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0009037148513855984], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.0004067982343555577], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00014548407311930413], ["'market for corrugated board box' (kilogram, RER, None)", 3.497535707747824e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000503520814957574], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 7.2255777674457005e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0004880060197482232], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -5.763223587600363e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.924398422749959e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -5.282583448789114e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -8.100483228600373e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0003331660614583805], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.870966509222013e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0009037148513855984], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.0004067982343555577], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00014548407311930413], ["'market for corrugated board box' (kilogram, RER, None)", 3.497535707747824e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000503520814957574], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 3.397776364157455e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 8.531300919021649e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -9.782561942202061e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.00017609746123929397], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0007242740467018087], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.870966509222013e-05]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0004126359538879128], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.816335531480803e-05], ["'market for polysulfone' (kilogram, GLO, None)", 3.88155116343156e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000755281222436361], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.00017789009719927412], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 3.4545200183282885e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.8623214273884847e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0003920041561935171], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 2.0352750182351766e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.5913182274828571e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.3089916043468713e-06], ["'market for corrugated board box' (kilogram, RER, None)", 4.0929462462865255e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.2608429731730944e-06]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0004126359538879128], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.816335531480803e-05], ["'market for polysulfone' (kilogram, GLO, None)", 3.88155116343156e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000755281222436361], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 3.4545200183282885e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.8623214273884847e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0003920041561935171], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 2.0352750182351766e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.4435783319875614e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -4.514381025885438e-05], ["'market for corrugated board box' (kilogram, RER, None)", 4.0929462462865255e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.2608429731730944e-06], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.0012260816744973165], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 7.203930192233402e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -4.844028065878497e-06], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 4.7009143857956334e-06]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.00024656153752978025], ["'alubox production - CONSQ' (kilogram, GLO, None)", 2.2803673492471236e-05], ["'market for polysulfone' (kilogram, GLO, None)", 1.94077558171578e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000503520814957574], ["'cabinet washer - CONSQ' (unit, GLO, None)", 8.894504859963706e-05], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.0641724481861174e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.1127892036191524e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.00023423346065329126], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.0176375091175883e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -7.956591137414286e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -6.544958021734357e-07], ["'market for corrugated board box' (kilogram, RER, None)", 2.4456499999001035e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.5459729959487106e-06]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.00024656153752978025], ["'alubox production - CONSQ' (kilogram, GLO, None)", 2.2803673492471236e-05], ["'market for polysulfone' (kilogram, GLO, None)", 1.94077558171578e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000503520814957574], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.0641724481861174e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.1127892036191524e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.00023423346065329126], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.0176375091175883e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.4435783319875614e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -4.514381025885438e-05], ["'market for corrugated board box' (kilogram, RER, None)", 2.4456499999001035e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.5459729959487106e-06], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.0012260816744973165], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 7.203930192233402e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -4.844028065878497e-06], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 4.7009143857956334e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0011196636272355163], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00032141079905200864], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00032401647559544063], ["'market for corrugated board box' (kilogram, RER, None)", 3.806130102374293e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0005504119066706546], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 4.711286406182188e-07], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0006046183587071789], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -7.04324891423178e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 4.1055814094313594e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.2988225258344675e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.4783938364494434e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00014662113252027055], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0002098095686832082]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0011196636272355163], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00032141079905200864], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00032401647559544063], ["'market for corrugated board box' (kilogram, RER, None)", 3.806130102374293e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0005504119066706546], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 4.711286406182188e-07], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 8.925176977024695e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -2.823527230074929e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.387812711558447e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00031874159242427835], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0002098095686832082]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0031855218690362576], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.000914436357866278], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0009771925256512753], ["'market for corrugated board box' (kilogram, RER, None)", 0.00011478805068582941], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0007338825422275394], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.420864154604482e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0017201818092795792], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.00021241543914212013], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.00011680668235283588], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -4.598315681543951e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -7.051205043754697e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0004171474473837644], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0005969229982741224]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0031855218690362576], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.000914436357866278], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0009771925256512753], ["'market for corrugated board box' (kilogram, RER, None)", 0.00011478805068582941], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0007338825422275394], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 6.6815122562860895e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0002539275703322519], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -8.515399410266577e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.00015328706594920652], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0009068422769877813], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0005969229982741224]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0008862513405582456], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0006035256209839753], ["'market for polysulfone' (kilogram, GLO, None)", 3.468695127676702e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0011008238133413091], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.00018270602189388239], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.4786413443271393e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.257875181621341e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0008419387735303332], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.1081310681762825e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.3851903392909875e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.6389499699034864e-06], ["'market for corrugated board box' (kilogram, RER, None)", 1.3432924219539876e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -6.57043959606068e-05]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0008862513405582456], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0006035256209839753], ["'market for polysulfone' (kilogram, GLO, None)", 3.468695127676702e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0011008238133413091], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.4786413443271393e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.257875181621341e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0008419387735303332], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.1081310681762825e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -4.738456448507028e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -5.6523239888918186e-05], ["'market for corrugated board box' (kilogram, RER, None)", 1.3432924219539876e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -6.57043959606068e-05], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.010838951150681493], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00048387611016301375], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -4.2165676005125665e-06], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 3.718321589217504e-06]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0005295599937596006], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0003606234591202047], ["'market for polysulfone' (kilogram, GLO, None)", 1.734347563838351e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0007338825422275394], ["'cabinet washer - CONSQ' (unit, GLO, None)", 9.135301094694119e-05], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.4810576128520979e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 7.516156454106661e-06], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0005030819940716205], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 5.540655340881412e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.925951696454937e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -8.194749849517432e-07], ["'market for corrugated board box' (kilogram, RER, None)", 8.026548393100001e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.9260216554343014e-05]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0005295599937596006], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0003606234591202047], ["'market for polysulfone' (kilogram, GLO, None)", 1.734347563838351e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0007338825422275394], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.4810576128520979e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 7.516156454106661e-06], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0005030819940716205], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 5.540655340881412e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -4.738456448507028e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -5.6523239888918186e-05], ["'market for corrugated board box' (kilogram, RER, None)", 8.026548393100001e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.9260216554343014e-05], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.010838951150681493], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00048387611016301375], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -4.2165676005125665e-06], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 3.718321589217504e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 5.757589568054192e-10], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 2.2601734744686658e-10], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 8.518376808030966e-11], ["'market for corrugated board box' (kilogram, RER, None)", 8.138664770554284e-11], ["'autoclave - CONSQ' (unit, GLO, None)", 2.5211332673493153e-09], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.2814611037247904e-12], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -3.109098366749264e-10], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -3.2772614457535437e-11], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.441007470333537e-10], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -6.111343873626605e-12], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.1661575532875856e-10], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -4.717017418144127e-10], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -8.071351980028816e-11]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 5.757589568054192e-10], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 2.2601734744686658e-10], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 8.518376808030966e-11], ["'market for corrugated board box' (kilogram, RER, None)", 8.138664770554284e-11], ["'autoclave - CONSQ' (unit, GLO, None)", 2.5211332673493153e-09], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.2814611037247904e-12], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.30653797898595e-10], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.3285530160057834e-11], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.535125126958779e-10], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.0254385691260812e-09], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -8.071351980028816e-11]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.6380747785168264e-09], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 6.430352702009443e-10], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 2.5690342233961884e-10], ["'market for corrugated board box' (kilogram, RER, None)", 2.454517946232539e-10], ["'autoclave - CONSQ' (unit, GLO, None)", 3.3615110231324204e-09], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 3.864723964591084e-12], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -8.845603803990862e-10], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -9.883804159989819e-11], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 6.944838155033444e-10], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -2.1636434393798238e-11], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -3.31780038370903e-10], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.3420246736748824e-09], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.2963564790122821e-10]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.6380747785168264e-09], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 6.430352702009443e-10], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 2.5690342233961884e-10], ["'market for corrugated board box' (kilogram, RER, None)", 2.454517946232539e-10], ["'autoclave - CONSQ' (unit, GLO, None)", 3.3615110231324204e-09], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.817358855376704e-11], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.5097474250072704e-09], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -4.006747109962636e-11], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -7.212609519480051e-10], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.9174449429855987e-09], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.2963564790122821e-10]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 6.880138454036532e-10], ["'alubox production - CONSQ' (kilogram, GLO, None)", 1.240919621881071e-10], ["'market for polysulfone' (kilogram, GLO, None)", 7.37809084738171e-12], ["'autoclave - CONSQ' (unit, GLO, None)", 5.0422665346986306e-09], ["'cabinet washer - CONSQ' (unit, GLO, None)", 1.14807229314759e-09], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 6.8801639197282534e-12], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 4.697413903335787e-11], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -6.536131531334705e-10], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 2.2066908919746314e-12], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.517729963448163e-12], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -5.272743036842063e-12], ["'market for corrugated board box' (kilogram, RER, None)", 2.872368105412271e-11], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.527641183200643e-11]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 6.880138454036532e-10], ["'alubox production - CONSQ' (kilogram, GLO, None)", 1.240919621881071e-10], ["'market for polysulfone' (kilogram, GLO, None)", 7.37809084738171e-12], ["'autoclave - CONSQ' (unit, GLO, None)", 5.0422665346986306e-09], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 6.8801639197282534e-12], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 4.697413903335787e-11], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -6.536131531334705e-10], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 2.2066908919746314e-12], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.2295838123399307e-10], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.8184357363977212e-10], ["'market for corrugated board box' (kilogram, RER, None)", 2.872368105412271e-11], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.527641183200643e-11], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 1.4282697117787904e-10], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.272107854144826e-10], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.984019684026415e-11], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 2.49490926141749e-12]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 4.1110753914231425e-10], ["'alubox production - CONSQ' (kilogram, GLO, None)", 7.414842236577893e-11], ["'market for polysulfone' (kilogram, GLO, None)", 3.689045423690855e-12], ["'autoclave - CONSQ' (unit, GLO, None)", 3.3615110231324204e-09], ["'cabinet washer - CONSQ' (unit, GLO, None)", 5.74036146573795e-10], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.111090607887061e-12], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 2.806836349347417e-11], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -3.9055216218519856e-10], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.1033454459873157e-12], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -3.2588649817240815e-12], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.6363715184210316e-12], ["'market for corrugated board box' (kilogram, RER, None)", 1.7163203799923082e-11], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.5103363903326964e-11]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 4.1110753914231425e-10], ["'alubox production - CONSQ' (kilogram, GLO, None)", 7.414842236577893e-11], ["'market for polysulfone' (kilogram, GLO, None)", 3.689045423690855e-12], ["'autoclave - CONSQ' (unit, GLO, None)", 3.3615110231324204e-09], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.111090607887061e-12], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 2.806836349347417e-11], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -3.9055216218519856e-10], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.1033454459873157e-12], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.2295838123399307e-10], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.8184357363977212e-10], ["'market for corrugated board box' (kilogram, RER, None)", 1.7163203799923082e-11], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.5103363903326964e-11], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 1.4282697117787904e-10], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.272107854144826e-10], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.984019684026415e-11], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 2.49490926141749e-12]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 2.5998969977386397e-07], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 1.315906263224426e-07], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 3.936728051402973e-08], ["'market for corrugated board box' (kilogram, RER, None)", 2.084536093333721e-08], ["'autoclave - CONSQ' (unit, GLO, None)", 4.303883193640819e-07], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 6.002837272676786e-10], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -1.4039443787788655e-07], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -1.5120211529131917e-08], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 9.183485854562929e-08], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -5.867817909548312e-10], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.1196882908300931e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.3644570721830188e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.4445082352527581e-08]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 2.5998969977386397e-07], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 1.315906263224426e-07], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 3.936728051402973e-08], ["'market for corrugated board box' (kilogram, RER, None)", 2.084536093333721e-08], ["'autoclave - CONSQ' (unit, GLO, None)", 4.303883193640819e-07], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 6.002837272676786e-10], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.9964099683832457e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.2756125890322416e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.434104990738661e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.9662110263815975e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.4445082352527581e-08]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 7.396890049904298e-07], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 3.7438459883286484e-07], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.1872671660548197e-07], ["'market for corrugated board box' (kilogram, RER, None)", 6.286696153365e-08], ["'autoclave - CONSQ' (unit, GLO, None)", 5.738510924854425e-07], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.8103794953917617e-09], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -3.994320626948321e-07], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -4.5600637021254796e-08], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.6127663980587493e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -2.077426174340871e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -3.185592058703976e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -3.88197645825155e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.109727655561152e-08]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 7.396890049904298e-07], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 3.7438459883286484e-07], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.1872671660548197e-07], ["'market for corrugated board box' (kilogram, RER, None)", 6.286696153365e-08], ["'autoclave - CONSQ' (unit, GLO, None)", 5.738510924854425e-07], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 8.513180340140398e-09], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.679926952301628e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -3.84708550803865e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.925200117706473e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -8.439079257687942e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.109727655561152e-08]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 4.7148338047659613e-07], ["'alubox production - CONSQ' (kilogram, GLO, None)", 5.558141419749438e-08], ["'market for polysulfone' (kilogram, GLO, None)", 3.741766550065263e-09], ["'autoclave - CONSQ' (unit, GLO, None)", 8.607766387281638e-07], ["'cabinet washer - CONSQ' (unit, GLO, None)", 2.11584331074012e-07], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.8740620316219478e-09], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 2.823891033022743e-08], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -4.4790921145276626e-07], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 9.182376688278926e-10], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.258010251094816e-10], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.5252077507175098e-09], ["'market for corrugated board box' (kilogram, RER, None)", 7.356925439091028e-09], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.523651692964974e-09]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 4.7148338047659613e-07], ["'alubox production - CONSQ' (kilogram, GLO, None)", 5.558141419749438e-08], ["'market for polysulfone' (kilogram, GLO, None)", 3.741766550065263e-09], ["'autoclave - CONSQ' (unit, GLO, None)", 8.607766387281638e-07], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.8740620316219478e-09], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 2.823891033022743e-08], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -4.4790921145276626e-07], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 9.182376688278926e-10], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.1407389430900466e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -5.2600558380265754e-08], ["'market for corrugated board box' (kilogram, RER, None)", 7.356925439091028e-09], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.523651692964974e-09], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 7.368453535230518e-08], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 5.878987026143975e-08], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.904960099703577e-09], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 2.164226678597048e-09]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 2.8172452282630134e-07], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.3211451434346776e-08], ["'market for polysulfone' (kilogram, GLO, None)", 1.8708832750326313e-09], ["'autoclave - CONSQ' (unit, GLO, None)", 5.738510924854425e-07], ["'cabinet washer - CONSQ' (unit, GLO, None)", 1.05792165537006e-07], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.7173325465118384e-09], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.687353969905826e-08], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -2.676382966849863e-07], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 4.591188344139463e-10], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -3.129005125547408e-10], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -7.626038753587549e-10], ["'market for corrugated board box' (kilogram, RER, None)", 4.395968971178735e-09], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.7030085656476538e-09]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 2.8172452282630134e-07], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.3211451434346776e-08], ["'market for polysulfone' (kilogram, GLO, None)", 1.8708832750326313e-09], ["'autoclave - CONSQ' (unit, GLO, None)", 5.738510924854425e-07], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.7173325465118384e-09], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.687353969905826e-08], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -2.676382966849863e-07], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 4.591188344139463e-10], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.1407389430900466e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -5.2600558380265754e-08], ["'market for corrugated board box' (kilogram, RER, None)", 4.395968971178735e-09], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.7030085656476538e-09], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 7.368453535230518e-08], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 5.878987026143975e-08], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.904960099703577e-09], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 2.164226678597048e-09]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.04791118722555781], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.002985829534919112], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.005089126095588483], ["'market for corrugated board box' (kilogram, RER, None)", 0.00020399786499775133], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0019518319803824608], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.5740261101999055e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.02587204110180122], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.002581673747240563], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.00010648017094743199], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -9.72324535852973e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.00018553752254476212], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.005192258215602436], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.00027187662283107366]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.04791118722555781], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.002985829534919112], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.005089126095588483], ["'market for corrugated board box' (kilogram, RER, None)", 0.00020399786499775133], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0019518319803824608], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.5740261101999055e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.00023147863249441738], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -2.1137489909847236e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0004033424420833057], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.011287517859612484], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.00027187662283107366]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.13631070168398135], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00849489529653043], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.015348157755148117], ["'market for corrugated board box' (kilogram, RER, None)", 0.0006152316562314952], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0026024426405099475], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 7.762935889866213e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.07360777890934994], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0077860000323671736], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0003029435849490319], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -3.442391144155824e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0005278673209773634], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.014772340272958212], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0007735081382584998]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.13631070168398135], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00849489529653043], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.015348157755148117], ["'market for corrugated board box' (kilogram, RER, None)", 0.0006152316562314952], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0026024426405099475], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.00036504651852057256], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0006585730107587649], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -6.374798415103376e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0011475376526563395], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.032113783204439944], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0007735081382584998]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.00609930794777992], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0017382487207744984], ["'market for polysulfone' (kilogram, GLO, None)", 0.0004331310817870554], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0039036639607649215], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.0012840456470791324], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.00022546720665815237], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.00019556570070000507], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.005794342550390923], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.6488607208151193e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.036981209464168e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -5.803973342666852e-05], ["'market for corrugated board box' (kilogram, RER, None)", 7.199669448380936e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -8.514144226614146e-05]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.00609930794777992], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0017382487207744984], ["'market for polysulfone' (kilogram, GLO, None)", 0.0004331310817870554], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0039036639607649215], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.00022546720665815237], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.00019556570070000507], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.005794342550390923], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.6488607208151193e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.00035473033269068174], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.002001643635136486], ["'market for corrugated board box' (kilogram, RER, None)", 7.199669448380936e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -8.514144226614146e-05], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.000672543007716674], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.007599942363230531], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -3.156606890866001e-05], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", -2.322725349258902e-05]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.003644507298267878], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0010386522869981264], ["'market for polysulfone' (kilogram, GLO, None)", 0.0002165655408935277], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0026024426405099475], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.0006420228235395662], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.00013472296975672516], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.00011685598261216989], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0034622819333544838], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 8.244303604075597e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.18490604732084e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.901986671333426e-05], ["'market for corrugated board box' (kilogram, RER, None)", 4.302004112975829e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -5.087439603161276e-05]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.003644507298267878], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0010386522869981264], ["'market for polysulfone' (kilogram, GLO, None)", 0.0002165655408935277], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0026024426405099475], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.00013472296975672516], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.00011685598261216989], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0034622819333544838], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 8.244303604075597e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.00035473033269068174], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.002001643635136486], ["'market for corrugated board box' (kilogram, RER, None)", 4.302004112975829e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -5.087439603161276e-05], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.000672543007716674], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.007599942363230531], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -3.156606890866001e-05], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", -2.322725349258902e-05]]</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
modified:   Brighway/Libaries/__pycache__/LCA_plots.cpython-311.pyc 	modified:   Brighway/Libaries/__pycache__/box_plot.cpython-311.pyc 	modified:   Brighway/Libaries/__pycache__/life_cycle_assessment.cpython-311.pyc 	modified:   Brighway/Libaries/box_plot.py 	modified:   Brighway/Ofir/Ofir.ipynb 	modified:   Brighway/Results/Ananas - APOS_recipe.xlsx 	modified:   Brighway/Results/Ananas - CONSQ_recipe.xlsx 	modified:   Brighway/Results_Ofir/GWP_life_stage_pr_scenario_APOS.jpg 	modified:   Brighway/Results_Ofir/scaled_impact_score_multi_APOS_ReCiPe 2016 v1.03, endpoint (H).jpg 	modified:   Brighway/Results_Ofir/scaled_impact_score_multi_APOS_ReCiPe 2016 v1.03, midpoint (H).jpg
</commit_message>
<xml_diff>
--- a/Brighway/Results/Ananas - APOS_recipe.xlsx
+++ b/Brighway/Results/Ananas - APOS_recipe.xlsx
@@ -79,508 +79,508 @@
     <t>('ReCiPe 2016 v1.03, endpoint (H)', 'total: natural resources', 'natural resources')</t>
   </si>
   <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.00032945166331691244], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00015801064853070173], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 4.6389205711862454e-05], ["'market for corrugated board box' (kilogram, RER, None)", 2.013778491028875e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0004622626384260705], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.1147787062239849e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.00017790389819113272], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -1.8781572123565963e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.66507922162909e-06], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 6.815256059071447e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.3860842943139076e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -8.303594843869356e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.0142047379371389e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.00032945166331691244], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00015801064853070173], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 4.6389205711862454e-05], ["'market for corrugated board box' (kilogram, RER, None)", 2.013778491028875e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0004622626384260705], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.1147787062239849e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.2315389612237151e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.4815774041459668e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.1871397929925744e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0001805129313821823], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.0142047379371389e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0009373131829579762], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.0004495514225803063], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0001399039509001107], ["'market for corrugated board box' (kilogram, RER, None)", 6.073300209944417e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000616350184568094], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 3.362031019620352e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0005061491187973072], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -5.664283541570399e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.6117549334775722e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.4128545807312035e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.78857789405792e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00023624312087142089], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.8854839025352327e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0009373131829579762], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.0004495514225803063], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0001399039509001107], ["'market for corrugated board box' (kilogram, RER, None)", 6.073300209944417e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000616350184568094], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 3.3620310201579298e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.5038150727773306e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 4.468249223576303e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.00014757778009440384], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.000513572001932085], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.8854839025352327e-05]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0006799317205210687], ["'alubox production - CONSQ' (kilogram, GLO, None)", 5.9310919264254154e-05], ["'market for polysulfone' (kilogram, GLO, None)", 4.019118309206293e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000924525276852141], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.00016623361404338074], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.495551281007104e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 5.907099145686869e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0006459351344950152], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 9.505013037587547e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.3335979393624514e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -9.281865639367464e-07], ["'market for corrugated board box' (kilogram, RER, None)", 7.107201576755263e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.176104412433239e-06]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0006799317205210687], ["'alubox production - CONSQ' (kilogram, GLO, None)", 5.9310919264254154e-05], ["'market for polysulfone' (kilogram, GLO, None)", 4.019118309206293e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000924525276852141], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.495551281007104e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 5.907099145686869e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0006459351344950152], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 9.505013037587547e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -4.561969266059266e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -3.201080739405175e-05], ["'market for corrugated board box' (kilogram, RER, None)", 7.107201576755263e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.176104412433239e-06], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.000406571962381337], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.927619458904985e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.2125415379144803e-06], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 1.6280211335475744e-06]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.00040627824320049955], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.543993514940177e-05], ["'market for polysulfone' (kilogram, GLO, None)", 2.0095591546031464e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000616350184568094], ["'cabinet washer - CONSQ' (unit, GLO, None)", 8.311680702169037e-05], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.4911617735488555e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 3.529657156576897e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0003859643310404746], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 4.752506518793773e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.667989696812257e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -4.640932819683732e-07], ["'market for corrugated board box' (kilogram, RER, None)", 4.246751970234578e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.8978113291855574e-06]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.00040627824320049955], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.543993514940177e-05], ["'market for polysulfone' (kilogram, GLO, None)", 2.0095591546031464e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000616350184568094], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.4911617735488555e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 3.529657156576897e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0003859643310404746], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 4.752506518793773e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -4.561969266059266e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -3.201080739405175e-05], ["'market for corrugated board box' (kilogram, RER, None)", 4.246751970234578e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.8978113291855574e-06], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.000406571962381337], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.927619458904985e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.2125415379144803e-06], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 1.6280211335475744e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.1542416527930872], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.04709841261544819], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.02063117391319887], ["'market for corrugated board box' (kilogram, RER, None)", 0.009064392528043634], ["'autoclave - CONSQ' (unit, GLO, None)", 0.3136194154086757], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.00022704880868272586], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.08329049250826709], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.008701529761054663], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.08382272141506765], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.010168445776458772], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0023423681624823384], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.10075442332658927], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.006893154355111719]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.1542416527930872], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.04709841261544819], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.02063117391319887], ["'market for corrugated board box' (kilogram, RER, None)", 0.009064392528043634], ["'autoclave - CONSQ' (unit, GLO, None)", 0.3136194154086757], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.00022704880868272586], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.18222330742406012], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.022105316905345156], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.005092104723376794], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.21903135505018034], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.006893154355111719]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.4388283642845579], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.1339983006805709], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.06222099943016971], ["'market for corrugated board box' (kilogram, RER, None)", 0.02733705682567877], ["'autoclave - CONSQ' (unit, GLO, None)", 0.41815922054490096], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.000684750375565388], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.23696731671366128], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.026242708271574065], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.23848154543441785], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0360000868022972], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.006664202419615243], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.28665342969915536], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.01961150957529672]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.4388283642845579], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.1339983006805709], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.06222099943016971], ["'market for corrugated board box' (kilogram, RER, None)", 0.02733705682567877], ["'autoclave - CONSQ' (unit, GLO, None)", 0.41815922054490096], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.0006847503756748774], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.5184381422487344], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.06666682741166148], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.014487396543647602], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.6231596298265071], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.01961150957529672]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.15652274511716874], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.02506742788826223], ["'market for polysulfone' (kilogram, GLO, None)", 0.0021337009725469172], ["'autoclave - CONSQ' (unit, GLO, None)", 0.6272388308173514], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.16276703443760637], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.0017058255370440256], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0050526572112086264], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.14869660786131028], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 0.000757439926670406], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.00013091647106343603], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0011262459663236265], ["'market for corrugated board box' (kilogram, RER, None)", 0.0031990839685017074], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0021586743922518232]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.15652274511716874], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.02506742788826223], ["'market for polysulfone' (kilogram, GLO, None)", 0.0021337009725469172], ["'autoclave - CONSQ' (unit, GLO, None)", 0.6272388308173514], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.0017058255370440256], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0050526572112086264], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.14869660786131028], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 0.000757439926670406], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.004478388124218693], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.038841375330197256], ["'market for corrugated board box' (kilogram, RER, None)", 0.0031990839685017074], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0021586743922518232], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.010868049153376982], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.030809952373161937], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.033011391591809644], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 0.0018118957594268734]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.09352672332802628], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.01497849012867581], ["'market for polysulfone' (kilogram, GLO, None)", 0.0010668504862734586], ["'autoclave - CONSQ' (unit, GLO, None)", 0.41815922054490096], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.08138351721880319], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.0010192785267698358], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0030191041737117597], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.08885038716162497], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 0.000378719963335203], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.545823553171801e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0005631229831618132], ["'market for corrugated board box' (kilogram, RER, None)", 0.0019115422574496515], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0012898684002959776]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.09352672332802628], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.01497849012867581], ["'market for polysulfone' (kilogram, GLO, None)", 0.0010668504862734586], ["'autoclave - CONSQ' (unit, GLO, None)", 0.41815922054490096], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.0010192785267698358], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0030191041737117597], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.08885038716162497], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 0.000378719963335203], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.004478388124218693], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.038841375330197256], ["'market for corrugated board box' (kilogram, RER, None)", 0.0019115422574496515], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0012898684002959776], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.010868049153376982], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.030809952373161937], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.033011391591809644], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 0.0018118957594268734]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.002575880061279917], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.002681386540153435], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0004757341683104748], ["'market for corrugated board box' (kilogram, RER, None)", 0.0001428264265713875], ["'autoclave - CONSQ' (unit, GLO, None)", 0.008117449325061815], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 4.499571160094361e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0013909752330911553], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.00014971537875144706], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.004375708434223258], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0005306180005877085], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.001108343554986862], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.002244252344669314], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.00012908718849570378]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.002575880061279917], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.002681386540153435], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0004757341683104748], ["'market for corrugated board box' (kilogram, RER, None)", 0.0001428264265713875], ["'autoclave - CONSQ' (unit, GLO, None)", 0.008117449325061815], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 4.499571160094361e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.009512409639615778], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.001153517392581975], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0024094425214061035], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.004878809444763506], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.00012908718849570378]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.007328560174345679], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.007628733536774561], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0014347538118721001], ["'market for corrugated board box' (kilogram, RER, None)", 0.00043074636577255046], ["'autoclave - CONSQ' (unit, GLO, None)", 0.010823265766749086], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.3570135248158271e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.003957422494146667], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0004515225616910651], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.012449198643846453], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0018785854298641296], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0031533154861022395], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.006385055965478946], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.000367262141947291]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.007328560174345679], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.007628733536774561], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0014347538118721001], ["'market for corrugated board box' (kilogram, RER, None)", 0.00043074636577255046], ["'autoclave - CONSQ' (unit, GLO, None)", 0.010823265766749086], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.3570135250328094e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.02706347531270968], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0034788619071557956], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.006855033655629201], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.013880556447712073], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.000367262141947291]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0037239953774620004], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0014142961560177963], ["'market for polysulfone' (kilogram, GLO, None)", 5.2525211287247595e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.01623489865012363], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.006926399749254169], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.632351514481635e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.001537849262441289], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0035377956085889], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 3.7775049817998695e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.194603788971084e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.508654277542893e-05], ["'market for corrugated board box' (kilogram, RER, None)", 5.0407540285717045e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.0425209391520094e-05]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0037239953774620004], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0014142961560177963], ["'market for polysulfone' (kilogram, GLO, None)", 5.2525211287247595e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.01623489865012363], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.632351514481635e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.001537849262441289], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0035377956085889], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 3.7775049817998695e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.002119048872721739], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0008651714215307485], ["'market for corrugated board box' (kilogram, RER, None)", 5.0407540285717045e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.0425209391520094e-05], ["'production of wet wipe - CONSQ' (unit, GLO, None)", -0.00301221424263572], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.000710446585812281], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0017226269371093741], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 2.354023179482034e-05]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0022251915214112454], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0008450815578831715], ["'market for polysulfone' (kilogram, GLO, None)", 2.6262605643623798e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.010823265766749086], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.0034631998746270844], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.767959750059128e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0009189079988399667], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0021139319453406832], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.8887524908999347e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -3.097301894485542e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.2543271387714466e-05], ["'market for corrugated board box' (kilogram, RER, None)", 3.0119916919646303e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.4155194667907616e-05]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0022251915214112454], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0008450815578831715], ["'market for polysulfone' (kilogram, GLO, None)", 2.6262605643623798e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.010823265766749086], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.767959750059128e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0009189079988399667], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0021139319453406832], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.8887524908999347e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.002119048872721739], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0008651714215307485], ["'market for corrugated board box' (kilogram, RER, None)", 3.0119916919646303e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.4155194667907616e-05], ["'production of wet wipe - CONSQ' (unit, GLO, None)", -0.00301221424263572], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.000710446585812281], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0017226269371093741], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 2.354023179482034e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0034951468413655707], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.003493197791441804], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0006326924433916711], ["'market for corrugated board box' (kilogram, RER, None)", 0.00020000116535978177], ["'autoclave - CONSQ' (unit, GLO, None)", 0.009204020002652483], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 6.396241821226289e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0018873792943374082], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.00020290888734322889], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.006334986637136535], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0007682661196503023], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0013683607828049085], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0028768610170369943], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.00016294154332445007]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0034951468413655707], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.003493197791441804], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0006326924433916711], ["'market for corrugated board box' (kilogram, RER, None)", 0.00020000116535978177], ["'autoclave - CONSQ' (unit, GLO, None)", 0.009204020002652483], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 6.396241821226289e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.013771710080731598], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0016701437383702224], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.002974697366967384], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.006254045688993213], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.00016294154332445007]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.009943938900786552], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.0099383937164964], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0019081200287183278], ["'market for corrugated board box' (kilogram, RER, None)", 0.0006031781176429667], ["'autoclave - CONSQ' (unit, GLO, None)", 0.012272026670203311], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.929025311650959e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.005369727006424739], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0006119474256228533], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.01802348310847296], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0027199483188183843], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.003893082814962413], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.008184872187976932], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0004635801655524203]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.009943938900786552], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.0099383937164964], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0019081200287183278], ["'market for corrugated board box' (kilogram, RER, None)", 0.0006031781176429667], ["'autoclave - CONSQ' (unit, GLO, None)", 0.012272026670203311], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.929025311959404e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.039181485018419476], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.005036941331145155], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.008463223498675876], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.01779320040995137], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0004635801655524203]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.005214791760272705], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0018439750484988964], ["'market for polysulfone' (kilogram, GLO, None)", 6.729644141243289e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.018408040005304965], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.008443231015985712], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 7.828661645115836e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0021159771037727914], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.004954052172259069], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 5.029642135612412e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -7.647856886706219e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -3.215792427900825e-05], ["'market for corrugated board box' (kilogram, RER, None)", 7.058614460976231e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -5.102710876445776e-05]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.005214791760272705], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0018439750484988964], ["'market for polysulfone' (kilogram, GLO, None)", 6.729644141243289e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.018408040005304965], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 7.828661645115836e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0021159771037727914], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.004954052172259069], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 5.029642135612412e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0026161774128904904], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0011090454874953188], ["'market for corrugated board box' (kilogram, RER, None)", 7.058614460976231e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -5.102710876445776e-05], ["'production of wet wipe - CONSQ' (unit, GLO, None)", -0.000575151872486603], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0009448431839007462], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0024941406268017227], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 3.126067645767488e-05]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.003115984107045915], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0011018267284773244], ["'market for polysulfone' (kilogram, GLO, None)", 3.3648220706216446e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.012272026670203311], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.004221615507992856], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.6778445596733054e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0012643555734015094], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0029601849016936193], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 2.514821067806206e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -3.8239284433531094e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.6078962139504127e-05], ["'market for corrugated board box' (kilogram, RER, None)", 4.2177198079363444e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.0490126435919597e-05]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.003115984107045915], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0011018267284773244], ["'market for polysulfone' (kilogram, GLO, None)", 3.3648220706216446e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.012272026670203311], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.6778445596733054e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0012643555734015094], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0029601849016936193], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 2.514821067806206e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0026161774128904904], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0011090454874953188], ["'market for corrugated board box' (kilogram, RER, None)", 4.2177198079363444e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.0490126435919597e-05], ["'production of wet wipe - CONSQ' (unit, GLO, None)", -0.000575151872486603], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0009448431839007462], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0024941406268017227], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 3.126067645767488e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.4246843526982598], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.26410464946150747], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.05097297854386099], ["'market for corrugated board box' (kilogram, RER, None)", 0.014805773880272764], ["'autoclave - CONSQ' (unit, GLO, None)", 1.1292716339098199], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.0008182394338512325], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.22932955045706033], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.024969496910015338], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.24355136923318338], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.02954250996483097], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.06945763472986953], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.22575725177525385], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.023218345690887605]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.4246843526982598], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.26410464946150747], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.05097297854386099], ["'market for corrugated board box' (kilogram, RER, None)", 0.014805773880272764], ["'autoclave - CONSQ' (unit, GLO, None)", 1.1292716339098199], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.0008182394338512325], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.5294594983330074], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.06422284774963255], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.1509948587705053], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.49077663427695084], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.023218345690887605]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.2082568907753308], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.7513963266369649], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.1537280274149883], ["'market for corrugated board box' (kilogram, RER, None)", 0.0446523339165811], ["'autoclave - CONSQ' (unit, GLO, None)", 1.50569551187976], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.0024677062296987484], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.6524587210186786], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.07530483042536665], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.6929207969732823], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.10459149278780218], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.19761186343013165], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.6422952795934875], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.06605782859072676]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.2082568907753308], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.7513963266369649], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.1537280274149883], ["'market for corrugated board box' (kilogram, RER, None)", 0.0446523339165811], ["'autoclave - CONSQ' (unit, GLO, None)", 1.50569551187976], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.002467706230093327], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.5063495586375701], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.19368794960704105], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.429591006842007], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.3962940861752748], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.06605782859072676]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.13224599475672763], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.06762232827194302], ["'market for polysulfone' (kilogram, GLO, None)", 0.008388737139565776], ["'autoclave - CONSQ' (unit, GLO, None)", 2.2585432678196398], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.4854281992055989], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.032035708103587614], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.47366216002384215], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.12563369501889124], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 0.0003957376479410388], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0038820321130095775], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0025235437391768374], ["'market for corrugated board box' (kilogram, RER, None)", 0.005225382033611543], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.007271104880482139]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.13224599475672763], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.06762232827194302], ["'market for polysulfone' (kilogram, GLO, None)", 0.008388737139565776], ["'autoclave - CONSQ' (unit, GLO, None)", 2.2585432678196398], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.032035708103587614], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.47366216002384215], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.12563369501889124], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 0.0003957376479410388], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.13279647985862383], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.087030642032392], ["'market for corrugated board box' (kilogram, RER, None)", 0.005225382033611543], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.007271104880482139], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.02761327726609024], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.07612145813233852], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.09590840001446192], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", -0.0014486263719564294]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.07902068516363756], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0404062347766303], ["'market for polysulfone' (kilogram, GLO, None)", 0.004194368569782888], ["'autoclave - CONSQ' (unit, GLO, None)", 1.50569551187976], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.24271409960279944], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.019142232690710696], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.2830264046183406], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.07506965090545568], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 0.0001978688239705194], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0019410160565047887], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0012617718695884187], ["'market for corrugated board box' (kilogram, RER, None)", 0.0031223120952479397], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.004344688784114543]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.07902068516363756], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0404062347766303], ["'market for polysulfone' (kilogram, GLO, None)", 0.004194368569782888], ["'autoclave - CONSQ' (unit, GLO, None)", 1.50569551187976], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.019142232690710696], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.2830264046183406], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.07506965090545568], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 0.0001978688239705194], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.13279647985862383], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.087030642032392], ["'market for corrugated board box' (kilogram, RER, None)", 0.0031223120952479397], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.004344688784114543], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.02761327726609024], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.07612145813233852], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.09590840001446192], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", -0.0014486263719564294]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.11757236403331361], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.011546059896976347], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.013085324881130274], ["'market for corrugated board box' (kilogram, RER, None)", 0.0010078044055488917], ["'autoclave - CONSQ' (unit, GLO, None)", 0.011794864263106601], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 6.275383538786159e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.06348907657798936], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.006385849014992495], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0003101352144363789], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.690670946455437e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0005584739167065958], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.015215451300440504], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0008178808066219231]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.11757236403331361], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.011546059896976347], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.013085324881130274], ["'market for corrugated board box' (kilogram, RER, None)", 0.0010078044055488917], ["'autoclave - CONSQ' (unit, GLO, None)", 0.011794864263106601], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 6.275383538786159e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0006742069879051715], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 8.023197709685732e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0012140737372944197], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.03307706804328478], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0008178808066219231]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.33450165541872323], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.03284935350970735], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.03946367741350463], ["'market for corrugated board box' (kilogram, RER, None)", 0.0030394101114248266], ["'autoclave - CONSQ' (unit, GLO, None)", 0.015726485684142134], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.00018925759883661535], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.18063089392611056], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.019258909337621453], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0008823565255795569], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.00013066350291084805], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0015888976321569858], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.04328903045332324], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0023269284922689485]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.33450165541872323], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.03284935350970735], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.03946367741350463], ["'market for corrugated board box' (kilogram, RER, None)", 0.0030394101114248266], ["'autoclave - CONSQ' (unit, GLO, None)", 0.015726485684142134], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.00018925759886687704], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0019181663599555584], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.00024196944983490376], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.00345412528235449], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.09410658794891366], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0023269284922689485]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.033832419440732626], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.006149296159342674], ["'market for polysulfone' (kilogram, GLO, None)", 0.0011275973997964702], ["'autoclave - CONSQ' (unit, GLO, None)", 0.023589728526213202], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.004343848313710668], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.000535042693546586], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.000971249625905885], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.032140798468696], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 4.876235116799861e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -3.1213468287034964e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00017008028121374185], ["'market for corrugated board box' (kilogram, RER, None)", 0.0003556830650484527], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.00025612923521141666]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.033832419440732626], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.006149296159342674], ["'market for polysulfone' (kilogram, GLO, None)", 0.0011275973997964702], ["'autoclave - CONSQ' (unit, GLO, None)", 0.023589728526213202], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.000535042693546586], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.000971249625905885], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.032140798468696], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 4.876235116799861e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0010677497228335797], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00586563880042361], ["'market for corrugated board box' (kilogram, RER, None)", 0.0003556830650484527], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.00025612923521141666], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.002322671898890378], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.019541216513959615], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.00011981593502914338], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", -3.41135056606014e-05]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.02021581802812413], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0036743766545010107], ["'market for polysulfone' (kilogram, GLO, None)", 0.0005637986998982351], ["'autoclave - CONSQ' (unit, GLO, None)", 0.015726485684142134], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.002171924156855334], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.000319702992242784], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0005803488494694493], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.019205027126717927], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 2.4381175583999304e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.5606734143517482e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -8.504014060687093e-05], ["'market for corrugated board box' (kilogram, RER, None)", 0.00021253059181743317], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.00015304439061166296]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.02021581802812413], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0036743766545010107], ["'market for polysulfone' (kilogram, GLO, None)", 0.0005637986998982351], ["'autoclave - CONSQ' (unit, GLO, None)", 0.015726485684142134], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.000319702992242784], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0005803488494694493], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.019205027126717927], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 2.4381175583999304e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0010677497228335797], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00586563880042361], ["'market for corrugated board box' (kilogram, RER, None)", 0.00021253059181743317], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.00015304439061166296], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.002322671898890378], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.019541216513959615], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.00011981593502914338], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", -3.41135056606014e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.6107683632415326e-05], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 2.1979795666106068e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 4.66479725541961e-06], ["'market for corrugated board box' (kilogram, RER, None)", 6.970377403646815e-06], ["'autoclave - CONSQ' (unit, GLO, None)", -2.297772908378533e-05], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.5474719020016852e-08], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -8.698149161504277e-06], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -1.0066393616264027e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.40526299876735e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.573026213528871e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -9.130485265809544e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -8.73795938304418e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.590766710592349e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.6107683632415326e-05], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 2.1979795666106068e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 4.66479725541961e-06], ["'market for corrugated board box' (kilogram, RER, None)", 6.970377403646815e-06], ["'autoclave - CONSQ' (unit, GLO, None)", -2.297772908378533e-05], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.5474719020016852e-08], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.054919562537718e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.419622203323633e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.9848881099664267e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.8995563875521945e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.590766710592349e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 4.5827494278139374e-05], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 6.253406654300599e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.4068435882149842e-05], ["'market for corrugated board box' (kilogram, RER, None)", 2.1021773118319107e-05], ["'autoclave - CONSQ' (unit, GLO, None)", -3.0636972111713774e-05], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 7.682851769883089e-08], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -2.4746846910195263e-05], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -3.035896425945613e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.998072193676123e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.569098904026384e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.5976873736272905e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.486010978994426e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.525843317828836e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 4.5827494278139374e-05], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 6.253406654300599e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.4068435882149842e-05], ["'market for corrugated board box' (kilogram, RER, None)", 2.1021773118319107e-05], ["'autoclave - CONSQ' (unit, GLO, None)", -3.0636972111713774e-05], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 7.682851771111553e-08], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 8.691461290600267e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.0313146118567377e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.647146456325348e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -5.404371693862777e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.525843317828836e-06]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 5.11835150644143e-05], ["'alubox production - CONSQ' (kilogram, GLO, None)", 1.2403929145125681e-05], ["'market for polysulfone' (kilogram, GLO, None)", 1.9126691235872395e-07], ["'autoclave - CONSQ' (unit, GLO, None)", -4.595545816757066e-05], ["'cabinet washer - CONSQ' (unit, GLO, None)", 3.457256187858905e-06], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.673248658294235e-07], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 2.9829706100578206e-06], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -4.862433931119358e-05], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 3.6405520745686866e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.1030872483757e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -9.767403935362618e-08], ["'market for corrugated board box' (kilogram, RER, None)", 2.4600460027988033e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.981677741853955e-07]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 5.11835150644143e-05], ["'alubox production - CONSQ' (kilogram, GLO, None)", 1.2403929145125681e-05], ["'market for polysulfone' (kilogram, GLO, None)", 1.9126691235872395e-07], ["'autoclave - CONSQ' (unit, GLO, None)", -4.595545816757066e-05], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.673248658294235e-07], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 2.9829706100578206e-06], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -4.862433931119358e-05], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 3.6405520745686866e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.7456631044464828e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -3.3685306194122313e-06], ["'market for corrugated board box' (kilogram, RER, None)", 2.4600460027988033e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.981677741853955e-07], ["'production of wet wipe - CONSQ' (unit, GLO, None)", -5.585643992490576e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.9662628929703256e-06], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.1067572626686445e-08], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 4.105538325255076e-08]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 3.0583583547566214e-05], ["'alubox production - CONSQ' (kilogram, GLO, None)", 7.411695012556751e-06], ["'market for polysulfone' (kilogram, GLO, None)", 9.563345617936197e-08], ["'autoclave - CONSQ' (unit, GLO, None)", -3.0636972111713774e-05], ["'cabinet washer - CONSQ' (unit, GLO, None)", 1.7286280939294524e-06], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 9.998129294635685e-08], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.7824084719039972e-06], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -2.90544043701879e-05], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.8202760372843433e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.55154362418785e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -4.883701967681309e-08], ["'market for corrugated board box' (kilogram, RER, None)", 1.4699463771257078e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.976691956294648e-07]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 3.0583583547566214e-05], ["'alubox production - CONSQ' (kilogram, GLO, None)", 7.411695012556751e-06], ["'market for polysulfone' (kilogram, GLO, None)", 9.563345617936197e-08], ["'autoclave - CONSQ' (unit, GLO, None)", -3.0636972111713774e-05], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 9.998129294635685e-08], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.7824084719039972e-06], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -2.90544043701879e-05], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.8202760372843433e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.7456631044464828e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -3.3685306194122313e-06], ["'market for corrugated board box' (kilogram, RER, None)", 1.4699463771257078e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.976691956294648e-07], ["'production of wet wipe - CONSQ' (unit, GLO, None)", -5.585643992490576e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.9662628929703256e-06], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.1067572626686445e-08], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 4.105538325255076e-08]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.889600857085989e-06], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 2.610063690232733e-06], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.497219433011155e-07], ["'market for corrugated board box' (kilogram, RER, None)", 4.0183387331173233e-07], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00013286553723601384], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 5.416698624596908e-09], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -1.0203844628264341e-06], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -1.1181151213323185e-07], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.3082978885587858e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.5813325777144055e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -9.75466626663982e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -7.69691715696436e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 7.777152232684407e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.889600857085989e-06], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 2.610063690232733e-06], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.497219433011155e-07], ["'market for corrugated board box' (kilogram, RER, None)", 4.0183387331173233e-07], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00013286553723601384], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 5.416698624596908e-09], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.8441258446930124e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.437679516770447e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.1205796324810419e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.6732428601514137e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 7.777152232684407e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 5.376047508892532e-06], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 7.425815006014254e-06], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.9594788369286424e-06], ["'market for corrugated board box' (kilogram, RER, None)", 1.2118799351660813e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00017715404964801845], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.633607522116651e-08], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -2.9030656548019673e-06], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -3.3720931547561873e-07], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.7221996266038696e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.5985065281869045e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.7752712651195124e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.18982713443991e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.2126545790567683e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 5.376047508892532e-06], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 7.425815006014254e-06], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.9594788369286424e-06], ["'market for corrugated board box' (kilogram, RER, None)", 1.2118799351660813e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00017715404964801845], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.6336075223778596e-08], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 8.091738318704064e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.03676046818276e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.033198393799426e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -4.760493770870923e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.2126545790567683e-05]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 3.692348298539384e-06], ["'alubox production - CONSQ' (kilogram, GLO, None)", 2.0619203610568115e-06], ["'market for polysulfone' (kilogram, GLO, None)", 8.462756924699476e-08], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0002657310744720277], ["'cabinet washer - CONSQ' (unit, GLO, None)", 1.1320412288153831e-05], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.5525177438659536e-08], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 6.292610430619047e-08], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -3.5077308836124148e-06], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 6.849922026495211e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.4519460453930945e-09], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -8.603713479714355e-09], ["'market for corrugated board box' (kilogram, RER, None)", 1.4181869310440799e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.435508985358827e-06]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 3.692348298539384e-06], ["'alubox production - CONSQ' (kilogram, GLO, None)", 2.0619203610568115e-06], ["'market for polysulfone' (kilogram, GLO, None)", 8.462756924699476e-08], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0002657310744720277], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.5525177438659536e-08], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 6.292610430619047e-08], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -3.5077308836124148e-06], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 6.849922026495211e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.865000654634105e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.967203208637608e-07], ["'market for corrugated board box' (kilogram, RER, None)", 1.4181869310440799e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.435508985358827e-06], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.00012707952535413478], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 9.70274508524164e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.1337234920080076e-08], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 4.5676381986026424e-07]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 2.2062815055389833e-06], ["'alubox production - CONSQ' (kilogram, GLO, None)", 1.2320551558728802e-06], ["'market for polysulfone' (kilogram, GLO, None)", 4.231378462349738e-08], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00017715404964801845], ["'cabinet washer - CONSQ' (unit, GLO, None)", 5.6602061440769155e-06], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.7202568365239955e-08], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 3.76001094483108e-08], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -2.095967430262034e-06], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 3.4249610132476057e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.7259730226965472e-09], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -4.3018567398571776e-09], ["'market for corrugated board box' (kilogram, RER, None)", 8.474064058166177e-08], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.4552848220774163e-06]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 2.2062815055389833e-06], ["'alubox production - CONSQ' (kilogram, GLO, None)", 1.2320551558728802e-06], ["'market for polysulfone' (kilogram, GLO, None)", 4.231378462349738e-08], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00017715404964801845], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.7202568365239955e-08], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 3.76001094483108e-08], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -2.095967430262034e-06], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 3.4249610132476057e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.865000654634105e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.967203208637608e-07], ["'market for corrugated board box' (kilogram, RER, None)", 8.474064058166177e-08], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.4552848220774163e-06], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.00012707952535413478], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 9.70274508524164e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.1337234920080076e-08], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 4.5676381986026424e-07]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.003517252466384169], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.0017785803198210638], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0005449558282524257], ["'market for corrugated board box' (kilogram, RER, None)", 0.00027532070921551684], ["'autoclave - CONSQ' (unit, GLO, None)", 0.001364620512139065], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.6041536632474646e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0018993163318474513], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0002603292224294203], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.00019388848660040697], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.3571724145239736e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0003403221579004145], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.000851953695479976], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -7.659206092784872e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.003517252466384169], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.0017785803198210638], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0005449558282524257], ["'market for corrugated board box' (kilogram, RER, None)", 0.00027532070921551684], ["'autoclave - CONSQ' (unit, GLO, None)", 0.001364620512139065], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.6041536632474646e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.00042149671000088474], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.124287857660812e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0007398307812884433], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0018520732509789732], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -7.659206092784872e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.010006830960698621], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.005060186262026125], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0016435175439759764], ["'market for corrugated board box' (kilogram, RER, None)", 0.0008303322974843852], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00181949401618542], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 7.85379676415959e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.005403688718777256], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0007851198612636768], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0005516263984969325], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 8.345268627709203e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0009682405116559995], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.002423868259982945], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.00021790980716459963]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.010006830960698621], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.005060186262026125], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0016435175439759764], ["'market for corrugated board box' (kilogram, RER, None)", 0.0008303322974843852], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00181949401618542], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 7.853796765415388e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0011991878228194185], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.00015454201162424448], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.002104870674500697], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.005269278826436599], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.00021790980716459963]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.03049272720877801], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.001165474968186897], ["'market for polysulfone' (kilogram, GLO, None)", 4.904841909964629e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00272924102427813], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.002007297634397571], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.2365670834025218e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.00047576668126590743], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.028968090848339106], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 6.736656759332428e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.9020825440950147e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -9.523248521989348e-06], ["'market for corrugated board box' (kilogram, RER, None)", 9.716857079202168e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.3985727296550403e-05]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.03049272720877801], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.001165474968186897], ["'market for polysulfone' (kilogram, GLO, None)", 4.904841909964629e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00272924102427813], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.2365670834025218e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.00047576668126590743], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.028968090848339106], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 6.736656759332428e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0006506640308560747], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00032843275915364747], ["'market for corrugated board box' (kilogram, RER, None)", 9.716857079202168e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.3985727296550403e-05], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.0003744621018078424], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.000813820056220492], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 7.652451843270921e-05], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 2.640739817933754e-06]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.018220258397829116], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0006964039303920935], ["'market for polysulfone' (kilogram, GLO, None)", 2.4524209549823146e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00181949401618542], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.0010036488171987854], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.3364114631223246e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0002842839149935723], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.017309245477937663], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 3.368328379666214e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -9.510412720475074e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -4.761624260994674e-06], ["'market for corrugated board box' (kilogram, RER, None)", 5.806094213023414e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.4332143749416316e-05]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.018220258397829116], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0006964039303920935], ["'market for polysulfone' (kilogram, GLO, None)", 2.4524209549823146e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00181949401618542], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.3364114631223246e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0002842839149935723], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.017309245477937663], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 3.368328379666214e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0006506640308560747], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00032843275915364747], ["'market for corrugated board box' (kilogram, RER, None)", 5.806094213023414e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.4332143749416316e-05], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.0003744621018078424], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.000813820056220492], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 7.652451843270921e-05], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 2.640739817933754e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.05867514610319985], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.04857522255953673], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.010937123796594487], ["'market for corrugated board box' (kilogram, RER, None)", 0.005092068621364678], ["'autoclave - CONSQ' (unit, GLO, None)", 0.030221729446096055], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 8.820584758614293e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.03168457889572792], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.003461367295099731], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.05279006118834249], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.006401953712917623], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.011034994882025827], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.033846953585926466], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.007571224971604384]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.05867514610319985], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.04857522255953673], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.010937123796594487], ["'market for corrugated board box' (kilogram, RER, None)", 0.005092068621364678], ["'autoclave - CONSQ' (unit, GLO, None)", 0.030221729446096055], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 8.820584758614293e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.11476100258335324], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.013917290680255701], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.023989119413941037], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0735803338798882], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.007571224971604384]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.16693492271614604], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.13819992897220307], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.03298497586122507], ["'market for corrugated board box' (kilogram, RER, None)", 0.01535703234737849], ["'autoclave - CONSQ' (unit, GLO, None)", 0.04029563926146141], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.00026601763564448053], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.09014485826671886], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.010439044011849703], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.15019144169077725], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.022665301505849826], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.03139533774882958], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.09629696652448094], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.021540668230827467]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.16693492271614604], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.13819992897220307], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.03298497586122507], ["'market for corrugated board box' (kilogram, RER, None)", 0.01535703234737849], ["'autoclave - CONSQ' (unit, GLO, None)", 0.04029563926146141], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 0.00026601763568701595], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.3265031341103853], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.04197278056638856], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.06825073413891031], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.20934123159032242], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.021540668230827467]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.13032565584744885], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.02856025811114962], ["'market for polysulfone' (kilogram, GLO, None)", 0.0014311051476188273], ["'autoclave - CONSQ' (unit, GLO, None)", 0.06044345889219211], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.062405983766129255], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.00140736120379972], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.043111645823239425], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.1238093730550764], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 0.0007369206162690872], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0006167529986519748], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0003783456218584972], ["'market for corrugated board box' (kilogram, RER, None)", 0.0017971369887965557], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0023710203808304294]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.13032565584744885], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.02856025811114962], ["'market for polysulfone' (kilogram, GLO, None)", 0.0014311051476188273], ["'autoclave - CONSQ' (unit, GLO, None)", 0.06044345889219211], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.00140736120379972], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.043111645823239425], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.1238093730550764], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 0.0007369206162690872], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.021097874715862962], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.013048183738329177], ["'market for corrugated board box' (kilogram, RER, None)", 0.0017971369887965557], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0023710203808304294], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.03006852054364752], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.016333159939913692], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.020783648319100637], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 0.00045464490567682323]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0778732288899202], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.017065553996890095], ["'market for polysulfone' (kilogram, GLO, None)", 0.0007155525738094137], ["'autoclave - CONSQ' (unit, GLO, None)", 0.04029563926146141], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.031202991883064628], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.000840937729732779], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.025760415638683427], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.07397956744542418], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 0.0003684603081345436], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0003083764993259874], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0001891728109292486], ["'market for corrugated board box' (kilogram, RER, None)", 0.0010738396773371857], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0014167510749505082]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0778732288899202], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.017065553996890095], ["'market for polysulfone' (kilogram, GLO, None)", 0.0007155525738094137], ["'autoclave - CONSQ' (unit, GLO, None)", 0.04029563926146141], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.000840937729732779], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.025760415638683427], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.07397956744542418], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 0.0003684603081345436], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.021097874715862962], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.013048183738329177], ["'market for corrugated board box' (kilogram, RER, None)", 0.0010738396773371857], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0014167510749505082], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.03006852054364752], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.016333159939913692], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.020783648319100637], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 0.00045464490567682323]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.002255350308311721], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.004441772806237658], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0009261542488092973], ["'market for corrugated board box' (kilogram, RER, None)", -9.542395253881106e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.001106686692725594], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 3.5998554509729677e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0012178891664883292], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0001548050699876318], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.921512688146157e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 9.581866602559197e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.669764553239924e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0034524003173216104], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0001837103101131711]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.002255350308311721], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.004441772806237658], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0009261542488092973], ["'market for corrugated board box' (kilogram, RER, None)", -9.542395253881106e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.001106686692725594], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 3.5998554509729677e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.2872853669882952e-06], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.0830144788172169e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.2325575169785046e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0075052180808727505], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0001837103101131711]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.006416630454633346], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.012637156434647984], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0027931635509381237], ["'market for corrugated board box' (kilogram, RER, None)", -0.00028778652347785823], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0014755822569674588], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.0856706918376308e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.003464980445502007], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0004668724238384532], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.6847120605711605e-06], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.392337796782687e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.61308795344571e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00982232202795531], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0005226687696603586]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.006416630454633346], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.012637156434647984], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0027931635509381237], ["'market for corrugated board box' (kilogram, RER, None)", -0.00028778652347785823], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0014755822569674588], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.0856706920112262e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.662417522980783e-06], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 6.282107031079051e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -3.5067129372547175e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.02135287397538301], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0005226687696603586]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0008274258581216459], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0018752795072104864], ["'market for polysulfone' (kilogram, GLO, None)", 0.00011308662079259678], ["'autoclave - CONSQ' (unit, GLO, None)", 0.002213373385451188], ["'cabinet washer - CONSQ' (unit, GLO, None)", 8.559651273248125e-05], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 7.260377921681201e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.00018725643970961882], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0007860545652155636], ["'plastic incineration - CONSQ' (kilogram, CH, None)", -7.254875744731232e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -3.1688680667692706e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -3.85913769653005e-05], ["'market for corrugated board box' (kilogram, RER, None)", -3.367784833164815e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -5.7531098478864144e-05]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0008274258581216459], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0018752795072104864], ["'market for polysulfone' (kilogram, GLO, None)", 0.00011308662079259678], ["'autoclave - CONSQ' (unit, GLO, None)", 0.002213373385451188], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 7.260377921681201e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.00018725643970961882], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0007860545652155636], ["'plastic incineration - CONSQ' (kilogram, CH, None)", -7.254875744731232e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.0840057788113499e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0013309190017446375], ["'market for corrugated board box' (kilogram, RER, None)", -3.367784833164815e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -5.7531098478864144e-05], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.0003322238773375482], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0013830899015281333], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.1107089279058106e-07], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", -2.364164646650264e-06]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0004944101207084536], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.001120532019179074], ["'market for polysulfone' (kilogram, GLO, None)", 5.654331039629839e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0014755822569674588], ["'cabinet washer - CONSQ' (unit, GLO, None)", 4.279825636624063e-05], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.33827912122086e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.00011189096648543079], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0004696896146730309], ["'plastic incineration - CONSQ' (kilogram, CH, None)", -3.627437872365616e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.5844340333846353e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.929568848265025e-05], ["'market for corrugated board box' (kilogram, RER, None)", -2.0123457483385945e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.4376442426221206e-05]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0004944101207084536], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.001120532019179074], ["'market for polysulfone' (kilogram, GLO, None)", 5.654331039629839e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0014755822569674588], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.33827912122086e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.00011189096648543079], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0004696896146730309], ["'plastic incineration - CONSQ' (kilogram, CH, None)", -3.627437872365616e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.0840057788113499e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0013309190017446375], ["'market for corrugated board box' (kilogram, RER, None)", -2.0123457483385945e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.4376442426221206e-05], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.0003322238773375482], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0013830899015281333], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.1107089279058106e-07], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", -2.364164646650264e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0017000890525980025], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.002503989405533837], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0008158651922520887], ["'market for corrugated board box' (kilogram, RER, None)", 0.005106828816268815], ["'autoclave - CONSQ' (unit, GLO, None)", 0.16825543378483399], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 7.892479440964108e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0009180480884029214], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -9.774151212120025e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.890777616975627e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -2.317893248869346e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.011166114867022986], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.016528115476612544], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.006324265221133046]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0017000890525980025], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.002503989405533837], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0008158651922520887], ["'market for corrugated board box' (kilogram, RER, None)", 0.005106828816268815], ["'autoclave - CONSQ' (unit, GLO, None)", 0.16825543378483399], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 7.892479440964108e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -4.110386123860059e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -5.038898367107273e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.024274162860836918], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.03593068581747251], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.006324265221133046]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0048368730792224856], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.007124026196025846], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.002460545768059087], ["'market for corrugated board box' (kilogram, RER, None)", 0.015401547220890875], ["'autoclave - CONSQ' (unit, GLO, None)", 0.22434057837977864], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.3802715780351274e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0026119114627801425], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0002947759829655848], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -5.3793954736489674e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -8.20620574591048e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.03176838334229084], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.04702365247506063], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.017992979926380392]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0048368730792224856], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.007124026196025846], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.002460545768059087], ["'market for corrugated board box' (kilogram, RER, None)", 0.015401547220890875], ["'autoclave - CONSQ' (unit, GLO, None)", 0.22434057837977864], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.3802715784157254e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -0.00011694337986193407], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -1.5196677307241627e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.06906170281918723], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.10222533147502556], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.017992979926380392]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0015002092875017413], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0029475230312975362], ["'market for polysulfone' (kilogram, GLO, None)", -2.4624839406446756e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.33651086756966797], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.069985841831298], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 6.877537770762638e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0010375830249309001], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0014251988231266542], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.1170202915333108e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0006240813793893255], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00018475341103514135], ["'market for corrugated board box' (kilogram, RER, None)", 0.001802346284702894], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0019805199012473667]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0015002092875017413], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0029475230312975362], ["'market for polysulfone' (kilogram, GLO, None)", -2.4624839406446756e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.33651086756966797], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 6.877537770762638e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0010375830249309001], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0014251988231266542], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.1170202915333108e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.02134856382317935], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0063716779425854915], ["'market for corrugated board box' (kilogram, RER, None)", 0.001802346284702894], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0019805199012473667], ["'production of wet wipe - CONSQ' (unit, GLO, None)", -0.010429304020692188], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0012183876604387558], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -7.5249338383240476e-06], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", -0.0004015194186031602]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0008964170597779814], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0017612275509529892], ["'market for polysulfone' (kilogram, GLO, None)", -1.2312419703223378e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.22434057837977864], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.034992920915649], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.109521410339819e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0006199849129270385], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0008515962067890824], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 5.585101457666554e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.00031204068969466274], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -9.237670551757067e-05], ["'market for corrugated board box' (kilogram, RER, None)", 0.0010769523775209166], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0011834161029313202]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0008964170597779814], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0017612275509529892], ["'market for polysulfone' (kilogram, GLO, None)", -1.2312419703223378e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.22434057837977864], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.109521410339819e-05], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.0006199849129270385], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0008515962067890824], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 5.585101457666554e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.02134856382317935], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0063716779425854915], ["'market for corrugated board box' (kilogram, RER, None)", 0.0010769523775209166], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0011834161029313202], ["'production of wet wipe - CONSQ' (unit, GLO, None)", -0.010429304020692188], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0012183876604387558], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", -7.5249338383240476e-06], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", -0.0004015194186031602]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.00015443045132739234], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 7.391801978784976e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 2.2017600119227295e-05], ["'market for corrugated board box' (kilogram, RER, None)", 1.064265430836516e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0006835164091632984], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 3.864587460542977e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -8.339244371679187e-05], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -6.646838932200662e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 8.698552676877363e-06], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 9.480740327022601e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.9432037467552094e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -5.371829091195071e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.238972508580597e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.00015443045132739234], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 7.391801978784976e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 2.2017600119227295e-05], ["'market for corrugated board box' (kilogram, RER, None)", 1.064265430836516e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0006835164091632984], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 3.864587460542977e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.8909897123646443e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.0610305058744784e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.398269042740835e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0001167788932827854], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.238972508580597e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0004393655094103275], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00021030197179078383], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.640228472872845e-05], ["'market for corrugated board box' (kilogram, RER, None)", 3.209689394007594e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0009113552122177312], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.1655105042678095e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.00023725737508157685], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -2.0046021770399717e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.4747994939848278e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.356535327286918e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -8.373621979971138e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0001528323205977195], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.2060175307085602e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0004393655094103275], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00021030197179078383], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.640228472872845e-05], ["'market for corrugated board box' (kilogram, RER, None)", 3.209689394007594e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0009113552122177312], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.165510504454171e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.379998899967016e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 6.21580616164244e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0001820352601736389], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0003322441752368176], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.2060175307085602e-05]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.001909903381614274], ["'alubox production - CONSQ' (kilogram, GLO, None)", 5.383540016672161e-05], ["'market for polysulfone' (kilogram, GLO, None)", 2.2951165960977628e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0013670328183265968], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.0001925900372458725], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 7.255637685124479e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", -0.00018516774676524117], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.00181440821253356], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 8.908884162993076e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.6449756033976153e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -6.004699988334661e-07], ["'market for corrugated board box' (kilogram, RER, None)", 3.7560977941833362e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.3274853473934867e-06]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.001909903381614274], ["'alubox production - CONSQ' (kilogram, GLO, None)", 5.383540016672161e-05], ["'market for polysulfone' (kilogram, GLO, None)", 2.2951165960977628e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0013670328183265968], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 7.255637685124479e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", -0.00018516774676524117], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.00181440821253356], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 8.908884162993076e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.627129380317419e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.0708691792563442e-05], ["'market for corrugated board box' (kilogram, RER, None)", 3.7560977941833362e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.3274853473934867e-06], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 2.90697019629001e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 3.288039807617217e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.077878747607377e-06], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 8.483230911981653e-07]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.001141220753710808], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.216815915717201e-05], ["'market for polysulfone' (kilogram, GLO, None)", 1.1475582980488814e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0009113552122177312], ["'cabinet washer - CONSQ' (unit, GLO, None)", 9.629501862293625e-05], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.335446697136949e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", -0.00011064291396130866], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0010841597160252676], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 4.454442081496538e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -8.224878016988077e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -3.002349994167331e-07], ["'market for corrugated board box' (kilogram, RER, None)", 2.2443736167567994e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -7.93209669603121e-07]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.001141220753710808], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.216815915717201e-05], ["'market for polysulfone' (kilogram, GLO, None)", 1.1475582980488814e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0009113552122177312], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.335446697136949e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", -0.00011064291396130866], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0010841597160252676], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 4.454442081496538e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.627129380317419e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.0708691792563442e-05], ["'market for corrugated board box' (kilogram, RER, None)", 2.2443736167567994e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -7.93209669603121e-07], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 2.90697019629001e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 3.288039807617217e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.077878747607377e-06], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 8.483230911981653e-07]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.1390439608595256e-08], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 1.5366018306686846e-08], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 3.0761387717593778e-09], ["'market for corrugated board box' (kilogram, RER, None)", 1.2242259622376303e-09], ["'autoclave - CONSQ' (unit, GLO, None)", -1.944112734983769e-07], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 6.943037542027535e-11], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -6.150837388641439e-09], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -1.2857762786126436e-09], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 6.5080690789901095e-09], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 7.893176660960214e-10], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.0720967482449381e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.6761919027072856e-08], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -9.475535564947016e-10]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.1390439608595256e-08], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 1.5366018306686846e-08], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 3.0761387717593778e-09], ["'market for corrugated board box' (kilogram, RER, None)", 1.2242259622376303e-09], ["'autoclave - CONSQ' (unit, GLO, None)", -1.944112734983769e-07], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 6.943037542027535e-11], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.4147976258674152e-08], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.7159079697739596e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.330645115099883e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -5.81780848394381e-08], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -9.475535564947016e-10]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 3.2406602830087913e-08], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 4.371740419648934e-08], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 9.27724372689787e-09], ["'market for corrugated board box' (kilogram, RER, None)", 3.6921100441779405e-09], ["'autoclave - CONSQ' (unit, GLO, None)", -2.592150313311692e-07], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.0939319576485633e-10], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -1.7499565528247473e-08], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -3.877737904564959e-09], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.8515914844450735e-08], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.794478637023258e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -3.050190767681859e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -7.613954426174581e-08], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.6958565975708696e-09]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 3.2406602830087913e-08], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 4.371740419648934e-08], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 9.27724372689787e-09], ["'market for corrugated board box' (kilogram, RER, None)", 3.6921100441779405e-09], ["'autoclave - CONSQ' (unit, GLO, None)", -2.592150313311692e-07], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.0939319579833765e-10], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 4.02519887922842e-08], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.1749604389319584e-09], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.630849485470951e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.6552074840724738e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.6958565975708696e-09]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 2.9426490598608053e-08], ["'alubox production - CONSQ' (kilogram, GLO, None)", 6.159776879286204e-09], ["'market for polysulfone' (kilogram, GLO, None)", 8.608425911461889e-10], ["'autoclave - CONSQ' (unit, GLO, None)", -3.888225469967538e-07], ["'cabinet washer - CONSQ' (unit, GLO, None)", 3.865988162882121e-08], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 7.510652856842942e-10], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 2.8252359290012935e-09], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -2.7955166068677648e-08], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 3.2674656970296917e-10], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.992018042546741e-10], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.9914818982807066e-10], ["'market for corrugated board box' (kilogram, RER, None)", 4.320644364750669e-10], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.967378202078723e-10]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 2.9426490598608053e-08], ["'alubox production - CONSQ' (kilogram, GLO, None)", 6.159776879286204e-09], ["'market for polysulfone' (kilogram, GLO, None)", 8.608425911461889e-10], ["'autoclave - CONSQ' (unit, GLO, None)", -3.888225469967538e-07], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 7.510652856842942e-10], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 2.8252359290012935e-09], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -2.7955166068677648e-08], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 3.2674656970296917e-10], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.04974837954826e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.0316864581890436e-08], ["'market for corrugated board box' (kilogram, RER, None)", 4.320644364750669e-10], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.967378202078723e-10], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 1.7828518486191989e-07], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 4.593809806940272e-09], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.562483504229626e-09], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 2.304408595474606e-08]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 1.7583152165332816e-08], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.6806391781598138e-09], ["'market for polysulfone' (kilogram, GLO, None)", 4.3042129557309444e-10], ["'autoclave - CONSQ' (unit, GLO, None)", -2.592150313311692e-07], ["'cabinet washer - CONSQ' (unit, GLO, None)", 1.9329940814410604e-08], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.487825403451534e-10], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.6881575829142531e-09], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -1.6703994557066173e-08], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.6337328485148458e-10], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.9960090212733706e-10], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.4957409491403533e-10], ["'market for corrugated board box' (kilogram, RER, None)", 2.5817060020780766e-10], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.773091573387197e-10]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 1.7583152165332816e-08], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.6806391781598138e-09], ["'market for polysulfone' (kilogram, GLO, None)", 4.3042129557309444e-10], ["'autoclave - CONSQ' (unit, GLO, None)", -2.592150313311692e-07], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.487825403451534e-10], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.6881575829142531e-09], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -1.6703994557066173e-08], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.6337328485148458e-10], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.04974837954826e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.0316864581890436e-08], ["'market for corrugated board box' (kilogram, RER, None)", 2.5817060020780766e-10], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.773091573387197e-10], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 1.7828518486191989e-07], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 4.593809806940272e-09], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.562483504229626e-09], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 2.304408595474606e-08]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.00014168997134467824], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00011137929805245783], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 2.4109122727607444e-05], ["'market for corrugated board box' (kilogram, RER, None)", 1.6328052074237104e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0002012539542205681], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 4.449414831409708e-07], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -7.651258452612626e-05], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -8.30383797456183e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.996131450780361e-06], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.3431747788794499e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -8.414208566166241e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -5.0787150428346334e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -8.888003634907142e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.00014168997134467824], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00011137929805245783], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 2.4109122727607444e-05], ["'market for corrugated board box' (kilogram, RER, None)", 1.6328052074237104e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0002012539542205681], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 4.449414831409708e-07], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 4.339416197348611e-06], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.093858214955326e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.829175783274234e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00011040684875343242], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -8.888003634907142e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0004031179466426057], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00031688194657178144], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 7.27100511976521e-05], ["'market for corrugated board box' (kilogram, RER, None)", 4.9243331643582276e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0002683386056274241], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.3418870129864744e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.00021768369118700708], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -2.5043320368352365e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.679134550107507e-06], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 8.295711782021299e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.3939016070969654e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.000144493019504886], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.5286996259120968e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0004031179466426057], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00031688194657178144], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 7.27100511976521e-05], ["'market for corrugated board box' (kilogram, RER, None)", 4.9243331643582276e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0002683386056274241], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.341887013201038e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.2345944674146753e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.5362429225965368e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.204133921023868e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0003141152598162838], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.5286996259120968e-05]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0003070959975220654], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.269211273872963e-05], ["'market for polysulfone' (kilogram, GLO, None)", 1.8956198489533308e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0004025079084411362], ["'cabinet washer - CONSQ' (unit, GLO, None)", 6.212970614681401e-05], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.411296257488632e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.9268351301255548e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0002917411976459621], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 3.50440480181107e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -4.702755569845327e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -5.677053316616167e-07], ["'market for corrugated board box' (kilogram, RER, None)", 5.762637646808395e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.7833854947245283e-06]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0003070959975220654], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.269211273872963e-05], ["'market for polysulfone' (kilogram, GLO, None)", 1.8956198489533308e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0004025079084411362], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.411296257488632e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.9268351301255548e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0002917411976459621], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 3.50440480181107e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.6087177208506912e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.9578721277024118e-05], ["'market for corrugated board box' (kilogram, RER, None)", 5.762637646808395e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.7833854947245283e-06], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 4.867140766356924e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 3.600381277970284e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 7.607009162867332e-07], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 5.476801820179796e-07]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.00018349845815629013], ["'alubox production - CONSQ' (kilogram, GLO, None)", 1.9534452841566142e-05], ["'market for polysulfone' (kilogram, GLO, None)", 9.478099244766654e-07], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0002683386056274241], ["'cabinet washer - CONSQ' (unit, GLO, None)", 3.1064853073407005e-05], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 8.432890345055666e-07], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.1513379475875757e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.00017432353524847563], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.752202400905535e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.3513777849226634e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.8385266583080837e-07], ["'market for corrugated board box' (kilogram, RER, None)", 3.443337369291871e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.6631507782617617e-06]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.00018349845815629013], ["'alubox production - CONSQ' (kilogram, GLO, None)", 1.9534452841566142e-05], ["'market for polysulfone' (kilogram, GLO, None)", 9.478099244766654e-07], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0002683386056274241], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 8.432890345055666e-07], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.1513379475875757e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.00017432353524847563], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.752202400905535e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.6087177208506912e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.9578721277024118e-05], ["'market for corrugated board box' (kilogram, RER, None)", 3.443337369291871e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.6631507782617617e-06], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 4.867140766356924e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 3.600381277970284e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 7.607009162867332e-07], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 5.476801820179796e-07]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0002935749893174448], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.0001387753076477897], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 4.3243948373555644e-05], ["'market for corrugated board box' (kilogram, RER, None)", 1.1226053340561828e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00037007040312632286], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.3446821182988132e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0001585304942314202], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -1.7558362767586567e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.3645575151839235e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.6487555901412544e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.7860216268534373e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00011080807991803284], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.326310774277151e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0002935749893174448], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.0001387753076477897], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 4.3243948373555644e-05], ["'market for corrugated board box' (kilogram, RER, None)", 1.1226053340561828e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.00037007040312632286], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.3446821182988132e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.966429380834616e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.5842512829157703e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.0565687805864964e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00024088713024821013], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.326310774277151e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0008352415189031528], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.000394825523166951], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00013041825435768927], ["'market for corrugated board box' (kilogram, RER, None)", 3.385635133844707e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0004934272041684305], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 7.07126353316432e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0004510304202077025], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -5.2953791400972424e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.882262226297923e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.837209113930959e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -7.926427776879018e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00031525679070111627], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.7734475552932816e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0008352415189031528], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.000394825523166951], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00013041825435768927], ["'market for corrugated board box' (kilogram, RER, None)", 3.385635133844707e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0004934272041684305], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 7.071263534294993e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 8.439700491952006e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.0809646507279553e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.00017231364707685353], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0006853408494005509], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.7734475552932816e-05]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.00040270113347142325], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.55134149702434e-05], ["'market for polysulfone' (kilogram, GLO, None)", 3.841999494362337e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0007401408062526457], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.00017398150328724294], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 3.092243820393865e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.7908722229360266e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0003825660767978521], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 2.012315978333832e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.5571255003207255e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.238627039124905e-06], ["'market for corrugated board box' (kilogram, RER, None)", 3.961996036714828e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.15350209367736e-06]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.00040270113347142325], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.55134149702434e-05], ["'market for polysulfone' (kilogram, GLO, None)", 3.841999494362337e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0007401408062526457], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 3.092243820393865e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.7908722229360266e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0003825660767978521], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 2.012315978333832e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.3266119166742874e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -4.2717114342105416e-05], ["'market for corrugated board box' (kilogram, RER, None)", 3.961996036714828e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.15350209367736e-06], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.0007846475745748834], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.457916526816494e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.352609201235566e-06], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 4.816899922592571e-06]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.00024062520412525756], ["'alubox production - CONSQ' (kilogram, GLO, None)", 2.1220259930075914e-05], ["'market for polysulfone' (kilogram, GLO, None)", 1.9209997471811684e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0004934272041684305], ["'cabinet washer - CONSQ' (unit, GLO, None)", 8.699075164362147e-05], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.8477022750673254e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.0700963031603065e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0002285939439189947], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.006157989166916e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -7.785627501603627e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -6.193135195624525e-07], ["'market for corrugated board box' (kilogram, RER, None)", 2.3674035825872675e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.481833814505466e-06]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.00024062520412525756], ["'alubox production - CONSQ' (kilogram, GLO, None)", 2.1220259930075914e-05], ["'market for polysulfone' (kilogram, GLO, None)", 1.9209997471811684e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0004934272041684305], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.8477022750673254e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.0700963031603065e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0002285939439189947], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.006157989166916e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.3266119166742874e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -4.2717114342105416e-05], ["'market for corrugated board box' (kilogram, RER, None)", 2.3674035825872675e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.481833814505466e-06], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.0007846475745748834], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.457916526816494e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.352609201235566e-06], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 4.816899922592571e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.000317642348754344], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00014298353781804255], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 4.8239456800970866e-05], ["'market for corrugated board box' (kilogram, RER, None)", 1.1597092085675906e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0003776406112181805], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.395849469652867e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0001715268683273458], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -1.910963649336365e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.379367762451718e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.6658765754626403e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.8471995327673646e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0001171029226109728], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.3605872382790101e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.000317642348754344], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00014298353781804255], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 4.8239456800970866e-05], ["'market for corrugated board box' (kilogram, RER, None)", 1.1597092085675906e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0003776406112181805], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.395849469652867e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.998625570547213e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.6214708162231313e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.189564228808637e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0002545715708845599], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.3605872382790101e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0009037148513855984], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.0004067982343555577], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00014548407311930413], ["'market for corrugated board box' (kilogram, RER, None)", 3.497535707747824e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000503520814957574], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 7.2255777674457005e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0004880060197482232], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -5.763223587600363e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.924398422749959e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.8978237812322e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -8.100483228600373e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0003331660614583805], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.870966509222013e-05]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0009037148513855984], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.0004067982343555577], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00014548407311930413], ["'market for corrugated board box' (kilogram, RER, None)", 3.497535707747824e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000503520814957574], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 7.2255777686010475e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 8.531300919021649e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.0921895891170739e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.00017609746123929397], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0007242740467018087], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.870966509222013e-05]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0004126359538879128], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.816335531480803e-05], ["'market for polysulfone' (kilogram, GLO, None)", 3.88155116343156e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000755281222436361], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.00017789009719927412], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 3.4545200183282885e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.8623214273884847e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0003920041561935171], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 2.0352750182351766e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.5913182274828571e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.3089916043468713e-06], ["'market for corrugated board box' (kilogram, RER, None)", 4.0929462462865255e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.2608429731730944e-06]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0004126359538879128], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.816335531480803e-05], ["'market for polysulfone' (kilogram, GLO, None)", 3.88155116343156e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000755281222436361], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 3.4545200183282885e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.8623214273884847e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0003920041561935171], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 2.0352750182351766e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.4435783319875614e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -4.514381025885438e-05], ["'market for corrugated board box' (kilogram, RER, None)", 4.0929462462865255e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.2608429731730944e-06], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.0012260816744973165], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 7.203930192233402e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.4081916927300264e-06], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 4.7009143857956334e-06]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.00024656153752978025], ["'alubox production - CONSQ' (kilogram, GLO, None)", 2.2803673492471236e-05], ["'market for polysulfone' (kilogram, GLO, None)", 1.94077558171578e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000503520814957574], ["'cabinet washer - CONSQ' (unit, GLO, None)", 8.894504859963706e-05], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.0641724481861174e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.1127892036191524e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.00023423346065329126], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.0176375091175883e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -7.956591137414286e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -6.544958021734357e-07], ["'market for corrugated board box' (kilogram, RER, None)", 2.4456499999001035e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.5459729959487106e-06]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.00024656153752978025], ["'alubox production - CONSQ' (kilogram, GLO, None)", 2.2803673492471236e-05], ["'market for polysulfone' (kilogram, GLO, None)", 1.94077558171578e-06], ["'autoclave - CONSQ' (unit, GLO, None)", 0.000503520814957574], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.0641724481861174e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.1127892036191524e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.00023423346065329126], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.0176375091175883e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.4435783319875614e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -4.514381025885438e-05], ["'market for corrugated board box' (kilogram, RER, None)", 2.4456499999001035e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.5459729959487106e-06], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.0012260816744973165], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 7.203930192233402e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.4081916927300264e-06], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 4.7009143857956334e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0011196636272355163], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00032141079905200864], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00032401647559544063], ["'market for corrugated board box' (kilogram, RER, None)", 3.806130102374293e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0005504119066706546], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 4.711286406182188e-07], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0006046183587071789], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -7.04324891423178e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 4.1055814094313594e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 4.348760124618535e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.4783938364494434e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00014662113252027055], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0002098095686832082]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0011196636272355163], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00032141079905200864], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00032401647559544063], ["'market for corrugated board box' (kilogram, RER, None)", 3.806130102374293e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0005504119066706546], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 4.711286406182188e-07], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 8.925176977024695e-05], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 9.45382635786638e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.387812711558447e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.00031874159242427835], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0002098095686832082]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0031855218690362576], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.000914436357866278], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0009771925256512753], ["'market for corrugated board box' (kilogram, RER, None)", 0.00011478805068582941], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0007338825422275394], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.420864154604482e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0017201818092795792], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.00021241543914212013], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.00011680668235283588], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.5396231185210454e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -7.051205043754697e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0004171474473837644], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0005969229982741224]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0031855218690362576], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.000914436357866278], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0009771925256512753], ["'market for corrugated board box' (kilogram, RER, None)", 0.00011478805068582941], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0007338825422275394], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.4208641548316735e-06], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0002539275703322519], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.8511539231871207e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.00015328706594920652], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.0009068422769877813], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0005969229982741224]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0008862513405582456], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0006035256209839753], ["'market for polysulfone' (kilogram, GLO, None)", 3.468695127676702e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0011008238133413091], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.00018270602189388239], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.4786413443271393e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.257875181621341e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0008419387735303332], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.1081310681762825e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.3851903392909875e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.6389499699034864e-06], ["'market for corrugated board box' (kilogram, RER, None)", 1.3432924219539876e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -6.57043959606068e-05]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0008862513405582456], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0006035256209839753], ["'market for polysulfone' (kilogram, GLO, None)", 3.468695127676702e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0011008238133413091], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.4786413443271393e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.257875181621341e-05], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0008419387735303332], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.1081310681762825e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -4.738456448507028e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -5.6523239888918186e-05], ["'market for corrugated board box' (kilogram, RER, None)", 1.3432924219539876e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -6.57043959606068e-05], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.010838951150681493], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00048387611016301375], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.4118049755940637e-05], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 3.718321589217504e-06]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0005295599937596006], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0003606234591202047], ["'market for polysulfone' (kilogram, GLO, None)", 1.734347563838351e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0007338825422275394], ["'cabinet washer - CONSQ' (unit, GLO, None)", 9.135301094694119e-05], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.4810576128520979e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 7.516156454106661e-06], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0005030819940716205], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 5.540655340881412e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.925951696454937e-07], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -8.194749849517432e-07], ["'market for corrugated board box' (kilogram, RER, None)", 8.026548393100001e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.9260216554343014e-05]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.0005295599937596006], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0003606234591202047], ["'market for polysulfone' (kilogram, GLO, None)", 1.734347563838351e-05], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0007338825422275394], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.4810576128520979e-06], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 7.516156454106661e-06], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0005030819940716205], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 5.540655340881412e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -4.738456448507028e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -5.6523239888918186e-05], ["'market for corrugated board box' (kilogram, RER, None)", 8.026548393100001e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -3.9260216554343014e-05], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.010838951150681493], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00048387611016301375], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.4118049755940637e-05], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 3.718321589217504e-06]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 5.757589568054192e-10], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 2.2601734744686658e-10], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 8.518376808030966e-11], ["'market for corrugated board box' (kilogram, RER, None)", 8.138664770554284e-11], ["'autoclave - CONSQ' (unit, GLO, None)", 2.5211332673493153e-09], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.2814611037247904e-12], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -3.109098366749264e-10], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -3.2772614457535437e-11], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.441007470333537e-10], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.960815268128032e-11], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.1661575532875856e-10], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -4.717017418144127e-10], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -8.071351980028816e-11]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 5.757589568054192e-10], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 2.2601734744686658e-10], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 8.518376808030966e-11], ["'market for corrugated board box' (kilogram, RER, None)", 8.138664770554284e-11], ["'autoclave - CONSQ' (unit, GLO, None)", 2.5211332673493153e-09], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.2814611037247904e-12], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.30653797898595e-10], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 6.436554930713113e-11], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.535125126958779e-10], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.0254385691260812e-09], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -8.071351980028816e-11]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.6380747785168264e-09], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 6.430352702009443e-10], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 2.5690342233961884e-10], ["'market for corrugated board box' (kilogram, RER, None)", 2.454517946232539e-10], ["'autoclave - CONSQ' (unit, GLO, None)", 3.3615110231324204e-09], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 3.864723964591084e-12], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -8.845603803990862e-10], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -9.883804159989819e-11], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 6.944838155033444e-10], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.0482389246244923e-10], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -3.31780038370903e-10], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.3420246736748824e-09], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.2963564790122821e-10]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.6380747785168264e-09], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 6.430352702009443e-10], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 2.5690342233961884e-10], ["'market for corrugated board box' (kilogram, RER, None)", 2.454517946232539e-10], ["'autoclave - CONSQ' (unit, GLO, None)", 3.3615110231324204e-09], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 3.864723965209041e-12], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.5097474250072704e-09], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.9411831937490595e-10], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -7.212609519480051e-10], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.9174449429855987e-09], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.2963564790122821e-10]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 6.880138454036532e-10], ["'alubox production - CONSQ' (kilogram, GLO, None)", 1.240919621881071e-10], ["'market for polysulfone' (kilogram, GLO, None)", 7.37809084738171e-12], ["'autoclave - CONSQ' (unit, GLO, None)", 5.0422665346986306e-09], ["'cabinet washer - CONSQ' (unit, GLO, None)", 1.14807229314759e-09], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 6.8801639197282534e-12], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 4.697413903335787e-11], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -6.536131531334705e-10], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 2.2066908919746314e-12], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.517729963448163e-12], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -5.272743036842063e-12], ["'market for corrugated board box' (kilogram, RER, None)", 2.872368105412271e-11], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.527641183200643e-11]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 6.880138454036532e-10], ["'alubox production - CONSQ' (kilogram, GLO, None)", 1.240919621881071e-10], ["'market for polysulfone' (kilogram, GLO, None)", 7.37809084738171e-12], ["'autoclave - CONSQ' (unit, GLO, None)", 5.0422665346986306e-09], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 6.8801639197282534e-12], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 4.697413903335787e-11], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -6.536131531334705e-10], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 2.2066908919746314e-12], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.2295838123399307e-10], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.8184357363977212e-10], ["'market for corrugated board box' (kilogram, RER, None)", 2.872368105412271e-11], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.527641183200643e-11], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 1.4282697117787904e-10], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.272107854144826e-10], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 9.612150607466991e-11], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 2.49490926141749e-12]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 4.1110753914231425e-10], ["'alubox production - CONSQ' (kilogram, GLO, None)", 7.414842236577893e-11], ["'market for polysulfone' (kilogram, GLO, None)", 3.689045423690855e-12], ["'autoclave - CONSQ' (unit, GLO, None)", 3.3615110231324204e-09], ["'cabinet washer - CONSQ' (unit, GLO, None)", 5.74036146573795e-10], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.111090607887061e-12], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 2.806836349347417e-11], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -3.9055216218519856e-10], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.1033454459873157e-12], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -3.2588649817240815e-12], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.6363715184210316e-12], ["'market for corrugated board box' (kilogram, RER, None)", 1.7163203799923082e-11], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.5103363903326964e-11]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 4.1110753914231425e-10], ["'alubox production - CONSQ' (kilogram, GLO, None)", 7.414842236577893e-11], ["'market for polysulfone' (kilogram, GLO, None)", 3.689045423690855e-12], ["'autoclave - CONSQ' (unit, GLO, None)", 3.3615110231324204e-09], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 4.111090607887061e-12], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 2.806836349347417e-11], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -3.9055216218519856e-10], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.1033454459873157e-12], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.2295838123399307e-10], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.8184357363977212e-10], ["'market for corrugated board box' (kilogram, RER, None)", 1.7163203799923082e-11], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.5103363903326964e-11], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 1.4282697117787904e-10], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.272107854144826e-10], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 9.612150607466991e-11], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 2.49490926141749e-12]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 2.5998969977386397e-07], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 1.315906263224426e-07], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 3.936728051402973e-08], ["'market for corrugated board box' (kilogram, RER, None)", 2.084536093333721e-08], ["'autoclave - CONSQ' (unit, GLO, None)", 4.303883193640819e-07], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 6.002837272676786e-10], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -1.4039443787788655e-07], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -1.5120211529131917e-08], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 9.183485854562929e-08], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.1133782181569887e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.1196882908300931e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.3644570721830188e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.4445082352527581e-08]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 2.5998969977386397e-07], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 1.315906263224426e-07], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 3.936728051402973e-08], ["'market for corrugated board box' (kilogram, RER, None)", 2.084536093333721e-08], ["'autoclave - CONSQ' (unit, GLO, None)", 4.303883193640819e-07], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 6.002837272676786e-10], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.9964099683832457e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.4203874307760626e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.434104990738661e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.9662110263815975e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -1.4445082352527581e-08]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 7.396890049904298e-07], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 3.7438459883286484e-07], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.1872671660548197e-07], ["'market for corrugated board box' (kilogram, RER, None)", 6.286696153365e-08], ["'autoclave - CONSQ' (unit, GLO, None)", 5.738510924854425e-07], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.8103794953917617e-09], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -3.994320626948321e-07], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -4.5600637021254796e-08], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.6127663980587493e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.941773735985571e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -3.185592058703976e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -3.88197645825155e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.109727655561152e-08]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 7.396890049904298e-07], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 3.7438459883286484e-07], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.1872671660548197e-07], ["'market for corrugated board box' (kilogram, RER, None)", 6.286696153365e-08], ["'autoclave - CONSQ' (unit, GLO, None)", 5.738510924854425e-07], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 1.8103794956812358e-09], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 5.679926952301628e-07], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 7.299580992565871e-08], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.925200117706473e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -8.439079257687942e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.109727655561152e-08]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 4.7148338047659613e-07], ["'alubox production - CONSQ' (kilogram, GLO, None)", 5.558141419749438e-08], ["'market for polysulfone' (kilogram, GLO, None)", 3.741766550065263e-09], ["'autoclave - CONSQ' (unit, GLO, None)", 8.607766387281638e-07], ["'cabinet washer - CONSQ' (unit, GLO, None)", 2.11584331074012e-07], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.8740620316219478e-09], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 2.823891033022743e-08], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -4.4790921145276626e-07], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 9.182376688278926e-10], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -6.258010251094816e-10], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -1.5252077507175098e-09], ["'market for corrugated board box' (kilogram, RER, None)", 7.356925439091028e-09], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.523651692964974e-09]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 4.7148338047659613e-07], ["'alubox production - CONSQ' (kilogram, GLO, None)", 5.558141419749438e-08], ["'market for polysulfone' (kilogram, GLO, None)", 3.741766550065263e-09], ["'autoclave - CONSQ' (unit, GLO, None)", 8.607766387281638e-07], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 2.8740620316219478e-09], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 2.823891033022743e-08], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -4.4790921145276626e-07], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 9.182376688278926e-10], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.1407389430900466e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -5.2600558380265754e-08], ["'market for corrugated board box' (kilogram, RER, None)", 7.356925439091028e-09], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -4.523651692964974e-09], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 7.368453535230518e-08], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 5.878987026143975e-08], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.6145311837588914e-08], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 2.164226678597048e-09]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 2.8172452282630134e-07], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.3211451434346776e-08], ["'market for polysulfone' (kilogram, GLO, None)", 1.8708832750326313e-09], ["'autoclave - CONSQ' (unit, GLO, None)", 5.738510924854425e-07], ["'cabinet washer - CONSQ' (unit, GLO, None)", 1.05792165537006e-07], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.7173325465118384e-09], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.687353969905826e-08], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -2.676382966849863e-07], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 4.591188344139463e-10], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -3.129005125547408e-10], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -7.626038753587549e-10], ["'market for corrugated board box' (kilogram, RER, None)", 4.395968971178735e-09], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.7030085656476538e-09]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 2.8172452282630134e-07], ["'alubox production - CONSQ' (kilogram, GLO, None)", 3.3211451434346776e-08], ["'market for polysulfone' (kilogram, GLO, None)", 1.8708832750326313e-09], ["'autoclave - CONSQ' (unit, GLO, None)", 5.738510924854425e-07], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 1.7173325465118384e-09], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 1.687353969905826e-08], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -2.676382966849863e-07], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 4.591188344139463e-10], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -2.1407389430900466e-08], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -5.2600558380265754e-08], ["'market for corrugated board box' (kilogram, RER, None)", 4.395968971178735e-09], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -2.7030085656476538e-09], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 7.368453535230518e-08], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 5.878987026143975e-08], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 3.6145311837588914e-08], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", 2.164226678597048e-09]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.04791118722555781], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.002985829534919112], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.005089126095588483], ["'market for corrugated board box' (kilogram, RER, None)", 0.00020399786499775133], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0019518319803824608], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.5740261101999055e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.02587204110180122], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.002581673747240563], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.00010648017094743199], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 1.2717493355269386e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.00018553752254476212], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.005192258215602436], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.00027187662283107366]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.04791118722555781], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.002985829534919112], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.005089126095588483], ["'market for corrugated board box' (kilogram, RER, None)", 0.00020399786499775133], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0019518319803824608], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 2.5740261101999055e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.00023147863249441738], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 2.7646724685368232e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0004033424420833057], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.011287517859612484], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.00027187662283107366]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.13631070168398135], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00849489529653043], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.015348157755148117], ["'market for corrugated board box' (kilogram, RER, None)", 0.0006152316562314952], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0026024426405099475], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 7.762935889866213e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.07360777890934994], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0077860000323671736], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0003029435849490319], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 4.502466500409254e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0005278673209773634], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.014772340272958212], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0007735081382584998]]</t>
-  </si>
-  <si>
-    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.13631070168398135], ["'sheet manufacturing - CONSQ' (kilogram, GLO, None)", 0.00849489529653043], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.015348157755148117], ["'market for corrugated board box' (kilogram, RER, None)", 0.0006152316562314952], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0026024426405099475], ["'transport Plastic - CONSQ' (ton kilometer, GLO, None)", 7.762935891107482e-05], ["'PP incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 0.0006585730107587649], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 8.337900926683803e-05], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.0011475376526563395], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.032113783204439944], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -0.0007735081382584998]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.00609930794777992], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0017382487207744984], ["'market for polysulfone' (kilogram, GLO, None)", 0.0004331310817870554], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0039036639607649215], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.0012840456470791324], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.00022546720665815237], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.00019556570070000507], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.005794342550390923], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.6488607208151193e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -1.036981209464168e-05], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -5.803973342666852e-05], ["'market for corrugated board box' (kilogram, RER, None)", 7.199669448380936e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -8.514144226614146e-05]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.00609930794777992], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0017382487207744984], ["'market for polysulfone' (kilogram, GLO, None)", 0.0004331310817870554], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0039036639607649215], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.00022546720665815237], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.00019556570070000507], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.005794342550390923], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 1.6488607208151193e-06], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.00035473033269068174], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.002001643635136486], ["'market for corrugated board box' (kilogram, RER, None)", 7.199669448380936e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -8.514144226614146e-05], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.000672543007716674], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.007599942363230531], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 4.128675733207683e-05], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", -2.322725349258902e-05]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.003644507298267878], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0010386522869981264], ["'market for polysulfone' (kilogram, GLO, None)", 0.0002165655408935277], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0026024426405099475], ["'cabinet washer - CONSQ' (unit, GLO, None)", 0.0006420228235395662], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.00013472296975672516], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.00011685598261216989], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0034622819333544838], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 8.244303604075597e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -5.18490604732084e-06], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -2.901986671333426e-05], ["'market for corrugated board box' (kilogram, RER, None)", 4.302004112975829e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -5.087439603161276e-05]]</t>
-  </si>
-  <si>
-    <t>[["'alubox raw materials - CONSQ' (kilogram, GLO, None)", 0.003644507298267878], ["'alubox production - CONSQ' (kilogram, GLO, None)", 0.0010386522869981264], ["'market for polysulfone' (kilogram, GLO, None)", 0.0002165655408935277], ["'autoclave - CONSQ' (unit, GLO, None)", 0.0026024426405099475], ["'transport Alu - CONSQ' (ton kilometer, GLO, None)", 0.00013472296975672516], ["'alubox EoL melting - CONSQ' (kilogram, GLO, None)", 0.00011685598261216989], ["'avoided alubox raw materials - CONSQ' (kilogram, GLO, None)", -0.0034622819333544838], ["'plastic incineration - CONSQ' (kilogram, CH, None)", 8.244303604075597e-07], ["'marginal electricity mix - CONSQ' (kilowatt hour, GLO, None)", -0.00035473033269068174], ["'marginal heating grid projection updated - CONSQ' (megajoule, GLO, None)", -0.002001643635136486], ["'market for corrugated board box' (kilogram, RER, None)", 4.302004112975829e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", -5.087439603161276e-05], ["'production of wet wipe - CONSQ' (unit, GLO, None)", 0.000672543007716674], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.007599942363230531], ["'PE incineration no Energy Recovery - CONSQ' (kilogram, CH, None)", 4.128675733207683e-05], ["'incineration of wet wipe - CONSQ' (kilogram, CH, None)", -2.322725349258902e-05]]</t>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.00044776822019924786], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.00020169124361394091], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.0439435721381354e-05], ["'market for corrugated board box' (kilogram, RER, None)", 8.278808770870672e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.001699141242943235], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 1.1147787062239849e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.00024179483890759387], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -5.786314428266833e-06], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 5.376232279255772e-06], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 6.471508634910819e-07], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -2.326769117870964e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0001283726845058098], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 6.191064121177316e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.00044776822019924786], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.00020169124361394091], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.0439435721381354e-05], ["'market for corrugated board box' (kilogram, RER, None)", 8.278808770870672e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.001699141242943235], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 1.1147787062239849e-06], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.1687461476642983e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.4068497032414825e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -5.058193756681633e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.00027907105326378773], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 6.191064121177316e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0012739321194401136], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.000573825791690367], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00018227765959425067], ["'market for corrugated board box' (kilogram, RER, None)", 2.4967835971139877e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.0022655216572576467], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 3.362031019620352e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0006879233444976614], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -1.74507891920606e-05], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.5295759442389663e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.9517247868649822e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -6.619822038892923e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0003652293276891479], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.76140134166163e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0012739321194401136], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.000573825791690367], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00018227765959425067], ["'market for corrugated board box' (kilogram, RER, None)", 2.4967835971139877e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.0022655216572576467], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 3.362031019620352e-06], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 3.325165096171666e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 4.242879971445614e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.00014390917455258894], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0007939767993825057], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.76140134166163e-05]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.0004896365811427861], ["'alubox production - APOS' (kilogram, GLO, None)", 6.612054933148283e-05], ["'market for polysulfone' (kilogram, GLO, None)", 7.94001955732489e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.00339828248588647], ["'cabinet washer - APOS' (unit, GLO, None)", 0.0005723265694732038], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 2.682371061413364e-06], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -4.9136106031342715e-05], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0004651547520856468], ["'plastic incineration - APOS' (kilogram, CH, None)", 8.578567644751003e-08], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.3004463037451628e-06], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -1.4349664594095203e-06], ["'market for corrugated board box' (kilogram, RER, None)", 2.921828940576546e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.938806370883582e-06]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.0004896365811427861], ["'alubox production - APOS' (kilogram, GLO, None)", 6.612054933148283e-05], ["'market for polysulfone' (kilogram, GLO, None)", 7.94001955732489e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.00339828248588647], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 2.682371061413364e-06], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -4.9136106031342715e-05], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0004651547520856468], ["'plastic incineration - APOS' (kilogram, CH, None)", 8.578567644751003e-08], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -4.4485642147002576e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -4.9488364445030745e-05], ["'market for corrugated board box' (kilogram, RER, None)", 2.921828940576546e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.938806370883582e-06], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.00018338041914667665], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 9.025837036084666e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 2.100945517469414e-06], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 2.796795156198302e-06]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.00029257156857006184], ["'alubox production - APOS' (kilogram, GLO, None)", 3.950887980525451e-05], ["'market for polysulfone' (kilogram, GLO, None)", 3.970009778662445e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.0022655216572576467], ["'cabinet washer - APOS' (unit, GLO, None)", 0.0002861632847366019], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 1.6027918238727194e-06], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -2.936019931652653e-05], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0002779429901415588], ["'plastic incineration - APOS' (kilogram, CH, None)", 4.2892838223755016e-08], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -6.502231518725814e-07], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -7.174832297047602e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.1584911004046972e-06], ["'market for corrugated board box' (kilogram, RER, None)", 1.7458746140906223e-06]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.00029257156857006184], ["'alubox production - APOS' (kilogram, GLO, None)", 3.950887980525451e-05], ["'market for polysulfone' (kilogram, GLO, None)", 3.970009778662445e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.0022655216572576467], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 1.6027918238727194e-06], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -2.936019931652653e-05], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0002779429901415588], ["'plastic incineration - APOS' (kilogram, CH, None)", 4.2892838223755016e-08], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -4.4485642147002576e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -4.9488364445030745e-05], ["'market for corrugated board box' (kilogram, RER, None)", 1.7458746140906223e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.1584911004046972e-06], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.00018338041914667665], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 9.025837036084666e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 2.100945517469414e-06], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 2.796795156198302e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.17080706158518175], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.05584503651893412], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.022502500104376023], ["'market for corrugated board box' (kilogram, RER, None)", 0.004246803666530992], ["'autoclave - APOS' (unit, GLO, None)", 1.3239735387996632], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 0.00022704880868272586], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.09223581325599814], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0022685172575133443], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.08332804089748311], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.010108844417752633], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.014187000144314751], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.14768299577910418], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.003662370801342493]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.17080706158518175], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.05584503651893412], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.022502500104376023], ["'market for corrugated board box' (kilogram, RER, None)", 0.004246803666530992], ["'autoclave - APOS' (unit, GLO, None)", 1.3239735387996632], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 0.00022704880868272586], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.1811479149945285], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.021975748734244856], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.030841304796789013], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.3210499908129668], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.003662370801342493]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.48595811887615087], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.15888306164541818], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0678646814797115], ["'market for corrugated board box' (kilogram, RER, None)", 0.012807820579292088], ["'autoclave - APOS' (unit, GLO, None)", 1.7652980517328842], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 0.000684750375565388], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.26241738419312144], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.006841559844385156], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.23707414452523368], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.03048699048357433], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.04036301474855665], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.4201685231337544], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.010419702844105446]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.48595811887615087], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.15888306164541818], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0678646814797115], ["'market for corrugated board box' (kilogram, RER, None)", 0.012807820579292088], ["'autoclave - APOS' (unit, GLO, None)", 1.7652980517328842], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 0.000684750375565388], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.5153785750548557], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.06627606626863984], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.08774568411041717], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.9134098329665025], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.010419702844105446]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.10942935516731966], ["'alubox production - APOS' (kilogram, GLO, None)", 0.022058003180153652], ["'market for polysulfone' (kilogram, GLO, None)", 0.0026526193575519097], ["'autoclave - APOS' (unit, GLO, None)", 2.6479470775993263], ["'cabinet washer - APOS' (unit, GLO, None)", 0.47885036908640016], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 0.0016686511101938139], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.0042922430874401405], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.10395788740895366], ["'plastic incineration - APOS' (kilogram, CH, None)", 0.000749633601018745], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0007929206106959067], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0016508196146551829], ["'market for corrugated board box' (kilogram, RER, None)", 0.0014988187553596386], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.0011469155710877297]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.10942935516731966], ["'alubox production - APOS' (kilogram, GLO, None)", 0.022058003180153652], ["'market for polysulfone' (kilogram, GLO, None)", 0.0026526193575519097], ["'autoclave - APOS' (unit, GLO, None)", 2.6479470775993263], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 0.0016686511101938139], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.0042922430874401405], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.10395788740895366], ["'plastic incineration - APOS' (kilogram, CH, None)", 0.000749633601018745], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.02712421300042628], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.05693259392047285], ["'market for corrugated board box' (kilogram, RER, None)", 0.0014988187553596386], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.0011469155710877297], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.0222116532216841], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.033604532607296525], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.032817898521688024], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 0.00332891369539865]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.06538710407255446], ["'alubox production - APOS' (kilogram, GLO, None)", 0.013180274592389995], ["'market for polysulfone' (kilogram, GLO, None)", 0.0013263096787759548], ["'autoclave - APOS' (unit, GLO, None)", 1.7652980517328842], ["'cabinet washer - APOS' (unit, GLO, None)", 0.23942518454320008], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 0.0009970657657280139], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.002564735440814947], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.06211774886892675], ["'plastic incineration - APOS' (kilogram, CH, None)", 0.0003748168005093725], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.00039646030534795337], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0008254098073275914], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.0006853141716339495], ["'market for corrugated board box' (kilogram, RER, None)", 0.0008955861788366533]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.06538710407255446], ["'alubox production - APOS' (kilogram, GLO, None)", 0.013180274592389995], ["'market for polysulfone' (kilogram, GLO, None)", 0.0013263096787759548], ["'autoclave - APOS' (unit, GLO, None)", 1.7652980517328842], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 0.0009970657657280139], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.002564735440814947], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.06211774886892675], ["'plastic incineration - APOS' (kilogram, CH, None)", 0.0003748168005093725], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.02712421300042628], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.05693259392047285], ["'market for corrugated board box' (kilogram, RER, None)", 0.0008955861788366533], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.0006853141716339495], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.0222116532216841], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.033604532607296525], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.032817898521688024], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 0.00332891369539865]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0038893164281314303], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.003196864257907693], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0005916230734843358], ["'market for corrugated board box' (kilogram, RER, None)", 0.00014086296987526385], ["'autoclave - APOS' (unit, GLO, None)", 0.18289560255800133], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 4.499571160094361e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0021002308711909725], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0002418228629488159], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.004374392906285103], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.00053069646304317], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0005936267349580011], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.00211037963182978], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.00014328905202340439]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0038893164281314303], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.003196864257907693], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0005916230734843358], ["'market for corrugated board box' (kilogram, RER, None)", 0.00014086296987526385], ["'autoclave - APOS' (unit, GLO, None)", 0.18289560255800133], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 4.499571160094361e-06], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.009509549796271964], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.001153687963137326], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0012904929077412585], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.004587781808165952], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.00014328905202340439]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.011065379133557027], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.009095303945033153], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0017842600267449584], ["'market for corrugated board box' (kilogram, RER, None)", 0.0004248248297059437], ["'autoclave - APOS' (unit, GLO, None)", 0.24386080341066843], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 1.3570135248158271e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.005975304732120794], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0007293070322146941], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.01244545587421959], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.001600513110089058], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0016889098762608527], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.006004178669856974], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.0004076674438181271]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.011065379133557027], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.009095303945033153], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0017842600267449584], ["'market for corrugated board box' (kilogram, RER, None)", 0.0004248248297059437], ["'autoclave - APOS' (unit, GLO, None)", 0.24386080341066843], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 1.3570135248158271e-05], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.027055338856999105], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.0034793763262805605], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.003671543204008265], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.013052562326733977], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.0004076674438181271]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.004540664081734213], ["'alubox production - APOS' (kilogram, GLO, None)", 0.001776359395416686], ["'market for polysulfone' (kilogram, GLO, None)", 9.050919199766397e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.36579120511600266], ["'cabinet washer - APOS' (unit, GLO, None)", 0.07507997292982625], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 4.096812045140882e-05], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.003880676105075475], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.004313630877647501], ["'plastic incineration - APOS' (kilogram, CH, None)", 3.793261229936504e-05], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -3.3178182027223115e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -2.3590096288433488e-05], ["'market for corrugated board box' (kilogram, RER, None)", 4.971458013201856e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 4.4872694177170966e-05]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.004540664081734213], ["'alubox production - APOS' (kilogram, GLO, None)", 0.001776359395416686], ["'market for polysulfone' (kilogram, GLO, None)", 9.050919199766397e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.36579120511600266], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 4.096812045140882e-05], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.003880676105075475], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.004313630877647501], ["'plastic incineration - APOS' (kilogram, CH, None)", 3.793261229936504e-05], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0011349586126705542], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0008135627664048369], ["'market for corrugated board box' (kilogram, RER, None)", 4.971458013201856e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 4.4872694177170966e-05], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.0010501800425814362], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0008835114663666673], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.0017228816618627373], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 3.667831067943272e-05]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.0027131739414611154], ["'alubox production - APOS' (kilogram, GLO, None)", 0.0010614244823134854], ["'market for polysulfone' (kilogram, GLO, None)", 4.525459599883198e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.24386080341066843], ["'cabinet washer - APOS' (unit, GLO, None)", 0.037539986464913126], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 2.4479599203680723e-05], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.0023188126437048125], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0025775152443880595], ["'plastic incineration - APOS' (kilogram, CH, None)", 1.896630614968252e-05], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.6589091013611557e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -1.1795048144216744e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.6812691373477915e-05], ["'market for corrugated board box' (kilogram, RER, None)", 2.970585382234541e-05]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.0027131739414611154], ["'alubox production - APOS' (kilogram, GLO, None)", 0.0010614244823134854], ["'market for polysulfone' (kilogram, GLO, None)", 4.525459599883198e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.24386080341066843], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 2.4479599203680723e-05], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.0023188126437048125], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0025775152443880595], ["'plastic incineration - APOS' (kilogram, CH, None)", 1.896630614968252e-05], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0011349586126705542], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0008135627664048369], ["'market for corrugated board box' (kilogram, RER, None)", 2.970585382234541e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.6812691373477915e-05], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.0010501800425814362], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0008835114663666673], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.0017228816618627373], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 3.667831067943272e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.005187092290987113], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.004161632668358269], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0007865998650084757], ["'market for corrugated board box' (kilogram, RER, None)", 0.00018484304338308005], ["'autoclave - APOS' (unit, GLO, None)", 0.2395255102724744], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 6.396241821226289e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0028010298371330413], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0003170268513029706], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.006334064001046305], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.000768449143903179], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0007611001365818738], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0027596641809934453], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.00018998561109331909]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.005187092290987113], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.004161632668358269], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0007865998650084757], ["'market for corrugated board box' (kilogram, RER, None)", 0.00018484304338308005], ["'autoclave - APOS' (unit, GLO, None)", 0.2395255102724744], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 6.396241821226289e-06], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.013769704350100663], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.0016705416171808238], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.001654565521563481], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.005999269958472625], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.00018998561109331909]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.014757642856047842], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.011840138014202398], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0023722852591123015], ["'market for corrugated board box' (kilogram, RER, None)", 0.0005574631466103629], ["'autoclave - APOS' (unit, GLO, None)", 0.3193673470299659], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 1.929025311650959e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.007969127142265834], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.000956112706783545], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.018020858143821882], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.002317544990221091], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0021653835007743615], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.007851438936189293], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.0005405224428729392]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.014757642856047842], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.011840138014202398], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0023722852591123015], ["'market for corrugated board box' (kilogram, RER, None)", 0.0005574631466103629], ["'autoclave - APOS' (unit, GLO, None)", 0.3193673470299659], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 1.929025311650959e-05], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.039175778573525825], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.0050381412830893275], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.004707355429729163], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.017068345514707657], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.0005405224428729392]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.005985809390783058], ["'alubox production - APOS' (kilogram, GLO, None)", 0.0022976263247923697], ["'market for polysulfone' (kilogram, GLO, None)", 0.0001175989876189449], ["'autoclave - APOS' (unit, GLO, None)", 0.4790510205449488], ["'cabinet washer - APOS' (unit, GLO, None)", 0.098414938582881], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 7.273796492625837e-05], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.004962173841942533], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.005686518921243904], ["'plastic incineration - APOS' (kilogram, CH, None)", 5.051402403444565e-05], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -4.25383787242068e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -3.084788289817386e-05], ["'market for corrugated board box' (kilogram, RER, None)", 6.523640883229748e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 5.949628463771938e-05]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.005985809390783058], ["'alubox production - APOS' (kilogram, GLO, None)", 0.0022976263247923697], ["'market for polysulfone' (kilogram, GLO, None)", 0.0001175989876189449], ["'autoclave - APOS' (unit, GLO, None)", 0.4790510205449488], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 7.273796492625837e-05], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.004962173841942533], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.005686518921243904], ["'plastic incineration - APOS' (kilogram, CH, None)", 5.051402403444565e-05], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.001455152041256106], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.001063865473100082], ["'market for corrugated board box' (kilogram, RER, None)", 6.523640883229748e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 5.949628463771938e-05], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.0009072609867581994], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0011746837324725496], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.002494734806621858], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 4.8690173987212356e-05]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.003576688732151947], ["'alubox production - APOS' (kilogram, GLO, None)", 0.0013728960697001918], ["'market for polysulfone' (kilogram, GLO, None)", 5.879949380947245e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.3193673470299659], ["'cabinet washer - APOS' (unit, GLO, None)", 0.0492074692914405], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 4.34629709312173e-05], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.0029650378267613363], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0033978542955443495], ["'plastic incineration - APOS' (kilogram, CH, None)", 2.5257012017222824e-05], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -2.12691893621034e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -1.542394144908693e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 3.5550696188671304e-05], ["'market for corrugated board box' (kilogram, RER, None)", 3.8980581139795035e-05]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.003576688732151947], ["'alubox production - APOS' (kilogram, GLO, None)", 0.0013728960697001918], ["'market for polysulfone' (kilogram, GLO, None)", 5.879949380947245e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.3193673470299659], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 4.34629709312173e-05], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.0029650378267613363], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0033978542955443495], ["'plastic incineration - APOS' (kilogram, CH, None)", 2.5257012017222824e-05], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.001455152041256106], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.001063865473100082], ["'market for corrugated board box' (kilogram, RER, None)", 3.8980581139795035e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 3.5550696188671304e-05], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.0009072609867581994], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0011746837324725496], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.002494734806621858], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 4.8690173987212356e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.3578401328221148], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.2611178645187945], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.04456693785426435], ["'market for corrugated board box' (kilogram, RER, None)", 0.011345660278595016], ["'autoclave - APOS' (unit, GLO, None)", 1.8184930985238714], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 0.0008182394338512325], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.19323367172394199], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.016232216181721347], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.24367517358232688], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.02955992029081428], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.019325612922416628], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.20297142052789444], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.004775465332273835]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.3578401328221148], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.2611178645187945], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.04456693785426435], ["'market for corrugated board box' (kilogram, RER, None)", 0.011345660278595016], ["'autoclave - APOS' (unit, GLO, None)", 1.8184930985238714], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 0.0008182394338512325], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.5297286382224498], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.06426069628437886], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.042012202189471715], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.44124221852354545], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.004775465332273835]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.01808037788827], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.7428987131379786], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.1344082225520165], ["'market for corrugated board box' (kilogram, RER, None)", 0.034217070675307514], ["'autoclave - APOS' (unit, GLO, None)", 2.424657464698495], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 0.0024677062296987484], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.549763404059666], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.048954301778588276], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.6932730290652117], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.08914896415050584], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.054982730068201896], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.5774679850693567], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.013586535171802049]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.01808037788827], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.7428987131379786], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.1344082225520165], ["'market for corrugated board box' (kilogram, RER, None)", 0.034217070675307514], ["'autoclave - APOS' (unit, GLO, None)", 2.424657464698495], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 0.0024677062296987484], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.507115280576547], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.19380209597936052], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.11952767389024874], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -1.255365185025517], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.013586535171802049]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.12275723913911238], ["'alubox production - APOS' (kilogram, GLO, None)", 0.07271287674687871], ["'market for polysulfone' (kilogram, GLO, None)", 0.008110339097513275], ["'autoclave - APOS' (unit, GLO, None)", 3.636986197047743], ["'cabinet washer - APOS' (unit, GLO, None)", 0.6430113020583837], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 0.031538618830432755], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.34033910168240944], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.11661937718215674], ["'plastic incineration - APOS' (kilogram, CH, None)", 0.0003997203771060025], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0010801210012432443], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0022688407724546105], ["'market for corrugated board box' (kilogram, RER, None)", 0.004004208753871521], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.001495494543252368]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.12275723913911238], ["'alubox production - APOS' (kilogram, GLO, None)", 0.07271287674687871], ["'market for polysulfone' (kilogram, GLO, None)", 0.008110339097513275], ["'autoclave - APOS' (unit, GLO, None)", 3.636986197047743], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 0.031538618830432755], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.34033910168240944], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.11661937718215674], ["'plastic incineration - APOS' (kilogram, CH, None)", 0.0003997203771060025], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.03694875843653827], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.07824658080244039], ["'market for corrugated board box' (kilogram, RER, None)", 0.004004208753871521], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.001495494543252368], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.04622897145967616], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.06655487654190648], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.09596492183710925], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 0.0002950255884151562]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.07335088796763493], ["'alubox production - APOS' (kilogram, GLO, None)", 0.04344798004149145], ["'market for polysulfone' (kilogram, GLO, None)", 0.004055169548756637], ["'autoclave - APOS' (unit, GLO, None)", 2.424657464698495], ["'cabinet washer - APOS' (unit, GLO, None)", 0.3215056510291919], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 0.018845207929965017], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.20336214380173326], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0696833435692532], ["'plastic incineration - APOS' (kilogram, CH, None)", 0.00019986018855300126], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0005400605006216221], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0011344203862273053], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.0008935998690122351], ["'market for corrugated board box' (kilogram, RER, None)", 0.0023926268632017433]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.07335088796763493], ["'alubox production - APOS' (kilogram, GLO, None)", 0.04344798004149145], ["'market for polysulfone' (kilogram, GLO, None)", 0.004055169548756637], ["'autoclave - APOS' (unit, GLO, None)", 2.424657464698495], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 0.018845207929965017], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.20336214380173326], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0696833435692532], ["'plastic incineration - APOS' (kilogram, CH, None)", 0.00019986018855300126], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.03694875843653827], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.07824658080244039], ["'market for corrugated board box' (kilogram, RER, None)", 0.0023926268632017433], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.0008935998690122351], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.04622897145967616], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.06655487654190648], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.09596492183710925], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 0.0002950255884151562]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.12160802955097787], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.01398801497552866], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.01341615937285153], ["'market for corrugated board box' (kilogram, RER, None)", 0.0007403664796185518], ["'autoclave - APOS' (unit, GLO, None)", 0.1777594167481993], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 6.275383538786159e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.06566833595752805], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0004943311668072049], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.00014232807687588331], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.6743018471277034e-05], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0034997922719116298], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.01148925222700415], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.0003492632851573382]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.12160802955097787], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.01398801497552866], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.01341615937285153], ["'market for corrugated board box' (kilogram, RER, None)", 0.0007403664796185518], ["'autoclave - APOS' (unit, GLO, None)", 0.1777594167481993], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 6.275383538786159e-05], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.00030940886277365943], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 3.63978662419066e-05], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.007608244102734292], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.02497663527522678], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.0003492632851573382]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.34598340801827504], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.039796887676856185], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.04046143220959501], ["'market for corrugated board box' (kilogram, RER, None)", 0.0022328512873358948], ["'autoclave - APOS' (unit, GLO, None)", 0.23701255566426574], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 0.00018925759883661535], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.18683104032986853], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0014908399966784642], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.00040493340181589345], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 5.049481658889875e-05], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.009957155540360136], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.03268773168274644], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.0009936786423596217]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.34598340801827504], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.039796887676856185], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.04046143220959501], ["'market for corrugated board box' (kilogram, RER, None)", 0.0022328512873358948], ["'autoclave - APOS' (unit, GLO, None)", 0.23701255566426574], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 0.00018925759883661535], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.0008802900039475944], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.00010977134041064945], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.02164599027415249], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0710602862720553], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.0009936786423596217]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.022981548034039796], ["'alubox production - APOS' (kilogram, GLO, None)", 0.005016176585510375], ["'market for polysulfone' (kilogram, GLO, None)", 0.0012730290747981396], ["'autoclave - APOS' (unit, GLO, None)", 0.3555188334963986], ["'cabinet washer - APOS' (unit, GLO, None)", 0.05477341734897272], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 0.0005208426789368262], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.0010836719002031965], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.021832470632337807], ["'plastic incineration - APOS' (kilogram, CH, None)", 2.495830869459455e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.00019560565287405393], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.00012842834636445536], ["'market for corrugated board box' (kilogram, RER, None)", 0.0002612965544504003], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.00010937600857055998]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.022981548034039796], ["'alubox production - APOS' (kilogram, GLO, None)", 0.005016176585510375], ["'market for polysulfone' (kilogram, GLO, None)", 0.0012730290747981396], ["'autoclave - APOS' (unit, GLO, None)", 0.3555188334963986], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 0.0005208426789368262], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.0010836719002031965], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.021832470632337807], ["'plastic incineration - APOS' (kilogram, CH, None)", 2.495830869459455e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.006691274411427875], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.004429168896792291], ["'market for corrugated board box' (kilogram, RER, None)", 0.0002612965544504003], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.00010937600857055998], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.002855191486274772], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.020035274436994724], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 5.43554394973342e-05], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 5.383455906749426e-05]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.013732118504696628], ["'alubox production - APOS' (kilogram, GLO, None)", 0.00299730597828681], ["'market for polysulfone' (kilogram, GLO, None)", 0.0006365145373990698], ["'autoclave - APOS' (unit, GLO, None)", 0.23701255566426574], ["'cabinet washer - APOS' (unit, GLO, None)", 0.02738670867448636], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 0.00031121808586916555], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.0006475243065331577], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.013045512579461797], ["'plastic incineration - APOS' (kilogram, CH, None)", 1.2479154347297276e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -9.780282643702696e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -6.421417318222768e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 6.535522805664957e-05], ["'market for corrugated board box' (kilogram, RER, None)", 0.00015613200856114617]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.013732118504696628], ["'alubox production - APOS' (kilogram, GLO, None)", 0.00299730597828681], ["'market for polysulfone' (kilogram, GLO, None)", 0.0006365145373990698], ["'autoclave - APOS' (unit, GLO, None)", 0.23701255566426574], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 0.00031121808586916555], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.0006475243065331577], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.013045512579461797], ["'plastic incineration - APOS' (kilogram, CH, None)", 1.2479154347297276e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.006691274411427875], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.004429168896792291], ["'market for corrugated board box' (kilogram, RER, None)", 0.00015613200856114617], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 6.535522805664957e-05], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.002855191486274772], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.020035274436994724], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 5.43554394973342e-05], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 5.383455906749426e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 2.7820788855704762e-05], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 2.03085312752671e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 5.771668255169241e-06], ["'market for corrugated board box' (kilogram, RER, None)", 1.516700055431044e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.00036381489119654544], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 2.5474719020016852e-08], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -1.5023225982080572e-05], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -3.840660149966872e-06], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 7.884780135491285e-08], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 8.886831188436638e-09], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -5.777294415194854e-06], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -1.242822888776668e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.1357420168807041e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 2.7820788855704762e-05], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 2.03085312752671e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 5.771668255169241e-06], ["'market for corrugated board box' (kilogram, RER, None)", 1.516700055431044e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.00036381489119654544], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 2.5474719020016852e-08], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.7140826381502794e-07], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.9319198235731823e-08], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.2559335740277296e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -2.7017888885509065e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.1357420168807041e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 7.915210350496285e-05], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 5.7779201656393715e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.740661819472455e-05], ["'market for corrugated board box' (kilogram, RER, None)", 4.574174769522845e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.0004850865215953939], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 7.682851769883089e-08], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -4.274213589267994e-05], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -1.1582943074784635e-05], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 2.2432754751679433e-07], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 2.6801553834897404e-08], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.6436809566165485e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -3.535918640729556e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 3.2312660201211675e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 7.915210350496285e-05], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 5.7779201656393715e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.740661819472455e-05], ["'market for corrugated board box' (kilogram, RER, None)", 4.574174769522845e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.0004850865215953939], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 7.682851769883089e-08], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 4.876685815582485e-07], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 5.826424746716827e-08], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -3.573219465791796e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -7.686779654324047e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 3.2312660201211675e-06]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 3.401088911889249e-05], ["'alubox production - APOS' (kilogram, GLO, None)", 1.2873970175015666e-05], ["'market for polysulfone' (kilogram, GLO, None)", 7.228334426162012e-07], ["'autoclave - APOS' (unit, GLO, None)", 0.0007276297823930909], ["'cabinet washer - APOS' (unit, GLO, None)", 0.00011033674379167988], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 1.1736799591732176e-07], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -5.467509718432362e-06], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 3.231034466294787e-05], ["'plastic incineration - APOS' (kilogram, CH, None)", 1.6535761758289208e-09], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -3.2289672018521146e-07], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -1.3892434883997888e-07], ["'market for corrugated board box' (kilogram, RER, None)", 5.352869282021617e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 3.5567130543460443e-07]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 3.401088911889249e-05], ["'alubox production - APOS' (kilogram, GLO, None)", 1.2873970175015666e-05], ["'market for polysulfone' (kilogram, GLO, None)", 7.228334426162012e-07], ["'autoclave - APOS' (unit, GLO, None)", 0.0007276297823930909], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 1.1736799591732176e-07], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -5.467509718432362e-06], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 3.231034466294787e-05], ["'plastic incineration - APOS' (kilogram, CH, None)", 1.6535761758289208e-09], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.1045644793816095e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -4.79114947990529e-06], ["'market for corrugated board box' (kilogram, RER, None)", 5.352869282021617e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 3.5567130543460443e-07], ["'production of wet wipe - APOS' (unit, GLO, None)", 9.71701290873255e-06], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 8.619229560257396e-06], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 2.885068877005467e-08], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 1.952361360397637e-08]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 2.0322458658527112e-05], ["'alubox production - APOS' (kilogram, GLO, None)", 7.692557690517278e-06], ["'market for polysulfone' (kilogram, GLO, None)", 3.614167213081006e-07], ["'autoclave - APOS' (unit, GLO, None)", 0.0004850865215953939], ["'cabinet washer - APOS' (unit, GLO, None)", 5.516837189583994e-05], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 7.013066422715202e-08], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -3.266990163930036e-06], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 1.9306335725600756e-05], ["'plastic incineration - APOS' (kilogram, CH, None)", 8.267880879144604e-10], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.6144836009260573e-07], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -6.946217441998944e-08], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.125235651188458e-07], ["'market for corrugated board box' (kilogram, RER, None)", 3.198489296290891e-07]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 2.0322458658527112e-05], ["'alubox production - APOS' (kilogram, GLO, None)", 7.692557690517278e-06], ["'market for polysulfone' (kilogram, GLO, None)", 3.614167213081006e-07], ["'autoclave - APOS' (unit, GLO, None)", 0.0004850865215953939], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 7.013066422715202e-08], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -3.266990163930036e-06], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 1.9306335725600756e-05], ["'plastic incineration - APOS' (kilogram, CH, None)", 8.267880879144604e-10], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.1045644793816095e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -4.79114947990529e-06], ["'market for corrugated board box' (kilogram, RER, None)", 3.198489296290891e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.125235651188458e-07], ["'production of wet wipe - APOS' (unit, GLO, None)", 9.71701290873255e-06], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 8.619229560257396e-06], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 2.885068877005467e-08], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 1.952361360397637e-08]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 2.8165094887766917e-06], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 2.712469693085515e-06], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 7.868421577361211e-07], ["'market for corrugated board box' (kilogram, RER, None)", 1.6026019729633196e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.0005291744184886976], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 5.416698624596908e-09], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -1.5209151239394136e-06], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -3.5050431936777156e-07], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.311470835321409e-07], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.5835262187088882e-08], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -4.870860264611179e-07], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -1.3482722082220904e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 9.019456703665286e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 2.8165094887766917e-06], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 2.712469693085515e-06], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 7.868421577361211e-07], ["'market for corrugated board box' (kilogram, RER, None)", 1.6026019729633196e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.0005291744184886976], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 5.416698624596908e-09], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 2.8510235550465413e-07], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 3.442448301541061e-08], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.0588826708628879e-06], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -2.931026539511239e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 9.019456703665286e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 8.013167841308334e-06], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 7.71716729582076e-06], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 2.373015983196747e-06], ["'market for corrugated board box' (kilogram, RER, None)", 4.833244044573473e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.0007055658913182633], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 1.633607522116651e-08], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -4.3271106343065004e-06], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -1.057076497314674e-06], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 3.731226883590488e-07], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 4.775713896188452e-08], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.3857940558169756e-06], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -3.835929380511093e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.5660989497026737e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 8.013167841308334e-06], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 7.71716729582076e-06], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 2.373015983196747e-06], ["'market for corrugated board box' (kilogram, RER, None)", 4.833244044573473e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.0007055658913182633], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 1.633607522116651e-08], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 8.111362790414103e-07], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.038198673084446e-07], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -3.012595769203746e-06], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -8.338976914766559e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.5660989497026737e-05]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 2.746686004102047e-06], ["'alubox production - APOS' (kilogram, GLO, None)", 2.7296373689588363e-06], ["'market for polysulfone' (kilogram, GLO, None)", 1.200900986770645e-07], ["'autoclave - APOS' (unit, GLO, None)", 0.0010583488369773951], ["'cabinet washer - APOS' (unit, GLO, None)", 0.000188952437183112], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 4.640461358369972e-08], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -1.6860703098206212e-07], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 2.6093517038969446e-06], ["'plastic incineration - APOS' (kilogram, CH, None)", 6.775843940454812e-09], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -2.7223552945247902e-08], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -1.507116100594709e-08], ["'market for corrugated board box' (kilogram, RER, None)", 5.656041774155925e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.8245516080439977e-06]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 2.746686004102047e-06], ["'alubox production - APOS' (kilogram, GLO, None)", 2.7296373689588363e-06], ["'market for polysulfone' (kilogram, GLO, None)", 1.200900986770645e-07], ["'autoclave - APOS' (unit, GLO, None)", 0.0010583488369773951], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 4.640461358369972e-08], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -1.6860703098206212e-07], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 2.6093517038969446e-06], ["'plastic incineration - APOS' (kilogram, CH, None)", 6.775843940454812e-09], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -9.312627755598563e-07], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -5.197662311765511e-07], ["'market for corrugated board box' (kilogram, RER, None)", 5.656041774155925e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.8245516080439977e-06], ["'production of wet wipe - APOS' (unit, GLO, None)", 9.480215969870325e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.1750455648835664e-06], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 5.1408450466165156e-08], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 4.6660602946941943e-07]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 1.6412218031463373e-06], ["'alubox production - APOS' (kilogram, GLO, None)", 1.6310347662338046e-06], ["'market for polysulfone' (kilogram, GLO, None)", 6.004504933853225e-08], ["'autoclave - APOS' (unit, GLO, None)", 0.0007055658913182633], ["'cabinet washer - APOS' (unit, GLO, None)", 9.4476218591556e-05], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 2.772805608883098e-08], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -1.0074742252964469e-07], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 1.5591607129890205e-06], ["'plastic incineration - APOS' (kilogram, CH, None)", 3.387921970227406e-09], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.3611776472623951e-08], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -7.535580502973545e-09], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.6877486837746894e-06], ["'market for corrugated board box' (kilogram, RER, None)", 3.3796433503004436e-07]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 1.6412218031463373e-06], ["'alubox production - APOS' (kilogram, GLO, None)", 1.6310347662338046e-06], ["'market for polysulfone' (kilogram, GLO, None)", 6.004504933853225e-08], ["'autoclave - APOS' (unit, GLO, None)", 0.0007055658913182633], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 2.772805608883098e-08], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -1.0074742252964469e-07], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 1.5591607129890205e-06], ["'plastic incineration - APOS' (kilogram, CH, None)", 3.387921970227406e-09], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -9.312627755598563e-07], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -5.197662311765511e-07], ["'market for corrugated board box' (kilogram, RER, None)", 3.3796433503004436e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.6877486837746894e-06], ["'production of wet wipe - APOS' (unit, GLO, None)", 9.480215969870325e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.1750455648835664e-06], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 5.1408450466165156e-08], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 4.6660602946941943e-07]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.006163217792741251], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.0027284119152065477], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.000905708533043928], ["'market for corrugated board box' (kilogram, RER, None)", 0.00015781328132461432], ["'autoclave - APOS' (unit, GLO, None)", 0.07359486666609583], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 2.6041536632474646e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0033281376080802755], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0003082963444235658], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.0002809081465027925], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 3.2899921324107254e-05], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0009226184376774954], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0018295054352353481], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 8.096556878010072e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.006163217792741251], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.0027284119152065477], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.000905708533043928], ["'market for corrugated board box' (kilogram, RER, None)", 0.00015781328132461432], ["'autoclave - APOS' (unit, GLO, None)", 0.07359486666609583], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 2.6041536632474646e-05], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.0006106698837017229], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 7.152156809588534e-05], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.002005692264615348], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.003977185728634087], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 8.096556878010072e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.017534788649770882], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.007762524040446798], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0027315018697202367], ["'market for corrugated board box' (kilogram, RER, None)", 0.00047594481660746596], ["'autoclave - APOS' (unit, GLO, None)", 0.09812648888812778], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 7.85379676415959e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.009468785870876276], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0009297826072044314], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.000799203459064283], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 9.922198293574986e-05], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.002624914444805326], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0052050718008036035], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.00023035274499878157]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.017534788649770882], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.007762524040446798], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0027315018697202367], ["'market for corrugated board box' (kilogram, RER, None)", 0.00047594481660746596], ["'autoclave - APOS' (unit, GLO, None)", 0.09812648888812778], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 7.85379676415959e-05], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.001737398824052789], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.00021569996290380402], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.005706335741410284], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.011315373480838284], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.00023035274499878157]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.021747164400469948], ["'alubox production - APOS' (kilogram, GLO, None)", 0.0015690717936241686], ["'market for polysulfone' (kilogram, GLO, None)", 0.00011911039136193448], ["'autoclave - APOS' (unit, GLO, None)", 0.14718973333219165], ["'cabinet washer - APOS' (unit, GLO, None)", 0.025571879387756444], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 8.548884920569733e-05], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.0005548138502198018], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.02065980618044645], ["'plastic incineration - APOS' (kilogram, CH, None)", 7.576165333493608e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -5.1565741002385704e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -2.0450448216273988e-05], ["'market for corrugated board box' (kilogram, RER, None)", 5.569683095036782e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.535534400881328e-05]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.021747164400469948], ["'alubox production - APOS' (kilogram, GLO, None)", 0.0015690717936241686], ["'market for polysulfone' (kilogram, GLO, None)", 0.00011911039136193448], ["'autoclave - APOS' (unit, GLO, None)", 0.14718973333219165], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 8.548884920569733e-05], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.0005548138502198018], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.02065980618044645], ["'plastic incineration - APOS' (kilogram, CH, None)", 7.576165333493608e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0017639598764445956], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0007052842439311452], ["'market for corrugated board box' (kilogram, RER, None)", 5.569683095036782e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.535534400881328e-05], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.000654604724331231], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00135255690657513], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.00010680808159337649], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 1.2977040930919572e-05]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.012994539717082662], ["'alubox production - APOS' (kilogram, GLO, None)", 0.000937564335549088], ["'market for polysulfone' (kilogram, GLO, None)", 5.955519568096724e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.09812648888812778], ["'cabinet washer - APOS' (unit, GLO, None)", 0.012785939693878222], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 5.108198135234208e-05], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.0003315168120085104], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.012344812731228528], ["'plastic incineration - APOS' (kilogram, CH, None)", 3.788082666746804e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -2.5782870501192852e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -1.0225224108136994e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.5150528089364082e-05], ["'market for corrugated board box' (kilogram, RER, None)", 3.328041621161996e-05]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.012994539717082662], ["'alubox production - APOS' (kilogram, GLO, None)", 0.000937564335549088], ["'market for polysulfone' (kilogram, GLO, None)", 5.955519568096724e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.09812648888812778], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 5.108198135234208e-05], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.0003315168120085104], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.012344812731228528], ["'plastic incineration - APOS' (kilogram, CH, None)", 3.788082666746804e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0017639598764445956], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0007052842439311452], ["'market for corrugated board box' (kilogram, RER, None)", 3.328041621161996e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.5150528089364082e-05], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.000654604724331231], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00135255690657513], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.00010680808159337649], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 1.2977040930919572e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.08227176533761078], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.05617292099088791], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.013688097170889708], ["'market for corrugated board box' (kilogram, RER, None)", 0.0032036538358738618], ["'autoclave - APOS' (unit, GLO, None)", 3.8280017765525995], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 8.820584758614293e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.04442675328230982], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.004557659174500415], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.0528962044425517], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.006417240333406325], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.011865380993004838], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.05072810362977204], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.00370090052776332]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.08227176533761078], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.05617292099088791], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.013688097170889708], ["'market for corrugated board box' (kilogram, RER, None)", 0.0032036538358738618], ["'autoclave - APOS' (unit, GLO, None)", 3.8280017765525995], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 8.820584758614293e-05], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.11499174878815586], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.013950522463926793], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.025794306619637015], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.1102784861478406], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.00370090052776332]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.23406896617179404], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.15981591605858247], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.04128156206008065], ["'market for corrugated board box' (kilogram, RER, None)", 0.009661813154067984], ["'autoclave - APOS' (unit, GLO, None)", 5.1040023687368], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 0.00026601763564448053], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.12639724173276878], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.013745321041478662], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.1504934267238795], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.019353581565840595], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.03375784472729563], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.14432502720474438], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.01052932262914265]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.23406896617179404], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.15981591605858247], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.04128156206008065], ["'market for corrugated board box' (kilogram, RER, None)", 0.009661813154067984], ["'autoclave - APOS' (unit, GLO, None)", 5.1040023687368], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 0.00026601763564448053], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.3271596233127815], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.04207300340400129], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.07338661886735595], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.3137500591637752], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.01052932262914265]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.09654217417855032], ["'alubox production - APOS' (kilogram, GLO, None)", 0.033842449781809336], ["'market for polysulfone' (kilogram, GLO, None)", 0.002310598647783998], ["'autoclave - APOS' (unit, GLO, None)", 7.656003553105199], ["'cabinet washer - APOS' (unit, GLO, None)", 1.5584801389813074], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 0.0012879710296650718], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.056716450046849505], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0917150654696228], ["'plastic incineration - APOS' (kilogram, CH, None)", 0.000742088521516806], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0006631638152822077], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0005670452989154309], ["'market for corrugated board box' (kilogram, RER, None)", 0.001130661276557168], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.0011589816194424178]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.09654217417855032], ["'alubox production - APOS' (kilogram, GLO, None)", 0.033842449781809336], ["'market for polysulfone' (kilogram, GLO, None)", 0.002310598647783998], ["'autoclave - APOS' (unit, GLO, None)", 7.656003553105199], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 0.0012879710296650718], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.056716450046849505], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0917150654696228], ["'plastic incineration - APOS' (kilogram, CH, None)", 0.000742088521516806], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.022685495038529725], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.019555958416697515], ["'market for corrugated board box' (kilogram, RER, None)", 0.001130661276557168], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.0011589816194424178], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.018810053238438915], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.020441377872566013], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.020833275629523654], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 0.000869493903790299]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.05768665255087576], ["'alubox production - APOS' (kilogram, GLO, None)", 0.02022181143779801], ["'market for polysulfone' (kilogram, GLO, None)", 0.001155299323891999], ["'autoclave - APOS' (unit, GLO, None)", 5.1040023687368], ["'cabinet washer - APOS' (unit, GLO, None)", 0.7792400694906537], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 0.0007695987573935358], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.03388966713884751], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.054802319923331975], ["'plastic incineration - APOS' (kilogram, CH, None)", 0.000371044260758403], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.00033158190764110383], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.00028352264945771544], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.0006925239734201838], ["'market for corrugated board box' (kilogram, RER, None)", 0.0006756017754711337]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.05768665255087576], ["'alubox production - APOS' (kilogram, GLO, None)", 0.02022181143779801], ["'market for polysulfone' (kilogram, GLO, None)", 0.001155299323891999], ["'autoclave - APOS' (unit, GLO, None)", 5.1040023687368], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 0.0007695987573935358], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.03388966713884751], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.054802319923331975], ["'plastic incineration - APOS' (kilogram, CH, None)", 0.000371044260758403], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.022685495038529725], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.019555958416697515], ["'market for corrugated board box' (kilogram, RER, None)", 0.0006756017754711337], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.0006925239734201838], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.018810053238438915], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.020441377872566013], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.020833275629523654], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 0.000869493903790299]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0033518088012856615], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.005699222367795836], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0017894591454651648], ["'market for corrugated board box' (kilogram, RER, None)", 0.0002570042584643343], ["'autoclave - APOS' (unit, GLO, None)", 0.09516491017293233], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 3.5998554509729677e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0018099767526942572], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0004546499972774677], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.2324953663342778e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.433427559309469e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0032068496033723346], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0033719954330666004], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.00013698684289934363]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0033518088012856615], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.005699222367795836], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0017894591454651648], ["'market for corrugated board box' (kilogram, RER, None)", 0.0002570042584643343], ["'autoclave - APOS' (unit, GLO, None)", 0.09516491017293233], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 3.5998554509729677e-06], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 2.679337752900604e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 3.116146868064063e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.006971412211812963], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0073304248542375074], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.00013698684289934363]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.009536132082531037], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.016214688990067026], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.005396781440491304], ["'market for corrugated board box' (kilogram, RER, None)", 0.0007750922079272868], ["'autoclave - APOS' (unit, GLO, None)", 0.1268865468972431], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 1.0856706918376308e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.00514951132456676], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.001371166630679708], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 3.506536112669354e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 4.323035408757078e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.009123713013366758], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.009593564469971453], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.00038973721504116876]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.009536132082531037], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.016214688990067026], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.005396781440491304], ["'market for corrugated board box' (kilogram, RER, None)", 0.0007750922079272868], ["'autoclave - APOS' (unit, GLO, None)", 0.1268865468972431], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 1.0856706918376308e-05], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 7.622904592759465e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 9.397903062515385e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.019834158696325068], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.020855574936251172], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.00038973721504116876]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.001713507960233992], ["'alubox production - APOS' (kilogram, GLO, None)", 0.006760525475713876], ["'market for polysulfone' (kilogram, GLO, None)", 0.0001246382208782475], ["'autoclave - APOS' (unit, GLO, None)", 0.19032982034586465], ["'cabinet washer - APOS' (unit, GLO, None)", 0.020920322230852356], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 2.6629610273703898e-05], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.0003865100370934076], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0016278325622222922], ["'plastic incineration - APOS' (kilogram, CH, None)", 3.29904104740962e-07], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0001792328977267898], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -3.769260077687061e-05], ["'market for corrugated board box' (kilogram, RER, None)", 9.07041702514809e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 4.2899081408636746e-05]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.001713507960233992], ["'alubox production - APOS' (kilogram, GLO, None)", 0.006760525475713876], ["'market for polysulfone' (kilogram, GLO, None)", 0.0001246382208782475], ["'autoclave - APOS' (unit, GLO, None)", 0.19032982034586465], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 2.6629610273703898e-05], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.0003865100370934076], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0016278325622222922], ["'plastic incineration - APOS' (kilogram, CH, None)", 3.29904104740962e-07], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.006131195518247818], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0012999224838289249], ["'market for corrugated board box' (kilogram, RER, None)", 9.07041702514809e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 4.2899081408636746e-05], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.0006033510993987782], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.002672322538574945], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 4.65355665153934e-06], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 3.654304976335396e-06]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.0010238689897574297], ["'alubox production - APOS' (kilogram, GLO, None)", 0.004039603287342358], ["'market for polysulfone' (kilogram, GLO, None)", 6.231911043912375e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.1268865468972431], ["'cabinet washer - APOS' (unit, GLO, None)", 0.010460161115426178], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 1.591193784991112e-05], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.0002309505706386642], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0009726755402695583], ["'plastic incineration - APOS' (kilogram, CH, None)", 1.64952052370481e-07], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -8.96164488633949e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -1.8846300388435306e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.563340247576815e-05], ["'market for corrugated board box' (kilogram, RER, None)", 5.41982817799616e-05]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.0010238689897574297], ["'alubox production - APOS' (kilogram, GLO, None)", 0.004039603287342358], ["'market for polysulfone' (kilogram, GLO, None)", 6.231911043912375e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.1268865468972431], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 1.591193784991112e-05], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.0002309505706386642], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0009726755402695583], ["'plastic incineration - APOS' (kilogram, CH, None)", 1.64952052370481e-07], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.006131195518247818], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0012999224838289249], ["'market for corrugated board box' (kilogram, RER, None)", 5.41982817799616e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.563340247576815e-05], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.0006033510993987782], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.002672322538574945], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 4.65355665153934e-06], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 3.654304976335396e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0013207950818693518], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.0011482939111115064], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0005957474106542295], ["'market for corrugated board box' (kilogram, RER, None)", 0.0011380431270982202], ["'autoclave - APOS' (unit, GLO, None)", 0.02865927517048255], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 7.892479440964108e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.00071322934420945], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.00012281030538521104], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 9.0551581947656e-06], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.0459819392531231e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.00026614484518127247], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.026135974489495777], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 5.478383471812598e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0013207950818693518], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.0011482939111115064], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0005957474106542295], ["'market for corrugated board box' (kilogram, RER, None)", 0.0011380431270982202], ["'autoclave - APOS' (unit, GLO, None)", 0.02865927517048255], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 7.892479440964108e-06], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.9685126510360004e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 2.27387378098505e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0005785757529310518], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.056817335844752674], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 5.478383471812598e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.003757755021656466], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.003266977042880624], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0017966985036720331], ["'market for corrugated board box' (kilogram, RER, None)", 0.003432193557296425], ["'autoclave - APOS' (unit, GLO, None)", 0.03821236689397673], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 2.3802715780351274e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0020291877116944915], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.0003703802785794745], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 2.5762562751304952e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 3.154548641781353e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0007572008318903769], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.07435868797202924], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.00015586386780230274]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.003757755021656466], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.003266977042880624], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0017966985036720331], ["'market for corrugated board box' (kilogram, RER, None)", 0.003432193557296425], ["'autoclave - APOS' (unit, GLO, None)", 0.03821236689397673], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 2.3802715780351274e-05], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 5.600557119848902e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 6.857714438655115e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.001646088762623312], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.1616493216901881], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.00015586386780230274]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.001252317123516156], ["'alubox production - APOS' (kilogram, GLO, None)", 0.0011490147079334023], ["'market for polysulfone' (kilogram, GLO, None)", 3.353268334471497e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.0573185503409651], ["'cabinet washer - APOS' (unit, GLO, None)", 0.010656897505563319], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 6.230212309070663e-05], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.0002647636366250949], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0011897012673403482], ["'plastic incineration - APOS' (kilogram, CH, None)", 1.757865092673772e-07], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.4875007473603942e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.00029215130088451147], ["'market for corrugated board box' (kilogram, RER, None)", 0.0004016480433851245], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.715621833242094e-05]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.001252317123516156], ["'alubox production - APOS' (kilogram, GLO, None)", 0.0011490147079334023], ["'market for polysulfone' (kilogram, GLO, None)", 3.353268334471497e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.0573185503409651], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 6.230212309070663e-05], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.0002647636366250949], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0011897012673403482], ["'plastic incineration - APOS' (kilogram, CH, None)", 1.757865092673772e-07], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0005088439695657025], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.010075559575944339], ["'market for corrugated board box' (kilogram, RER, None)", 0.0004016480433851245], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.715621833242094e-05], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.019660182631987582], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0008896706230055435], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 3.395732263684289e-06], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 1.59683313047684e-06]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.0007482945500500169], ["'alubox production - APOS' (kilogram, GLO, None)", 0.0006865684639524811], ["'market for polysulfone' (kilogram, GLO, None)", 1.6766341672357485e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.03821236689397673], ["'cabinet washer - APOS' (unit, GLO, None)", 0.0053284487527816594], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 3.7227263198657037e-05], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.00015820368708343834], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.000710879822547516], ["'plastic incineration - APOS' (kilogram, CH, None)", 8.78932546336886e-08], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -7.437503736801971e-06], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.00014607565044225573], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.02513208916534e-05], ["'market for corrugated board box' (kilogram, RER, None)", 0.00023999595356423876]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.0007482945500500169], ["'alubox production - APOS' (kilogram, GLO, None)", 0.0006865684639524811], ["'market for polysulfone' (kilogram, GLO, None)", 1.6766341672357485e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.03821236689397673], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 3.7227263198657037e-05], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.00015820368708343834], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.000710879822547516], ["'plastic incineration - APOS' (kilogram, CH, None)", 8.78932546336886e-08], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0005088439695657025], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.010075559575944339], ["'market for corrugated board box' (kilogram, RER, None)", 0.00023999595356423876], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.02513208916534e-05], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.019660182631987582], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0008896706230055435], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 3.395732263684289e-06], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 1.59683313047684e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0012989509221187153], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.0005892081487004746], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00014519187021813312], ["'market for corrugated board box' (kilogram, RER, None)", 3.0438550705806856e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.009751364919147791], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 3.864587460542977e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0007014334979441063], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -6.005277350824894e-05], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.905648197566849e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 2.09196053591378e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -7.917330401631962e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.00023595892111971968], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.3580584486039177e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0012989509221187153], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.0005892081487004746], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00014519187021813312], ["'market for corrugated board box' (kilogram, RER, None)", 3.0438550705806856e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.009751364919147791], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 3.864587460542977e-06], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 4.1427134729714115e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 4.54774029546474e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.00017211587905105325], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0005129541763293656], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.3580584486039177e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0036956068488447954], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.001676338676584449], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0004378802346447291], ["'market for corrugated board box' (kilogram, RER, None)", 9.179880369937363e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.013001819892197055], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 1.1655105042678095e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0019956276983761896], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.00018111153548302944], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 5.42170332265498e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 6.309087202728489e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.000225253626925724], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.000671319747301161], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 3.863771924512008e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0036956068488447954], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.001676338676584449], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0004378802346447291], ["'market for corrugated board box' (kilogram, RER, None)", 9.179880369937363e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.013001819892197055], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 1.1655105042678095e-05], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.00011786311570989085], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.3715406962453237e-05], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0004896817969638187], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0014593907551096307], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 3.863771924512008e-05]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.0016993364308568917], ["'alubox production - APOS' (kilogram, GLO, None)", 0.00020228344345516995], ["'market for polysulfone' (kilogram, GLO, None)", 6.169988243712124e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.019502729838295582], ["'cabinet washer - APOS' (unit, GLO, None)", 0.0034651248250365157], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 1.8556450010247273e-05], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.00019946384308320068], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.001614369609314047], ["'plastic incineration - APOS' (kilogram, CH, None)", 3.9970205978131766e-07], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -4.425047151112515e-06], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -2.6375793176618552e-06], ["'market for corrugated board box' (kilogram, RER, None)", 1.0742637113972112e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 4.25292376342703e-06]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.0016993364308568917], ["'alubox production - APOS' (kilogram, GLO, None)", 0.00020228344345516995], ["'market for polysulfone' (kilogram, GLO, None)", 6.169988243712124e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.019502729838295582], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 1.8556450010247273e-05], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.00019946384308320068], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.001614369609314047], ["'plastic incineration - APOS' (kilogram, CH, None)", 3.9970205978131766e-07], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.00015137192783822912], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -9.096344076142203e-05], ["'market for corrugated board box' (kilogram, RER, None)", 1.0742637113972112e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 4.25292376342703e-06], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.00011335676606923576], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00021682501563951944], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 6.791453675795855e-06], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 4.196312874609168e-06]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.0010154011041079998], ["'alubox production - APOS' (kilogram, GLO, None)", 0.00012087002202593586], ["'market for polysulfone' (kilogram, GLO, None)", 3.084994121856062e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.013001819892197055], ["'cabinet washer - APOS' (unit, GLO, None)", 0.0017325624125182578], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 1.1087998519062382e-05], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.00011918523184616125], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0009646310489025998], ["'plastic incineration - APOS' (kilogram, CH, None)", 1.9985102989065883e-07], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -2.2125235755562576e-06], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -1.3187896588309276e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.54124104635806e-06], ["'market for corrugated board box' (kilogram, RER, None)", 6.419026509461157e-06]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.0010154011041079998], ["'alubox production - APOS' (kilogram, GLO, None)", 0.00012087002202593586], ["'market for polysulfone' (kilogram, GLO, None)", 3.084994121856062e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.013001819892197055], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 1.1087998519062382e-05], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.00011918523184616125], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0009646310489025998], ["'plastic incineration - APOS' (kilogram, CH, None)", 1.9985102989065883e-07], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.00015137192783822912], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -9.096344076142203e-05], ["'market for corrugated board box' (kilogram, RER, None)", 6.419026509461157e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.54124104635806e-06], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.00011335676606923576], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00021682501563951944], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 6.791453675795855e-06], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 4.196312874609168e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.942586541245365e-08], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 2.1365172293593314e-08], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 4.025177202411406e-09], ["'market for corrugated board box' (kilogram, RER, None)", 2.5011791136710915e-09], ["'autoclave - APOS' (unit, GLO, None)", 4.6873260419332326e-07], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 6.943037542027535e-11], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -1.048996732272497e-08], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -9.599595730614724e-10], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 6.08381577473906e-09], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 7.378602237886549e-10], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -6.348190414613136e-09], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -3.856382607831381e-08], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.6158711102267305e-09]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.942586541245365e-08], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 2.1365172293593314e-08], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 4.025177202411406e-09], ["'market for corrugated board box' (kilogram, RER, None)", 2.5011791136710915e-09], ["'autoclave - APOS' (unit, GLO, None)", 4.6873260419332326e-07], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 6.943037542027535e-11], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.3225686466824044e-08], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.6040439647579454e-09], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.3800414005324228e-08], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -8.383440451515602e-08], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.6158711102267305e-09]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 5.5267955117121646e-08], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 6.078541976487112e-08], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.2139423062947743e-08], ["'market for corrugated board box' (kilogram, RER, None)", 7.543238595425746e-09], ["'autoclave - APOS' (unit, GLO, None)", 6.249768055910977e-07], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 2.0939319576485633e-10], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -2.984469576324569e-08], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -2.8951161140778123e-09], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.7308884316863242e-08], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 2.225292693331786e-09], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.806104889865371e-08], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -1.0971680093724575e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 4.597267102709941e-09]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 5.5267955117121646e-08], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 6.078541976487112e-08], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.2139423062947743e-08], ["'market for corrugated board box' (kilogram, RER, None)", 7.543238595425746e-09], ["'autoclave - APOS' (unit, GLO, None)", 6.249768055910977e-07], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 2.0939319576485633e-10], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 3.7628009384485305e-08], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 4.837592811590839e-09], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -3.9263149723491276e-08], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -2.385147846636913e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 4.597267102709941e-09]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 2.2538925097084422e-08], ["'alubox production - APOS' (kilogram, GLO, None)", 9.066373066979957e-09], ["'market for polysulfone' (kilogram, GLO, None)", 7.169071248888733e-10], ["'autoclave - APOS' (unit, GLO, None)", 9.374652083866465e-07], ["'cabinet washer - APOS' (unit, GLO, None)", 1.517304219876885e-07], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 7.563958925857879e-10], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -1.881641801436443e-09], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 2.1411978842230197e-08], ["'plastic incineration - APOS' (kilogram, CH, None)", 3.2123499214498354e-10], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -3.5480446670652224e-10], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -4.3107143222807705e-10], ["'market for corrugated board box' (kilogram, RER, None)", 8.827378095268184e-10], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 5.060295195971182e-10]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 2.2538925097084422e-08], ["'alubox production - APOS' (kilogram, GLO, None)", 9.066373066979957e-09], ["'market for polysulfone' (kilogram, GLO, None)", 7.169071248888733e-10], ["'autoclave - APOS' (unit, GLO, None)", 9.374652083866465e-07], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 7.563958925857879e-10], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -1.881641801436443e-09], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 2.1411978842230197e-08], ["'plastic incineration - APOS' (kilogram, CH, None)", 3.2123499214498354e-10], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.2137144373134713e-08], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -1.486656360506353e-08], ["'market for corrugated board box' (kilogram, RER, None)", 8.827378095268184e-10], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 5.060295195971182e-10], ["'production of wet wipe - APOS' (unit, GLO, None)", 1.3763590934157995e-07], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.011074232692752e-09], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 2.3954292841782104e-09], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 2.334751771912932e-08]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 1.3467638905055853e-08], ["'alubox production - APOS' (kilogram, GLO, None)", 5.417411793981457e-09], ["'market for polysulfone' (kilogram, GLO, None)", 3.5845356244443666e-10], ["'autoclave - APOS' (unit, GLO, None)", 6.249768055910977e-07], ["'cabinet washer - APOS' (unit, GLO, None)", 7.586521099384425e-08], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 4.519677272422607e-10], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -1.1243336681429808e-09], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 1.279425695980306e-08], ["'plastic incineration - APOS' (kilogram, CH, None)", 1.6061749607249177e-10], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.7740223335326112e-10], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -2.1553571611403853e-10], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 3.023668086711309e-10], ["'market for corrugated board box' (kilogram, RER, None)", 5.274605611397395e-10]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 1.3467638905055853e-08], ["'alubox production - APOS' (kilogram, GLO, None)", 5.417411793981457e-09], ["'market for polysulfone' (kilogram, GLO, None)", 3.5845356244443666e-10], ["'autoclave - APOS' (unit, GLO, None)", 6.249768055910977e-07], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 4.519677272422607e-10], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -1.1243336681429808e-09], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 1.279425695980306e-08], ["'plastic incineration - APOS' (kilogram, CH, None)", 1.6061749607249177e-10], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.2137144373134713e-08], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -1.486656360506353e-08], ["'market for corrugated board box' (kilogram, RER, None)", 5.274605611397395e-10], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 3.023668086711309e-10], ["'production of wet wipe - APOS' (unit, GLO, None)", 1.3763590934157995e-07], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.011074232692752e-09], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 2.3954292841782104e-09], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 2.334751771912932e-08]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.00016998806206562595], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.000110838933467122], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 2.563845938850817e-05], ["'market for corrugated board box' (kilogram, RER, None)", 3.2210710524177033e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.0006560896967725333], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 4.449414831409708e-07], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -9.179355351543801e-05], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -2.7731595025459803e-06], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.8140406646135314e-06], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 2.132991509327611e-07], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -8.612086268481757e-06], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -5.5954923554735624e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 3.187934530495913e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.00016998806206562595], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.000110838933467122], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 2.563845938850817e-05], ["'market for corrugated board box' (kilogram, RER, None)", 3.2210710524177033e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.0006560896967725333], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 4.449414831409708e-07], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 3.94356666220333e-06], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 4.6369380637556756e-07], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.872192675270579e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.00012164113815823557], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 3.187934530495913e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0004836280075669921], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.0003153445712726569], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 7.732233627201546e-05], ["'market for corrugated board box' (kilogram, RER, None)", 9.714341267444702e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.0008747862623633778], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 1.3418870129864744e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.00026115912408617575], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -8.363496743018314e-06], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 5.161073440168076e-06], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 6.43283140575554e-07], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -2.450199207264203e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.00015919569797474215], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 9.06989824243191e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0004836280075669921], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.0003153445712726569], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 7.732233627201546e-05], ["'market for corrugated board box' (kilogram, RER, None)", 9.714341267444702e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.0008747862623633778], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 1.3418870129864744e-06], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.1219724869930598e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.3984416099468563e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -5.3265200081687986e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0003460776043183169], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 9.06989824243191e-06]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.00021599600147081347], ["'alubox production - APOS' (kilogram, GLO, None)", 2.597174833237654e-05], ["'market for polysulfone' (kilogram, GLO, None)", 3.868790417823136e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.0013121793935450667], ["'cabinet washer - APOS' (unit, GLO, None)", 0.00022338461312882037], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 1.3138137780382486e-06], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -1.7084091274759938e-05], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0002051962013972728], ["'plastic incineration - APOS' (kilogram, CH, None)", 2.8984146201064396e-08], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -4.81335069705127e-07], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -6.254713675963946e-07], ["'market for corrugated board box' (kilogram, RER, None)", 1.1368083115679469e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 9.983401329253032e-07]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.00021599600147081347], ["'alubox production - APOS' (kilogram, GLO, None)", 2.597174833237654e-05], ["'market for polysulfone' (kilogram, GLO, None)", 3.868790417823136e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.0013121793935450667], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 1.3138137780382486e-06], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -1.7084091274759938e-05], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0002051962013972728], ["'plastic incineration - APOS' (kilogram, CH, None)", 2.8984146201064396e-08], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.6465500806945155e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -2.1570925777790906e-05], ["'market for corrugated board box' (kilogram, RER, None)", 1.1368083115679469e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 9.983401329253032e-07], ["'production of wet wipe - APOS' (unit, GLO, None)", 3.66743140902013e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 3.8287676503750914e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 6.924658844071709e-07], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 8.776607994799e-07]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.00012906365943427905], ["'alubox production - APOS' (kilogram, GLO, None)", 1.551884691780089e-05], ["'market for polysulfone' (kilogram, GLO, None)", 1.934395208911568e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.0008747862623633778], ["'cabinet washer - APOS' (unit, GLO, None)", 0.00011169230656441018], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 7.850405232233174e-07], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -1.0208222944014532e-05], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0001226104764625651], ["'plastic incineration - APOS' (kilogram, CH, None)", 1.4492073100532198e-08], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -2.406675348525635e-07], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -3.127356837981973e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 5.965361866660864e-07], ["'market for corrugated board box' (kilogram, RER, None)", 6.792748010299562e-07]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.00012906365943427905], ["'alubox production - APOS' (kilogram, GLO, None)", 1.551884691780089e-05], ["'market for polysulfone' (kilogram, GLO, None)", 1.934395208911568e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.0008747862623633778], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 7.850405232233174e-07], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -1.0208222944014532e-05], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0001226104764625651], ["'plastic incineration - APOS' (kilogram, CH, None)", 1.4492073100532198e-08], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.6465500806945155e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -2.1570925777790906e-05], ["'market for corrugated board box' (kilogram, RER, None)", 6.792748010299562e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 5.965361866660864e-07], ["'production of wet wipe - APOS' (unit, GLO, None)", 3.66743140902013e-05], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 3.8287676503750914e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 6.924658844071709e-07], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 8.776607994799e-07]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0003504637141768082], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.00017202377786909893], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 5.042776174752089e-05], ["'market for corrugated board box' (kilogram, RER, None)", 8.205839676126542e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.001173434895622745], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 2.3446821182988132e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.00018925040565547643], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -4.6240275497054505e-06], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.286386276443755e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.5549615719126231e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.9310921884561185e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.00014686255948619177], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 3.6356299116105775e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0003504637141768082], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.00017202377786909893], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 5.042776174752089e-05], ["'market for corrugated board box' (kilogram, RER, None)", 8.205839676126542e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.001173434895622745], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 2.3446821182988132e-06], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 2.796491905312511e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 3.380351243288311e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -4.198026515051549e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0003192664336545236], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 3.6356299116105775e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.000997093947376271], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.0004894197623881406], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00015208372282441468], ["'market for corrugated board box' (kilogram, RER, None)", 2.4747770447348056e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.0015645798608303267], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 7.07126353316432e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0005384307315831864], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -1.394547962931219e-05], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 3.6598595470653314e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 4.689566550452766e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -5.494093303066056e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.00041783432410359684], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.0343623129650697e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.000997093947376271], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.0004894197623881406], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.00015208372282441468], ["'market for corrugated board box' (kilogram, RER, None)", 2.4747770447348056e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.0015645798608303267], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 7.07126353316432e-06], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 7.956216406663763e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.0194709892288622e-05], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.00011943681076528892], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0009083354872483962], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.0343623129650697e-05]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.00028581829031370945], ["'alubox production - APOS' (kilogram, GLO, None)", 3.66508666591304e-05], ["'market for polysulfone' (kilogram, GLO, None)", 5.830554314203478e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.00234686979124549], ["'cabinet washer - APOS' (unit, GLO, None)", 0.00037993232930458136], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 3.0530269051826787e-06], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -1.2499992244360293e-05], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.00027152737579802397], ["'plastic incineration - APOS' (kilogram, CH, None)", 1.9033009747171134e-07], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.079299909638987e-06], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -1.641648671732677e-06], ["'market for corrugated board box' (kilogram, RER, None)", 2.8960760552651672e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.138541339071946e-06]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.00028581829031370945], ["'alubox production - APOS' (kilogram, GLO, None)", 3.66508666591304e-05], ["'market for polysulfone' (kilogram, GLO, None)", 5.830554314203478e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.00234686979124549], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 3.0530269051826787e-06], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -1.2499992244360293e-05], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.00027152737579802397], ["'plastic incineration - APOS' (kilogram, CH, None)", 1.9033009747171134e-07], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -3.69206705507319e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -5.661631129053577e-05], ["'market for corrugated board box' (kilogram, RER, None)", 2.8960760552651672e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.138541339071946e-06], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.0007658611910073358], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 7.530724835450617e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 5.048111234409315e-06], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 6.316669418757423e-06]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.0001707844322577476], ["'alubox production - APOS' (kilogram, GLO, None)", 2.1899919166347908e-05], ["'market for polysulfone' (kilogram, GLO, None)", 2.915277157101739e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.0015645798608303267], ["'cabinet washer - APOS' (unit, GLO, None)", 0.00018996616465229068], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 1.8242690700338352e-06], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -7.4690954044130455e-06], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0001622452106448602], ["'plastic incineration - APOS' (kilogram, CH, None)", 9.516504873585567e-08], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -5.396499548194935e-07], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -8.208243358663385e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 6.803103334948225e-07], ["'market for corrugated board box' (kilogram, RER, None)", 1.7304865439403376e-06]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.0001707844322577476], ["'alubox production - APOS' (kilogram, GLO, None)", 2.1899919166347908e-05], ["'market for polysulfone' (kilogram, GLO, None)", 2.915277157101739e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.0015645798608303267], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 1.8242690700338352e-06], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -7.4690954044130455e-06], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0001622452106448602], ["'plastic incineration - APOS' (kilogram, CH, None)", 9.516504873585567e-08], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -3.69206705507319e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -5.661631129053577e-05], ["'market for corrugated board box' (kilogram, RER, None)", 1.7304865439403376e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 6.803103334948225e-07], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.0007658611910073358], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 7.530724835450617e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 5.048111234409315e-06], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 6.316669418757423e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0003752848134254249], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.00017648306688504862], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 5.542429940590573e-05], ["'market for corrugated board box' (kilogram, RER, None)", 8.53350850804001e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.0012279241797793225], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 2.395849469652867e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.00020265379924972948], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -4.820451221870887e-06], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.2937392412833076e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.5632753833092448e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.985032419720325e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.00015214914656646293], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 3.7489374398610376e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0003752848134254249], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.00017648306688504862], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 5.542429940590573e-05], ["'market for corrugated board box' (kilogram, RER, None)", 8.53350850804001e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.0012279241797793225], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 2.395849469652867e-06], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 2.8124766114854516e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 3.3984247463244455e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -4.315287887879218e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.00033075901426340884], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 3.7489374398610376e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0010677117227033215], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.0005021067536729552], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.000167152645615875], ["'market for corrugated board box' (kilogram, RER, None)", 2.5735978035480335e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.0016372322397057632], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 7.2255777674457005e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0005765643302597937], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -1.4537868469874413e-05], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 3.680779249848284e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 4.714639949394975e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -5.647557060584252e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0004328750366393715], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.066599102695293e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0010677117227033215], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.0005021067536729552], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.000167152645615875], ["'market for corrugated board box' (kilogram, RER, None)", 2.5735978035480335e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.0016372322397057632], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 7.2255777674457005e-06], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 8.001694021409312e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.0249217281293424e-05], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.00012277297940221433], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0009410326884155234], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.066599102695293e-05]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.0002902557988383286], ["'alubox production - APOS' (kilogram, GLO, None)", 3.860467294312466e-05], ["'market for polysulfone' (kilogram, GLO, None)", 6.29803767904099e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.002455848359558645], ["'cabinet washer - APOS' (unit, GLO, None)", 0.0003999088094947557], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 3.3998082355773054e-06], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -1.3025156638695387e-05], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.00027574300889641215], ["'plastic incineration - APOS' (kilogram, CH, None)", 1.91629166926558e-07], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.1094474536440758e-06], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -1.7007428254004966e-06], ["'market for corrugated board box' (kilogram, RER, None)", 3.0117197792002222e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.1740249576133233e-06]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.0002902557988383286], ["'alubox production - APOS' (kilogram, GLO, None)", 3.860467294312466e-05], ["'market for polysulfone' (kilogram, GLO, None)", 6.29803767904099e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.002455848359558645], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 3.3998082355773054e-06], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -1.3025156638695387e-05], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.00027574300889641215], ["'plastic incineration - APOS' (kilogram, CH, None)", 1.91629166926558e-07], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -3.795195715622962e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -5.8654319213373987e-05], ["'market for corrugated board box' (kilogram, RER, None)", 3.0117197792002222e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.1740249576133233e-06], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.0012091062151199882], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 8.276892203014035e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 5.075101640776993e-06], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 6.338024624840571e-06]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.00017343596786515813], ["'alubox production - APOS' (kilogram, GLO, None)", 2.3067373133647682e-05], ["'market for polysulfone' (kilogram, GLO, None)", 3.149018839520495e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.0016372322397057632], ["'cabinet washer - APOS' (unit, GLO, None)", 0.00019995440474737786], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 2.0314806258934286e-06], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -7.782895836254061e-06], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.00016476416947190021], ["'plastic incineration - APOS' (kilogram, CH, None)", 9.5814583463279e-08], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -5.547237268220379e-07], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -8.503714127002483e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 7.015127892468152e-07], ["'market for corrugated board box' (kilogram, RER, None)", 1.7995869074466548e-06]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.00017343596786515813], ["'alubox production - APOS' (kilogram, GLO, None)", 2.3067373133647682e-05], ["'market for polysulfone' (kilogram, GLO, None)", 3.149018839520495e-06], ["'autoclave - APOS' (unit, GLO, None)", 0.0016372322397057632], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 2.0314806258934286e-06], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -7.782895836254061e-06], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.00016476416947190021], ["'plastic incineration - APOS' (kilogram, CH, None)", 9.5814583463279e-08], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -3.795195715622962e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -5.8654319213373987e-05], ["'market for corrugated board box' (kilogram, RER, None)", 1.7995869074466548e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 7.015127892468152e-07], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.0012091062151199882], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 8.276892203014035e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 5.075101640776993e-06], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 6.338024624840571e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0012426762753245935], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.00036398055433329543], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0003511865862773925], ["'market for corrugated board box' (kilogram, RER, None)", 4.2225104178167744e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.010704359580710858], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 4.711286406182188e-07], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0006710451886752805], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -1.9004050940381406e-05], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 4.73351468627404e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 5.111994846159728e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -7.640119589227457e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.00027095474400126615], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.183085572672973e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0012426762753245935], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.00036398055433329543], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0003511865862773925], ["'market for corrugated board box' (kilogram, RER, None)", 4.2225104178167744e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.010704359580710858], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 4.711286406182188e-07], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.00010290249317987043], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.1113032274260279e-05], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.00016608955701583503], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0005890320521561669], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.183085572672973e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0035355015157122237], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.0010355503095116293], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0010591341276353407], ["'market for corrugated board box' (kilogram, RER, None)", 0.00012734555226040197], ["'autoclave - APOS' (unit, GLO, None)", 0.01427247944094781], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 1.420864154604482e-06], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.0019091708184846008], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -5.731380326234904e-05], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.00013467182628554313], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.5417127001505536e-05], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.00021736678404440758], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0007708853278774344], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 3.3659617704143766e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.0035355015157122237], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.0010355503095116293], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0010591341276353407], ["'market for corrugated board box' (kilogram, RER, None)", 0.00012734555226040197], ["'autoclave - APOS' (unit, GLO, None)", 0.01427247944094781], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 1.420864154604482e-06], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.0002927648397511807], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 3.3515493481533774e-05], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0004725364863767985], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0016758376694217625], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 3.3659617704143766e-05]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.0006367618977553125], ["'alubox production - APOS' (kilogram, GLO, None)", 0.0006762028182161041], ["'market for polysulfone' (kilogram, GLO, None)", 4.240918684364896e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.021408719161421716], ["'cabinet washer - APOS' (unit, GLO, None)", 0.004039357611284405], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 2.6740040886812073e-06], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -3.511925773874729e-05], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0006049238028675468], ["'plastic incineration - APOS' (kilogram, CH, None)", 1.175813793438848e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -4.270112235748204e-06], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -3.028767148996665e-06], ["'market for corrugated board box' (kilogram, RER, None)", 1.4902449714834396e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 3.704975107191457e-06]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.0006367618977553125], ["'alubox production - APOS' (kilogram, GLO, None)", 0.0006762028182161041], ["'market for polysulfone' (kilogram, GLO, None)", 4.240918684364896e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.021408719161421716], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 2.6740040886812073e-06], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -3.511925773874729e-05], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.0006049238028675468], ["'plastic incineration - APOS' (kilogram, CH, None)", 1.175813793438848e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.00014607191723331337], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.00010445451982923834], ["'market for corrugated board box' (kilogram, RER, None)", 1.4902449714834396e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 3.704975107191457e-06], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.009010382556659601], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0005244511069909417], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.659585618016259e-05], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 4.24396011408411e-06]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.0003804830652095282], ["'alubox production - APOS' (kilogram, GLO, None)", 0.0004040501196524964], ["'market for polysulfone' (kilogram, GLO, None)", 2.120459342182448e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.01427247944094781], ["'cabinet washer - APOS' (unit, GLO, None)", 0.0020196788056422027], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 1.5977923233641655e-06], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -2.098473994663656e-05], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.00036145891194905175], ["'plastic incineration - APOS' (kilogram, CH, None)", 5.87906896719424e-07], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -2.135056117874102e-06], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -1.5143835744983325e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.213826379653449e-06], ["'market for corrugated board box' (kilogram, RER, None)", 8.904631028727327e-06]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.0003804830652095282], ["'alubox production - APOS' (kilogram, GLO, None)", 0.0004040501196524964], ["'market for polysulfone' (kilogram, GLO, None)", 2.120459342182448e-05], ["'autoclave - APOS' (unit, GLO, None)", 0.01427247944094781], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 1.5977923233641655e-06], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -2.098473994663656e-05], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.00036145891194905175], ["'plastic incineration - APOS' (kilogram, CH, None)", 5.87906896719424e-07], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.00014607191723331337], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.00010445451982923834], ["'market for corrugated board box' (kilogram, RER, None)", 8.904631028727327e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.213826379653449e-06], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.009010382556659601], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.0005244511069909417], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.659585618016259e-05], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 4.24396011408411e-06]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 6.594758818767752e-10], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 2.513503048988018e-10], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 9.314310917586194e-11], ["'market for corrugated board box' (kilogram, RER, None)", 2.6107095004555252e-11], ["'autoclave - APOS' (unit, GLO, None)", 4.897503985765704e-09], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 1.2814611037247904e-12], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -3.561169762134587e-10], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -1.2252929497775287e-11], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 2.4275037332741033e-10], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 2.944618815966076e-11], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -5.4167145333541937e-11], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -7.045313455879403e-10], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.348792747494446e-11]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 6.594758818767752e-10], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 2.513503048988018e-10], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 9.314310917586194e-11], ["'market for corrugated board box' (kilogram, RER, None)", 2.6107095004555252e-11], ["'autoclave - APOS' (unit, GLO, None)", 4.897503985765704e-09], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 1.2814611037247904e-12], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 5.277182028856747e-10], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 6.401345252100166e-11], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.1775466428490867e-10], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -1.5315898816596134e-09], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.348792747494446e-11]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.876255325902938e-09], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 7.151093181627883e-10], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 2.8090778388756033e-10], ["'market for corrugated board box' (kilogram, RER, None)", 7.873568333287495e-11], ["'autoclave - APOS' (unit, GLO, None)", 6.530005314354272e-09], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 3.864723964591084e-12], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -1.0131778759875866e-09], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -3.695327868916099e-11], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 6.906419072131957e-10], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 8.880596249207051e-11], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.5410934402937285e-10], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -2.004441292753123e-09], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 3.83741035233925e-11]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 1.876255325902938e-09], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 7.151093181627883e-10], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 2.8090778388756033e-10], ["'market for corrugated board box' (kilogram, RER, None)", 7.873568333287495e-11], ["'autoclave - APOS' (unit, GLO, None)", 6.530005314354272e-09], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 3.864723964591084e-12], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.5013954504634687e-09], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.9305644020015327e-10], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -3.350203126278744e-10], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -4.357481071522242e-09], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 3.83741035233925e-11]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 4.868087151423871e-10], ["'alubox production - APOS' (kilogram, GLO, None)", 1.018901480440111e-10], ["'market for polysulfone' (kilogram, GLO, None)", 1.0875171631154611e-11], ["'autoclave - APOS' (unit, GLO, None)", 9.795007971531408e-09], ["'cabinet washer - APOS' (unit, GLO, None)", 1.75224406374857e-09], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 6.707778065272973e-12], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -3.7222590595168694e-11], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 4.624682793852677e-10], ["'plastic incineration - APOS' (kilogram, CH, None)", 2.1807394992709287e-12], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -3.0274367745557354e-12], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -7.87534244074796e-12], ["'market for corrugated board box' (kilogram, RER, None)", 9.213942228873176e-12], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 4.223907103301839e-12]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 4.868087151423871e-10], ["'alubox production - APOS' (kilogram, GLO, None)", 1.018901480440111e-10], ["'market for polysulfone' (kilogram, GLO, None)", 1.0875171631154611e-11], ["'autoclave - APOS' (unit, GLO, None)", 9.795007971531408e-09], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 6.707778065272973e-12], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -3.7222590595168694e-11], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 4.624682793852677e-10], ["'plastic incineration - APOS' (kilogram, CH, None)", 2.1807394992709287e-12], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.0356249895724549e-10], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -2.716006456328795e-10], ["'market for corrugated board box' (kilogram, RER, None)", 9.213942228873176e-12], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 4.223907103301839e-12], ["'production of wet wipe - APOS' (unit, GLO, None)", 4.392788796950162e-10], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.3909701743925513e-10], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 9.559569570357645e-11], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 1.0792811361554383e-11]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 2.9088183944583734e-10], ["'alubox production - APOS' (kilogram, GLO, None)", 6.088221669528204e-11], ["'market for polysulfone' (kilogram, GLO, None)", 5.4375858155773054e-12], ["'autoclave - APOS' (unit, GLO, None)", 6.530005314354272e-09], ["'cabinet washer - APOS' (unit, GLO, None)", 8.76122031874285e-10], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 4.008085232513434e-12], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -2.224154022816762e-11], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 2.7633774747354547e-10], ["'plastic incineration - APOS' (kilogram, CH, None)", 1.0903697496354644e-12], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.5137183872778677e-12], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -3.93767122037398e-12], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.5239027793586677e-12], ["'market for corrugated board box' (kilogram, RER, None)", 5.505588506462332e-12]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 2.9088183944583734e-10], ["'alubox production - APOS' (kilogram, GLO, None)", 6.088221669528204e-11], ["'market for polysulfone' (kilogram, GLO, None)", 5.4375858155773054e-12], ["'autoclave - APOS' (unit, GLO, None)", 6.530005314354272e-09], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 4.008085232513434e-12], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -2.224154022816762e-11], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 2.7633774747354547e-10], ["'plastic incineration - APOS' (kilogram, CH, None)", 1.0903697496354644e-12], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.0356249895724549e-10], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -2.716006456328795e-10], ["'market for corrugated board box' (kilogram, RER, None)", 5.505588506462332e-12], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.5239027793586677e-12], ["'production of wet wipe - APOS' (unit, GLO, None)", 4.392788796950162e-10], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.3909701743925513e-10], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 9.559569570357645e-11], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 1.0792811361554383e-11]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 3.076268826759314e-07], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 1.4437574095097888e-07], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 4.3960972279403205e-08], ["'market for corrugated board box' (kilogram, RER, None)", 7.325167901430008e-09], ["'autoclave - APOS' (unit, GLO, None)", 2.7845578783600164e-06], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 6.002837272676786e-10], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -1.66118516645003e-07], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -5.961856734412428e-09], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 9.15874890852756e-08], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.1101302285616891e-08], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -2.4561663639056362e-08], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -1.9064393577245598e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 6.54901193661524e-09]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 3.076268826759314e-07], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 1.4437574095097888e-07], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 4.3960972279403205e-08], ["'market for corrugated board box' (kilogram, RER, None)", 7.325167901430008e-09], ["'autoclave - APOS' (unit, GLO, None)", 2.7845578783600164e-06], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 6.002837272676786e-10], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.9910323714190347e-07], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 2.413326583829759e-08], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -5.3394921188600304e-08], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -4.14443338621351e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 6.54901193661524e-09]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 8.75220145078002e-07], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 4.107591503112357e-07], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.3258070736326534e-07], ["'market for corrugated board box' (kilogram, RER, None)", 2.2091776206678668e-08], ["'autoclave - APOS' (unit, GLO, None)", 3.712743837813355e-06], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 1.8103794953917617e-09], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -4.726188783421211e-07], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -1.798020248558473e-08], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 2.605728562707841e-07], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 3.348011732602431e-08], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -6.987966318655482e-08], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -5.423954228131452e-07], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.8632400159212842e-08]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 8.75220145078002e-07], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 4.107591503112357e-07], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 1.3258070736326534e-07], ["'market for corrugated board box' (kilogram, RER, None)", 2.2091776206678668e-08], ["'autoclave - APOS' (unit, GLO, None)", 3.712743837813355e-06], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 1.8103794953917617e-09], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 5.664627310234437e-07], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 7.278286375222676e-08], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.519123110577128e-07], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -1.1791204844629398e-06], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.8632400159212842e-08]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 3.331508929349619e-07], ["'alubox production - APOS' (kilogram, GLO, None)", 5.130891409080537e-08], ["'market for polysulfone' (kilogram, GLO, None)", 5.915531344963806e-09], ["'autoclave - APOS' (unit, GLO, None)", 5.569115756720033e-06], ["'cabinet washer - APOS' (unit, GLO, None)", 1.0348270460808225e-06], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 2.9610874763512365e-09], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -2.9578093637089378e-08], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 3.164933482882138e-07], ["'plastic incineration - APOS' (kilogram, CH, None)", 9.112894422399398e-10], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.372767261174135e-09], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -2.1310425545468453e-09], ["'market for corrugated board box' (kilogram, RER, None)", 2.585261740105352e-09], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.050902044814825e-09]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 3.331508929349619e-07], ["'alubox production - APOS' (kilogram, GLO, None)", 5.130891409080537e-08], ["'market for polysulfone' (kilogram, GLO, None)", 5.915531344963806e-09], ["'autoclave - APOS' (unit, GLO, None)", 5.569115756720033e-06], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 2.9610874763512365e-09], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -2.9578093637089378e-08], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 3.164933482882138e-07], ["'plastic incineration - APOS' (kilogram, CH, None)", 9.112894422399398e-10], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -4.695959606778231e-08], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -7.349426873062975e-08], ["'market for corrugated board box' (kilogram, RER, None)", 2.585261740105352e-09], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.050902044814825e-09], ["'production of wet wipe - APOS' (unit, GLO, None)", 7.092161060082882e-08], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.564994643081361e-08], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 3.603986734904693e-08], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 3.911140445855908e-09]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 1.9906698778307688e-07], ["'alubox production - APOS' (kilogram, GLO, None)", 3.06585129773951e-08], ["'market for polysulfone' (kilogram, GLO, None)", 2.957765672481903e-09], ["'autoclave - APOS' (unit, GLO, None)", 3.712743837813355e-06], ["'cabinet washer - APOS' (unit, GLO, None)", 5.174135230404112e-07], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 1.7693326867189491e-09], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -1.767373922617894e-08], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 1.8911363839392304e-07], ["'plastic incineration - APOS' (kilogram, CH, None)", 4.556447211199699e-10], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -6.863836305870675e-10], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -1.0655212772734226e-09], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.2254714046751174e-09], ["'market for corrugated board box' (kilogram, RER, None)", 1.5447662866735288e-09]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 1.9906698778307688e-07], ["'alubox production - APOS' (kilogram, GLO, None)", 3.06585129773951e-08], ["'market for polysulfone' (kilogram, GLO, None)", 2.957765672481903e-09], ["'autoclave - APOS' (unit, GLO, None)", 3.712743837813355e-06], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 1.7693326867189491e-09], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -1.767373922617894e-08], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 1.8911363839392304e-07], ["'plastic incineration - APOS' (kilogram, CH, None)", 4.556447211199699e-10], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -4.695959606778231e-08], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -7.349426873062975e-08], ["'market for corrugated board box' (kilogram, RER, None)", 1.5447662866735288e-09], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.2254714046751174e-09], ["'production of wet wipe - APOS' (unit, GLO, None)", 7.092161060082882e-08], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 6.564994643081361e-08], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 3.603986734904693e-08], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 3.911140445855908e-09]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.04813660124284061], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.003585106468493621], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.005074179597921867], ["'market for corrugated board box' (kilogram, RER, None)", 0.00024889132757794676], ["'autoclave - APOS' (unit, GLO, None)", 0.05087673060843365], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 2.5740261101999055e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.02599376467113393], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.00015679095243401186], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 5.226880221697493e-05], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 6.146015557016038e-06], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0006061891267982785], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.003509209681066763], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 7.894024659335565e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.04813660124284061], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.003585106468493621], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.005074179597921867], ["'market for corrugated board box' (kilogram, RER, None)", 0.00024889132757794676], ["'autoclave - APOS' (unit, GLO, None)", 0.05087673060843365], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 2.5740261101999055e-05], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.00011362783090646725], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.3360903384817474e-05], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0013178024553398714], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.00762871669770574], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 7.894024659335565e-05]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.1369520204373775], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.010199880375150865], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.015303081017066697], ["'market for corrugated board box' (kilogram, RER, None)", 0.0007506246385917995], ["'autoclave - APOS' (unit, GLO, None)", 0.06783564081124487], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 7.762935889866213e-05], ["'market for polypropylene, granulate' (kilogram, GLO, None)", -0.07395409103618385], ["'polyethylene, high density, granulate, recycled to generic market for high density PE granulate' (kilogram, Europe without Switzerland, None)", -0.00047286159299986225], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.00014870842320885828], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.8535602098059e-05], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0017246507659463624], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.009983948668443234], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.00022459056074869915]]</t>
+  </si>
+  <si>
+    <t>[["'market for polypropylene, granulate' (kilogram, GLO, None)", 0.1369520204373775], ["'sheet manufacturing - APOS' (kilogram, GLO, None)", 0.010199880375150865], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.015303081017066697], ["'market for corrugated board box' (kilogram, RER, None)", 0.0007506246385917995], ["'autoclave - APOS' (unit, GLO, None)", 0.06783564081124487], ["'transport Plastic - APOS' (ton kilometer, GLO, None)", 7.762935889866213e-05], ["'PP incineration no Energy Recovery - APOS' (kilogram, CH, None)", 0.0003232791808888223], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 4.029478716969348e-05], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0037492407901699165], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.021704236237339063], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 0.00022459056074869915]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.0045326307586048215], ["'alubox production - APOS' (kilogram, GLO, None)", 0.0012805993133763874], ["'market for polysulfone' (kilogram, GLO, None)", 0.0004548315760085618], ["'autoclave - APOS' (unit, GLO, None)", 0.1017534612168673], ["'cabinet washer - APOS' (unit, GLO, None)", 0.018091794245463536], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 0.00022504716122111656], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.00035513013294828546], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.004305999220674581], ["'plastic incineration - APOS' (kilogram, CH, None)", 9.422288368560032e-07], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -3.3880302229412986e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -3.9226399375780656e-05], ["'market for corrugated board box' (kilogram, RER, None)", 8.784088437149415e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.4721089948138736e-05]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.0045326307586048215], ["'alubox production - APOS' (kilogram, GLO, None)", 0.0012805993133763874], ["'market for polysulfone' (kilogram, GLO, None)", 0.0004548315760085618], ["'autoclave - APOS' (unit, GLO, None)", 0.1017534612168673], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 0.00022504716122111656], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.00035513013294828546], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.004305999220674581], ["'plastic incineration - APOS' (kilogram, CH, None)", 9.422288368560032e-07], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0011589767270431721], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0013528193188388333], ["'market for corrugated board box' (kilogram, RER, None)", 8.784088437149415e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 2.4721089948138736e-05], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.0009750444546189048], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.007577621729262176], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.995275686592369e-05], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 1.93932876931901e-05]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.0027083738059334337], ["'alubox production - APOS' (kilogram, GLO, None)", 0.0007651939504802129], ["'market for polysulfone' (kilogram, GLO, None)", 0.0002274157880042809], ["'autoclave - APOS' (unit, GLO, None)", 0.06783564081124487], ["'cabinet washer - APOS' (unit, GLO, None)", 0.009045897122731768], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 0.00013447198084552608], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.00021220019917767387], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.002572955115636762], ["'plastic incineration - APOS' (kilogram, CH, None)", 4.711144184280016e-07], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -1.6940151114706493e-05], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -1.9613199687890328e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.4771543526634314e-05], ["'market for corrugated board box' (kilogram, RER, None)", 5.2487388283997186e-05]]</t>
+  </si>
+  <si>
+    <t>[["'alubox raw materials - APOS' (kilogram, GLO, None)", 0.0027083738059334337], ["'alubox production - APOS' (kilogram, GLO, None)", 0.0007651939504802129], ["'market for polysulfone' (kilogram, GLO, None)", 0.0002274157880042809], ["'autoclave - APOS' (unit, GLO, None)", 0.06783564081124487], ["'transport Alu - APOS' (ton kilometer, GLO, None)", 0.00013447198084552608], ["'alubox EoL melting - APOS' (kilogram, GLO, None)", -0.00021220019917767387], ["'avoided alubox raw materials - APOS' (kilogram, GLO, None)", 0.002572955115636762], ["'plastic incineration - APOS' (kilogram, CH, None)", 4.711144184280016e-07], ["'mixed electricity mix - APOS' (kilowatt hour, GLO, None)", -0.0011589767270431721], ["'mixed heating grid DK 23 - APOS' (megajoule, GLO, None)", -0.0013528193188388333], ["'market for corrugated board box' (kilogram, RER, None)", 5.2487388283997186e-05], ["'treatment of waste paper to pulp, wet lap, totally chlorine free bleached' (kilogram, RoW, None)", 1.4771543526634314e-05], ["'production of wet wipe - APOS' (unit, GLO, None)", 0.0009750444546189048], ["'packaging film production, low density polyethylene' (kilogram, RER, None)", 0.007577621729262176], ["'PE incineration no Energy Recovery - APOS' (kilogram, CH, None)", 1.995275686592369e-05], ["'incineration of wet wipe - APOS' (kilogram, CH, None)", 1.93932876931901e-05]]</t>
   </si>
 </sst>
 </file>

</xml_diff>